<commit_message>
Updated quantity conversions to support SI-compatible mL unit
</commit_message>
<xml_diff>
--- a/src/carpy/utility/data/quantities.xlsx
+++ b/src/carpy/utility/data/quantities.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://sotonac-my.sharepoint.com/personal/yr3g17_soton_ac_uk/Documents/Documents/Python/ADRpy_restructure1/src/ADRpy/utility/data/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://sotonac-my.sharepoint.com/personal/yr3g17_soton_ac_uk/Documents/Documents/Python/carpy/src/carpy/utility/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="915" documentId="13_ncr:1_{848856CE-4ADE-4AE2-9F79-561287E38E1C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{05883607-9836-49A9-8DB3-4F1301FD1C81}"/>
+  <xr:revisionPtr revIDLastSave="934" documentId="13_ncr:1_{848856CE-4ADE-4AE2-9F79-561287E38E1C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{6DD52F89-8BDB-4BCF-9746-9DC57D68CA16}"/>
   <bookViews>
-    <workbookView xWindow="2977" yWindow="2977" windowWidth="15474" windowHeight="7952" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-107" yWindow="-107" windowWidth="20847" windowHeight="11208" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="dimensions" sheetId="1" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="633" uniqueCount="432">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="637" uniqueCount="435">
   <si>
     <t>Symbol</t>
   </si>
@@ -781,9 +781,6 @@
     <t>Exact definition, joules to the ISO thermochemical small calorie</t>
   </si>
   <si>
-    <t>USCS</t>
-  </si>
-  <si>
     <t>Exact definition, metres cubed to an imperial gallon</t>
   </si>
   <si>
@@ -1331,6 +1328,18 @@
   </si>
   <si>
     <t>dB shift of 1 watt to 1 watt</t>
+  </si>
+  <si>
+    <t>ml,mL</t>
+  </si>
+  <si>
+    <t>millilitre</t>
+  </si>
+  <si>
+    <t>metres cubed to a millilitre</t>
+  </si>
+  <si>
+    <t>USC</t>
   </si>
 </sst>
 </file>
@@ -1650,11 +1659,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:N155"/>
+  <dimension ref="A1:N156"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A25" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="N150" sqref="N150"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A101" sqref="A101"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14" x14ac:dyDescent="0.3"/>
@@ -1677,7 +1686,7 @@
         <v>76</v>
       </c>
       <c r="B1" t="s">
-        <v>349</v>
+        <v>348</v>
       </c>
       <c r="C1" t="s">
         <v>1</v>
@@ -1710,7 +1719,7 @@
         <v>18</v>
       </c>
       <c r="M1" t="s">
-        <v>421</v>
+        <v>420</v>
       </c>
       <c r="N1" t="s">
         <v>130</v>
@@ -3179,7 +3188,7 @@
         <v>243</v>
       </c>
       <c r="C35" t="s">
-        <v>291</v>
+        <v>290</v>
       </c>
       <c r="D35">
         <v>0</v>
@@ -3213,7 +3222,7 @@
         <v>9460750000000000</v>
       </c>
       <c r="N35" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
     </row>
     <row r="36" spans="1:14" x14ac:dyDescent="0.3">
@@ -3311,7 +3320,7 @@
         <v>219</v>
       </c>
       <c r="B38" s="1" t="s">
-        <v>341</v>
+        <v>340</v>
       </c>
       <c r="C38" t="s">
         <v>107</v>
@@ -3356,7 +3365,7 @@
         <v>219</v>
       </c>
       <c r="B39" t="s">
-        <v>342</v>
+        <v>341</v>
       </c>
       <c r="C39" t="s">
         <v>108</v>
@@ -3490,19 +3499,19 @@
         <v>219</v>
       </c>
       <c r="B42" t="s">
-        <v>125</v>
+        <v>431</v>
       </c>
       <c r="C42" t="s">
-        <v>111</v>
+        <v>432</v>
       </c>
       <c r="D42">
         <v>0</v>
       </c>
       <c r="E42">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="F42">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G42">
         <v>0</v>
@@ -3523,10 +3532,11 @@
         <v>0</v>
       </c>
       <c r="M42">
-        <v>1000</v>
+        <f>M41/1000</f>
+        <v>9.9999999999999995E-7</v>
       </c>
       <c r="N42" t="s">
-        <v>170</v>
+        <v>433</v>
       </c>
     </row>
     <row r="43" spans="1:14" x14ac:dyDescent="0.3">
@@ -3534,10 +3544,10 @@
         <v>219</v>
       </c>
       <c r="B43" t="s">
-        <v>100</v>
+        <v>125</v>
       </c>
       <c r="C43" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="D43">
         <v>0</v>
@@ -3567,11 +3577,10 @@
         <v>0</v>
       </c>
       <c r="M43">
-        <f>1.6605390666*10^-27</f>
-        <v>1.6605390666E-27</v>
+        <v>1000</v>
       </c>
       <c r="N43" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
     </row>
     <row r="44" spans="1:14" x14ac:dyDescent="0.3">
@@ -3579,16 +3588,16 @@
         <v>219</v>
       </c>
       <c r="B44" t="s">
-        <v>363</v>
+        <v>100</v>
       </c>
       <c r="C44" t="s">
-        <v>364</v>
+        <v>112</v>
       </c>
       <c r="D44">
-        <v>-2</v>
+        <v>0</v>
       </c>
       <c r="E44">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F44">
         <v>1</v>
@@ -3611,11 +3620,12 @@
       <c r="L44">
         <v>0</v>
       </c>
-      <c r="M44" s="2">
-        <v>1.0000000000000001E-5</v>
+      <c r="M44">
+        <f>1.6605390666*10^-27</f>
+        <v>1.6605390666E-27</v>
       </c>
       <c r="N44" t="s">
-        <v>365</v>
+        <v>171</v>
       </c>
     </row>
     <row r="45" spans="1:14" x14ac:dyDescent="0.3">
@@ -3623,10 +3633,10 @@
         <v>219</v>
       </c>
       <c r="B45" t="s">
-        <v>293</v>
+        <v>362</v>
       </c>
       <c r="C45" t="s">
-        <v>294</v>
+        <v>363</v>
       </c>
       <c r="D45">
         <v>-2</v>
@@ -3655,12 +3665,11 @@
       <c r="L45">
         <v>0</v>
       </c>
-      <c r="M45">
-        <f>9.80665</f>
-        <v>9.8066499999999994</v>
+      <c r="M45" s="2">
+        <v>1.0000000000000001E-5</v>
       </c>
       <c r="N45" t="s">
-        <v>172</v>
+        <v>364</v>
       </c>
     </row>
     <row r="46" spans="1:14" x14ac:dyDescent="0.3">
@@ -3668,16 +3677,16 @@
         <v>219</v>
       </c>
       <c r="B46" t="s">
-        <v>221</v>
+        <v>292</v>
       </c>
       <c r="C46" t="s">
-        <v>223</v>
+        <v>293</v>
       </c>
       <c r="D46">
         <v>-2</v>
       </c>
       <c r="E46">
-        <v>-1</v>
+        <v>1</v>
       </c>
       <c r="F46">
         <v>1</v>
@@ -3701,11 +3710,11 @@
         <v>0</v>
       </c>
       <c r="M46">
-        <f>M47 / 1000</f>
-        <v>100</v>
+        <f>9.80665</f>
+        <v>9.8066499999999994</v>
       </c>
       <c r="N46" t="s">
-        <v>227</v>
+        <v>172</v>
       </c>
     </row>
     <row r="47" spans="1:14" x14ac:dyDescent="0.3">
@@ -3713,10 +3722,10 @@
         <v>219</v>
       </c>
       <c r="B47" t="s">
-        <v>220</v>
+        <v>221</v>
       </c>
       <c r="C47" t="s">
-        <v>220</v>
+        <v>223</v>
       </c>
       <c r="D47">
         <v>-2</v>
@@ -3746,11 +3755,11 @@
         <v>0</v>
       </c>
       <c r="M47">
-        <f>POWER(10, 5)</f>
-        <v>100000</v>
+        <f>M48 / 1000</f>
+        <v>100</v>
       </c>
       <c r="N47" t="s">
-        <v>225</v>
+        <v>227</v>
       </c>
     </row>
     <row r="48" spans="1:14" x14ac:dyDescent="0.3">
@@ -3758,10 +3767,10 @@
         <v>219</v>
       </c>
       <c r="B48" t="s">
-        <v>222</v>
+        <v>220</v>
       </c>
       <c r="C48" t="s">
-        <v>224</v>
+        <v>220</v>
       </c>
       <c r="D48">
         <v>-2</v>
@@ -3791,11 +3800,11 @@
         <v>0</v>
       </c>
       <c r="M48">
-        <f>M47*10</f>
-        <v>1000000</v>
+        <f>POWER(10, 5)</f>
+        <v>100000</v>
       </c>
       <c r="N48" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
     </row>
     <row r="49" spans="1:14" x14ac:dyDescent="0.3">
@@ -3803,88 +3812,89 @@
         <v>219</v>
       </c>
       <c r="B49" t="s">
-        <v>101</v>
+        <v>222</v>
       </c>
       <c r="C49" t="s">
-        <v>113</v>
+        <v>224</v>
       </c>
       <c r="D49">
         <v>-2</v>
       </c>
       <c r="E49">
+        <v>-1</v>
+      </c>
+      <c r="F49">
+        <v>1</v>
+      </c>
+      <c r="G49">
+        <v>0</v>
+      </c>
+      <c r="H49">
+        <v>0</v>
+      </c>
+      <c r="I49">
+        <v>0</v>
+      </c>
+      <c r="J49">
+        <v>0</v>
+      </c>
+      <c r="K49">
+        <v>0</v>
+      </c>
+      <c r="L49">
+        <v>0</v>
+      </c>
+      <c r="M49">
+        <f>M48*10</f>
+        <v>1000000</v>
+      </c>
+      <c r="N49" t="s">
+        <v>226</v>
+      </c>
+    </row>
+    <row r="50" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A50" t="s">
+        <v>219</v>
+      </c>
+      <c r="B50" t="s">
+        <v>101</v>
+      </c>
+      <c r="C50" t="s">
+        <v>113</v>
+      </c>
+      <c r="D50">
+        <v>-2</v>
+      </c>
+      <c r="E50">
         <v>2</v>
       </c>
-      <c r="F49">
-        <v>1</v>
-      </c>
-      <c r="G49">
-        <v>0</v>
-      </c>
-      <c r="H49">
-        <v>0</v>
-      </c>
-      <c r="I49">
-        <v>0</v>
-      </c>
-      <c r="J49">
-        <v>0</v>
-      </c>
-      <c r="K49">
-        <v>0</v>
-      </c>
-      <c r="L49">
-        <v>0</v>
-      </c>
-      <c r="M49">
+      <c r="F50">
+        <v>1</v>
+      </c>
+      <c r="G50">
+        <v>0</v>
+      </c>
+      <c r="H50">
+        <v>0</v>
+      </c>
+      <c r="I50">
+        <v>0</v>
+      </c>
+      <c r="J50">
+        <v>0</v>
+      </c>
+      <c r="K50">
+        <v>0</v>
+      </c>
+      <c r="L50">
+        <v>0</v>
+      </c>
+      <c r="M50">
         <f>1.602176634 * 10^-19</f>
         <v>1.6021766340000001E-19</v>
       </c>
-      <c r="N49" t="s">
+      <c r="N50" t="s">
         <v>234</v>
-      </c>
-    </row>
-    <row r="50" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A50" t="s">
-        <v>228</v>
-      </c>
-      <c r="B50" t="s">
-        <v>229</v>
-      </c>
-      <c r="C50" t="s">
-        <v>230</v>
-      </c>
-      <c r="D50">
-        <v>-2</v>
-      </c>
-      <c r="E50">
-        <v>-1</v>
-      </c>
-      <c r="F50">
-        <v>1</v>
-      </c>
-      <c r="G50">
-        <v>0</v>
-      </c>
-      <c r="H50">
-        <v>0</v>
-      </c>
-      <c r="I50">
-        <v>0</v>
-      </c>
-      <c r="J50">
-        <v>0</v>
-      </c>
-      <c r="K50">
-        <v>0</v>
-      </c>
-      <c r="L50">
-        <v>0</v>
-      </c>
-      <c r="M50">
-        <v>101325</v>
-      </c>
-      <c r="N50" t="s">
-        <v>233</v>
       </c>
     </row>
     <row r="51" spans="1:14" x14ac:dyDescent="0.3">
@@ -3892,10 +3902,10 @@
         <v>228</v>
       </c>
       <c r="B51" t="s">
-        <v>231</v>
+        <v>229</v>
       </c>
       <c r="C51" t="s">
-        <v>232</v>
+        <v>230</v>
       </c>
       <c r="D51">
         <v>-2</v>
@@ -3925,7 +3935,7 @@
         <v>0</v>
       </c>
       <c r="M51">
-        <v>133.32238741500001</v>
+        <v>101325</v>
       </c>
       <c r="N51" t="s">
         <v>233</v>
@@ -3936,10 +3946,10 @@
         <v>228</v>
       </c>
       <c r="B52" t="s">
-        <v>240</v>
+        <v>231</v>
       </c>
       <c r="C52" t="s">
-        <v>241</v>
+        <v>232</v>
       </c>
       <c r="D52">
         <v>-2</v>
@@ -3969,11 +3979,10 @@
         <v>0</v>
       </c>
       <c r="M52">
-        <f>M51*M57*POWER(1000,2)</f>
-        <v>3386.3886403410002</v>
+        <v>133.32238741500001</v>
       </c>
       <c r="N52" t="s">
-        <v>242</v>
+        <v>233</v>
       </c>
     </row>
     <row r="53" spans="1:14" x14ac:dyDescent="0.3">
@@ -3981,10 +3990,10 @@
         <v>228</v>
       </c>
       <c r="B53" t="s">
-        <v>237</v>
+        <v>240</v>
       </c>
       <c r="C53" t="s">
-        <v>238</v>
+        <v>241</v>
       </c>
       <c r="D53">
         <v>-2</v>
@@ -4014,11 +4023,11 @@
         <v>0</v>
       </c>
       <c r="M53">
-        <f>M54/1000</f>
-        <v>0.13332236842105263</v>
+        <f>M52*M58*POWER(1000,2)</f>
+        <v>3386.3886403410002</v>
       </c>
       <c r="N53" t="s">
-        <v>239</v>
+        <v>242</v>
       </c>
     </row>
     <row r="54" spans="1:14" x14ac:dyDescent="0.3">
@@ -4026,10 +4035,10 @@
         <v>228</v>
       </c>
       <c r="B54" t="s">
-        <v>236</v>
+        <v>237</v>
       </c>
       <c r="C54" t="s">
-        <v>235</v>
+        <v>238</v>
       </c>
       <c r="D54">
         <v>-2</v>
@@ -4059,11 +4068,11 @@
         <v>0</v>
       </c>
       <c r="M54">
-        <f>M50/760</f>
-        <v>133.32236842105263</v>
+        <f>M55/1000</f>
+        <v>0.13332236842105263</v>
       </c>
       <c r="N54" t="s">
-        <v>233</v>
+        <v>239</v>
       </c>
     </row>
     <row r="55" spans="1:14" x14ac:dyDescent="0.3">
@@ -4071,19 +4080,19 @@
         <v>228</v>
       </c>
       <c r="B55" t="s">
-        <v>369</v>
+        <v>236</v>
       </c>
       <c r="C55" t="s">
-        <v>372</v>
+        <v>235</v>
       </c>
       <c r="D55">
+        <v>-2</v>
+      </c>
+      <c r="E55">
         <v>-1</v>
       </c>
-      <c r="E55">
-        <v>0</v>
-      </c>
       <c r="F55">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G55">
         <v>0</v>
@@ -4098,17 +4107,17 @@
         <v>0</v>
       </c>
       <c r="K55">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="L55">
         <v>0</v>
       </c>
       <c r="M55">
-        <f>M56*60</f>
-        <v>6.2831853071795862</v>
+        <f>M51/760</f>
+        <v>133.32236842105263</v>
       </c>
       <c r="N55" t="s">
-        <v>373</v>
+        <v>233</v>
       </c>
     </row>
     <row r="56" spans="1:14" x14ac:dyDescent="0.3">
@@ -4116,7 +4125,7 @@
         <v>228</v>
       </c>
       <c r="B56" t="s">
-        <v>370</v>
+        <v>368</v>
       </c>
       <c r="C56" t="s">
         <v>371</v>
@@ -4149,56 +4158,56 @@
         <v>0</v>
       </c>
       <c r="M56">
+        <f>M57*60</f>
+        <v>6.2831853071795862</v>
+      </c>
+      <c r="N56" t="s">
+        <v>372</v>
+      </c>
+    </row>
+    <row r="57" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A57" t="s">
+        <v>228</v>
+      </c>
+      <c r="B57" t="s">
+        <v>369</v>
+      </c>
+      <c r="C57" t="s">
+        <v>370</v>
+      </c>
+      <c r="D57">
+        <v>-1</v>
+      </c>
+      <c r="E57">
+        <v>0</v>
+      </c>
+      <c r="F57">
+        <v>0</v>
+      </c>
+      <c r="G57">
+        <v>0</v>
+      </c>
+      <c r="H57">
+        <v>0</v>
+      </c>
+      <c r="I57">
+        <v>0</v>
+      </c>
+      <c r="J57">
+        <v>0</v>
+      </c>
+      <c r="K57">
+        <v>1</v>
+      </c>
+      <c r="L57">
+        <v>0</v>
+      </c>
+      <c r="M57">
         <f>2*PI()/60</f>
         <v>0.10471975511965977</v>
       </c>
-      <c r="N56" t="s">
-        <v>374</v>
-      </c>
-    </row>
-    <row r="57" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A57" t="s">
-        <v>77</v>
-      </c>
-      <c r="B57" t="s">
-        <v>64</v>
-      </c>
-      <c r="C57" t="s">
-        <v>62</v>
-      </c>
-      <c r="D57">
-        <v>0</v>
-      </c>
-      <c r="E57">
-        <v>1</v>
-      </c>
-      <c r="F57">
-        <v>0</v>
-      </c>
-      <c r="G57">
-        <v>0</v>
-      </c>
-      <c r="H57">
-        <v>0</v>
-      </c>
-      <c r="I57">
-        <v>0</v>
-      </c>
-      <c r="J57">
-        <v>0</v>
-      </c>
-      <c r="K57">
-        <v>0</v>
-      </c>
-      <c r="L57">
-        <v>0</v>
-      </c>
-      <c r="M57">
-        <f>M60/12000</f>
-        <v>2.5399999999999997E-5</v>
-      </c>
       <c r="N57" t="s">
-        <v>176</v>
+        <v>373</v>
       </c>
     </row>
     <row r="58" spans="1:14" x14ac:dyDescent="0.3">
@@ -4206,10 +4215,10 @@
         <v>77</v>
       </c>
       <c r="B58" t="s">
-        <v>343</v>
+        <v>64</v>
       </c>
       <c r="C58" t="s">
-        <v>58</v>
+        <v>62</v>
       </c>
       <c r="D58">
         <v>0</v>
@@ -4239,11 +4248,11 @@
         <v>0</v>
       </c>
       <c r="M58">
-        <f>0.0254</f>
-        <v>2.5399999999999999E-2</v>
+        <f>M61/12000</f>
+        <v>2.5399999999999997E-5</v>
       </c>
       <c r="N58" t="s">
-        <v>132</v>
+        <v>176</v>
       </c>
     </row>
     <row r="59" spans="1:14" x14ac:dyDescent="0.3">
@@ -4251,10 +4260,10 @@
         <v>77</v>
       </c>
       <c r="B59" t="s">
-        <v>350</v>
+        <v>342</v>
       </c>
       <c r="C59" t="s">
-        <v>63</v>
+        <v>58</v>
       </c>
       <c r="D59">
         <v>0</v>
@@ -4284,11 +4293,11 @@
         <v>0</v>
       </c>
       <c r="M59">
-        <f>M60/3</f>
-        <v>0.10159999999999998</v>
+        <f>0.0254</f>
+        <v>2.5399999999999999E-2</v>
       </c>
       <c r="N59" t="s">
-        <v>177</v>
+        <v>132</v>
       </c>
     </row>
     <row r="60" spans="1:14" x14ac:dyDescent="0.3">
@@ -4296,10 +4305,10 @@
         <v>77</v>
       </c>
       <c r="B60" t="s">
-        <v>344</v>
+        <v>349</v>
       </c>
       <c r="C60" t="s">
-        <v>59</v>
+        <v>63</v>
       </c>
       <c r="D60">
         <v>0</v>
@@ -4329,11 +4338,11 @@
         <v>0</v>
       </c>
       <c r="M60">
-        <f>M58*12</f>
-        <v>0.30479999999999996</v>
+        <f>M61/3</f>
+        <v>0.10159999999999998</v>
       </c>
       <c r="N60" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
     </row>
     <row r="61" spans="1:14" x14ac:dyDescent="0.3">
@@ -4341,10 +4350,10 @@
         <v>77</v>
       </c>
       <c r="B61" t="s">
-        <v>61</v>
+        <v>343</v>
       </c>
       <c r="C61" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="D61">
         <v>0</v>
@@ -4374,11 +4383,11 @@
         <v>0</v>
       </c>
       <c r="M61">
-        <f>M60*3</f>
-        <v>0.91439999999999988</v>
+        <f>M59*12</f>
+        <v>0.30479999999999996</v>
       </c>
       <c r="N61" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
     </row>
     <row r="62" spans="1:14" x14ac:dyDescent="0.3">
@@ -4386,10 +4395,10 @@
         <v>77</v>
       </c>
       <c r="B62" t="s">
-        <v>66</v>
+        <v>61</v>
       </c>
       <c r="C62" t="s">
-        <v>67</v>
+        <v>60</v>
       </c>
       <c r="D62">
         <v>0</v>
@@ -4419,11 +4428,11 @@
         <v>0</v>
       </c>
       <c r="M62">
-        <f>M60*66</f>
-        <v>20.116799999999998</v>
+        <f>M61*3</f>
+        <v>0.91439999999999988</v>
       </c>
       <c r="N62" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
     </row>
     <row r="63" spans="1:14" x14ac:dyDescent="0.3">
@@ -4431,10 +4440,10 @@
         <v>77</v>
       </c>
       <c r="B63" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="C63" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="D63">
         <v>0</v>
@@ -4464,11 +4473,11 @@
         <v>0</v>
       </c>
       <c r="M63">
-        <f>M60*660</f>
-        <v>201.16799999999998</v>
+        <f>M61*66</f>
+        <v>20.116799999999998</v>
       </c>
       <c r="N63" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
     </row>
     <row r="64" spans="1:14" x14ac:dyDescent="0.3">
@@ -4476,10 +4485,10 @@
         <v>77</v>
       </c>
       <c r="B64" t="s">
-        <v>118</v>
+        <v>68</v>
       </c>
       <c r="C64" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="D64">
         <v>0</v>
@@ -4509,11 +4518,11 @@
         <v>0</v>
       </c>
       <c r="M64">
-        <f>M60*5280</f>
-        <v>1609.3439999999998</v>
+        <f>M61*660</f>
+        <v>201.16799999999998</v>
       </c>
       <c r="N64" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
     </row>
     <row r="65" spans="1:14" x14ac:dyDescent="0.3">
@@ -4521,10 +4530,10 @@
         <v>77</v>
       </c>
       <c r="B65" t="s">
-        <v>71</v>
+        <v>118</v>
       </c>
       <c r="C65" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="D65">
         <v>0</v>
@@ -4554,11 +4563,11 @@
         <v>0</v>
       </c>
       <c r="M65">
-        <f>M60*15840</f>
-        <v>4828.0319999999992</v>
+        <f>M61*5280</f>
+        <v>1609.3439999999998</v>
       </c>
       <c r="N65" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
     </row>
     <row r="66" spans="1:14" x14ac:dyDescent="0.3">
@@ -4566,10 +4575,10 @@
         <v>77</v>
       </c>
       <c r="B66" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="C66" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="D66">
         <v>0</v>
@@ -4599,11 +4608,11 @@
         <v>0</v>
       </c>
       <c r="M66">
-        <f>M67/1000</f>
-        <v>1.8520000000000001</v>
+        <f>M61*15840</f>
+        <v>4828.0319999999992</v>
       </c>
       <c r="N66" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
     </row>
     <row r="67" spans="1:14" x14ac:dyDescent="0.3">
@@ -4611,10 +4620,10 @@
         <v>77</v>
       </c>
       <c r="B67" t="s">
-        <v>362</v>
+        <v>73</v>
       </c>
       <c r="C67" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="D67">
         <v>0</v>
@@ -4644,11 +4653,11 @@
         <v>0</v>
       </c>
       <c r="M67">
-        <f>1852</f>
-        <v>1852</v>
+        <f>M68/1000</f>
+        <v>1.8520000000000001</v>
       </c>
       <c r="N67" t="s">
-        <v>132</v>
+        <v>184</v>
       </c>
     </row>
     <row r="68" spans="1:14" x14ac:dyDescent="0.3">
@@ -4656,13 +4665,13 @@
         <v>77</v>
       </c>
       <c r="B68" t="s">
-        <v>128</v>
+        <v>361</v>
       </c>
       <c r="C68" t="s">
-        <v>129</v>
+        <v>75</v>
       </c>
       <c r="D68">
-        <v>-1</v>
+        <v>0</v>
       </c>
       <c r="E68">
         <v>1</v>
@@ -4689,11 +4698,11 @@
         <v>0</v>
       </c>
       <c r="M68">
-        <f>M67/M32</f>
-        <v>0.51444444444444448</v>
+        <f>1852</f>
+        <v>1852</v>
       </c>
       <c r="N68" t="s">
-        <v>185</v>
+        <v>132</v>
       </c>
     </row>
     <row r="69" spans="1:14" x14ac:dyDescent="0.3">
@@ -4701,16 +4710,16 @@
         <v>77</v>
       </c>
       <c r="B69" t="s">
-        <v>78</v>
+        <v>128</v>
       </c>
       <c r="C69" t="s">
-        <v>79</v>
+        <v>129</v>
       </c>
       <c r="D69">
-        <v>0</v>
+        <v>-1</v>
       </c>
       <c r="E69">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="F69">
         <v>0</v>
@@ -4734,11 +4743,11 @@
         <v>0</v>
       </c>
       <c r="M69">
-        <f>M74/160</f>
-        <v>2.8413062500000005E-5</v>
+        <f>M68/M32</f>
+        <v>0.51444444444444448</v>
       </c>
       <c r="N69" t="s">
-        <v>189</v>
+        <v>185</v>
       </c>
     </row>
     <row r="70" spans="1:14" x14ac:dyDescent="0.3">
@@ -4746,10 +4755,10 @@
         <v>77</v>
       </c>
       <c r="B70" t="s">
-        <v>333</v>
+        <v>78</v>
       </c>
       <c r="C70" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="D70">
         <v>0</v>
@@ -4779,11 +4788,11 @@
         <v>0</v>
       </c>
       <c r="M70">
-        <f>M69*5</f>
-        <v>1.4206531250000003E-4</v>
+        <f>M75/160</f>
+        <v>2.8413062500000005E-5</v>
       </c>
       <c r="N70" t="s">
-        <v>188</v>
+        <v>189</v>
       </c>
     </row>
     <row r="71" spans="1:14" x14ac:dyDescent="0.3">
@@ -4791,10 +4800,10 @@
         <v>77</v>
       </c>
       <c r="B71" t="s">
-        <v>316</v>
+        <v>332</v>
       </c>
       <c r="C71" t="s">
-        <v>276</v>
+        <v>80</v>
       </c>
       <c r="D71">
         <v>0</v>
@@ -4824,11 +4833,11 @@
         <v>0</v>
       </c>
       <c r="M71">
-        <f>M69*10</f>
-        <v>2.8413062500000006E-4</v>
+        <f>M70*5</f>
+        <v>1.4206531250000003E-4</v>
       </c>
       <c r="N71" t="s">
-        <v>277</v>
+        <v>188</v>
       </c>
     </row>
     <row r="72" spans="1:14" x14ac:dyDescent="0.3">
@@ -4836,10 +4845,10 @@
         <v>77</v>
       </c>
       <c r="B72" t="s">
-        <v>334</v>
+        <v>315</v>
       </c>
       <c r="C72" t="s">
-        <v>81</v>
+        <v>275</v>
       </c>
       <c r="D72">
         <v>0</v>
@@ -4869,11 +4878,11 @@
         <v>0</v>
       </c>
       <c r="M72">
-        <f>M69*20</f>
-        <v>5.6826125000000011E-4</v>
+        <f>M70*10</f>
+        <v>2.8413062500000006E-4</v>
       </c>
       <c r="N72" t="s">
-        <v>186</v>
+        <v>276</v>
       </c>
     </row>
     <row r="73" spans="1:14" x14ac:dyDescent="0.3">
@@ -4881,10 +4890,10 @@
         <v>77</v>
       </c>
       <c r="B73" t="s">
-        <v>335</v>
+        <v>333</v>
       </c>
       <c r="C73" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="D73">
         <v>0</v>
@@ -4914,11 +4923,11 @@
         <v>0</v>
       </c>
       <c r="M73">
-        <f>M69*40</f>
-        <v>1.1365225000000002E-3</v>
+        <f>M70*20</f>
+        <v>5.6826125000000011E-4</v>
       </c>
       <c r="N73" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
     </row>
     <row r="74" spans="1:14" x14ac:dyDescent="0.3">
@@ -4926,10 +4935,10 @@
         <v>77</v>
       </c>
       <c r="B74" t="s">
-        <v>336</v>
+        <v>334</v>
       </c>
       <c r="C74" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="D74">
         <v>0</v>
@@ -4959,11 +4968,11 @@
         <v>0</v>
       </c>
       <c r="M74">
-        <f>M41*4.54609</f>
-        <v>4.5460900000000009E-3</v>
+        <f>M70*40</f>
+        <v>1.1365225000000002E-3</v>
       </c>
       <c r="N74" t="s">
-        <v>249</v>
+        <v>187</v>
       </c>
     </row>
     <row r="75" spans="1:14" x14ac:dyDescent="0.3">
@@ -4971,10 +4980,10 @@
         <v>77</v>
       </c>
       <c r="B75" t="s">
-        <v>280</v>
+        <v>335</v>
       </c>
       <c r="C75" t="s">
-        <v>284</v>
+        <v>83</v>
       </c>
       <c r="D75">
         <v>0</v>
@@ -5004,11 +5013,11 @@
         <v>0</v>
       </c>
       <c r="M75">
-        <f>2*M74</f>
-        <v>9.0921800000000018E-3</v>
+        <f>M41*4.54609</f>
+        <v>4.5460900000000009E-3</v>
       </c>
       <c r="N75" t="s">
-        <v>360</v>
+        <v>248</v>
       </c>
     </row>
     <row r="76" spans="1:14" x14ac:dyDescent="0.3">
@@ -5016,10 +5025,10 @@
         <v>77</v>
       </c>
       <c r="B76" t="s">
-        <v>359</v>
+        <v>279</v>
       </c>
       <c r="C76" t="s">
-        <v>285</v>
+        <v>283</v>
       </c>
       <c r="D76">
         <v>0</v>
@@ -5049,22 +5058,22 @@
         <v>0</v>
       </c>
       <c r="M76">
-        <f>M75*4</f>
-        <v>3.6368720000000007E-2</v>
+        <f>2*M75</f>
+        <v>9.0921800000000018E-3</v>
       </c>
       <c r="N76" t="s">
-        <v>361</v>
+        <v>359</v>
       </c>
     </row>
     <row r="77" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A77" t="s">
-        <v>248</v>
+        <v>77</v>
       </c>
       <c r="B77" t="s">
-        <v>273</v>
+        <v>358</v>
       </c>
       <c r="C77" t="s">
-        <v>274</v>
+        <v>284</v>
       </c>
       <c r="D77">
         <v>0</v>
@@ -5094,22 +5103,22 @@
         <v>0</v>
       </c>
       <c r="M77">
-        <f>M78/3</f>
-        <v>4.9289215937500005E-6</v>
+        <f>M76*4</f>
+        <v>3.6368720000000007E-2</v>
       </c>
       <c r="N77" t="s">
-        <v>278</v>
+        <v>360</v>
       </c>
     </row>
     <row r="78" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A78" t="s">
-        <v>248</v>
+        <v>434</v>
       </c>
       <c r="B78" t="s">
         <v>272</v>
       </c>
       <c r="C78" t="s">
-        <v>275</v>
+        <v>273</v>
       </c>
       <c r="D78">
         <v>0</v>
@@ -5139,22 +5148,22 @@
         <v>0</v>
       </c>
       <c r="M78">
-        <f>M80/2</f>
-        <v>1.4786764781250001E-5</v>
+        <f>M79/3</f>
+        <v>4.9289215937500005E-6</v>
       </c>
       <c r="N78" t="s">
-        <v>279</v>
+        <v>277</v>
       </c>
     </row>
     <row r="79" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A79" t="s">
-        <v>248</v>
+        <v>434</v>
       </c>
       <c r="B79" t="s">
-        <v>356</v>
+        <v>271</v>
       </c>
       <c r="C79" t="s">
-        <v>357</v>
+        <v>274</v>
       </c>
       <c r="D79">
         <v>0</v>
@@ -5184,22 +5193,22 @@
         <v>0</v>
       </c>
       <c r="M79">
-        <f>M80/8</f>
-        <v>3.6966911953125001E-6</v>
+        <f>M81/2</f>
+        <v>1.4786764781250001E-5</v>
       </c>
       <c r="N79" t="s">
-        <v>358</v>
+        <v>278</v>
       </c>
     </row>
     <row r="80" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A80" t="s">
-        <v>248</v>
+        <v>434</v>
       </c>
       <c r="B80" t="s">
-        <v>78</v>
+        <v>355</v>
       </c>
       <c r="C80" t="s">
-        <v>264</v>
+        <v>356</v>
       </c>
       <c r="D80">
         <v>0</v>
@@ -5229,22 +5238,22 @@
         <v>0</v>
       </c>
       <c r="M80">
-        <f>M85/128</f>
-        <v>2.9573529562500001E-5</v>
+        <f>M81/8</f>
+        <v>3.6966911953125001E-6</v>
       </c>
       <c r="N80" t="s">
-        <v>268</v>
+        <v>357</v>
       </c>
     </row>
     <row r="81" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A81" t="s">
-        <v>248</v>
+        <v>434</v>
       </c>
       <c r="B81" t="s">
-        <v>333</v>
+        <v>78</v>
       </c>
       <c r="C81" t="s">
-        <v>265</v>
+        <v>263</v>
       </c>
       <c r="D81">
         <v>0</v>
@@ -5274,22 +5283,22 @@
         <v>0</v>
       </c>
       <c r="M81">
-        <f>M80*32</f>
-        <v>9.4635294600000004E-4</v>
+        <f>M86/128</f>
+        <v>2.9573529562500001E-5</v>
       </c>
       <c r="N81" t="s">
-        <v>269</v>
+        <v>267</v>
       </c>
     </row>
     <row r="82" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A82" t="s">
-        <v>248</v>
+        <v>434</v>
       </c>
       <c r="B82" t="s">
-        <v>334</v>
+        <v>332</v>
       </c>
       <c r="C82" t="s">
-        <v>266</v>
+        <v>264</v>
       </c>
       <c r="D82">
         <v>0</v>
@@ -5319,22 +5328,22 @@
         <v>0</v>
       </c>
       <c r="M82">
-        <f>M80*16</f>
-        <v>4.7317647300000002E-4</v>
+        <f>M81*32</f>
+        <v>9.4635294600000004E-4</v>
       </c>
       <c r="N82" t="s">
-        <v>270</v>
+        <v>268</v>
       </c>
     </row>
     <row r="83" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A83" t="s">
-        <v>248</v>
+        <v>434</v>
       </c>
       <c r="B83" t="s">
-        <v>335</v>
+        <v>333</v>
       </c>
       <c r="C83" t="s">
-        <v>263</v>
+        <v>265</v>
       </c>
       <c r="D83">
         <v>0</v>
@@ -5364,19 +5373,19 @@
         <v>0</v>
       </c>
       <c r="M83">
-        <f>M80*32</f>
-        <v>9.4635294600000004E-4</v>
+        <f>M81*16</f>
+        <v>4.7317647300000002E-4</v>
       </c>
       <c r="N83" t="s">
-        <v>271</v>
+        <v>269</v>
       </c>
     </row>
     <row r="84" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A84" t="s">
-        <v>248</v>
+        <v>434</v>
       </c>
       <c r="B84" t="s">
-        <v>337</v>
+        <v>334</v>
       </c>
       <c r="C84" t="s">
         <v>262</v>
@@ -5409,16 +5418,16 @@
         <v>0</v>
       </c>
       <c r="M84">
-        <f>M80*64</f>
-        <v>1.8927058920000001E-3</v>
+        <f>M81*32</f>
+        <v>9.4635294600000004E-4</v>
       </c>
       <c r="N84" t="s">
-        <v>267</v>
+        <v>270</v>
       </c>
     </row>
     <row r="85" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A85" t="s">
-        <v>248</v>
+        <v>434</v>
       </c>
       <c r="B85" t="s">
         <v>336</v>
@@ -5454,67 +5463,67 @@
         <v>0</v>
       </c>
       <c r="M85">
+        <f>M81*64</f>
+        <v>1.8927058920000001E-3</v>
+      </c>
+      <c r="N85" t="s">
+        <v>266</v>
+      </c>
+    </row>
+    <row r="86" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A86" t="s">
+        <v>434</v>
+      </c>
+      <c r="B86" t="s">
+        <v>335</v>
+      </c>
+      <c r="C86" t="s">
+        <v>260</v>
+      </c>
+      <c r="D86">
+        <v>0</v>
+      </c>
+      <c r="E86">
+        <v>3</v>
+      </c>
+      <c r="F86">
+        <v>0</v>
+      </c>
+      <c r="G86">
+        <v>0</v>
+      </c>
+      <c r="H86">
+        <v>0</v>
+      </c>
+      <c r="I86">
+        <v>0</v>
+      </c>
+      <c r="J86">
+        <v>0</v>
+      </c>
+      <c r="K86">
+        <v>0</v>
+      </c>
+      <c r="L86">
+        <v>0</v>
+      </c>
+      <c r="M86">
         <f>M41*3.785411784</f>
         <v>3.7854117840000001E-3</v>
       </c>
-      <c r="N85" t="s">
-        <v>250</v>
-      </c>
-    </row>
-    <row r="86" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A86" t="s">
-        <v>248</v>
-      </c>
-      <c r="B86" t="s">
-        <v>351</v>
-      </c>
-      <c r="C86" t="s">
-        <v>281</v>
-      </c>
-      <c r="D86">
-        <v>0</v>
-      </c>
-      <c r="E86">
-        <v>3</v>
-      </c>
-      <c r="F86">
-        <v>0</v>
-      </c>
-      <c r="G86">
-        <v>0</v>
-      </c>
-      <c r="H86">
-        <v>0</v>
-      </c>
-      <c r="I86">
-        <v>0</v>
-      </c>
-      <c r="J86">
-        <v>0</v>
-      </c>
-      <c r="K86">
-        <v>0</v>
-      </c>
-      <c r="L86">
-        <v>0</v>
-      </c>
-      <c r="M86">
-        <f>POWER(M58,3)*33.6003125</f>
-        <v>5.506104713575E-4</v>
-      </c>
       <c r="N86" t="s">
-        <v>287</v>
+        <v>249</v>
       </c>
     </row>
     <row r="87" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A87" t="s">
-        <v>248</v>
+        <v>434</v>
       </c>
       <c r="B87" t="s">
-        <v>352</v>
+        <v>350</v>
       </c>
       <c r="C87" t="s">
-        <v>282</v>
+        <v>280</v>
       </c>
       <c r="D87">
         <v>0</v>
@@ -5544,8 +5553,8 @@
         <v>0</v>
       </c>
       <c r="M87">
-        <f>M86*2</f>
-        <v>1.101220942715E-3</v>
+        <f>POWER(M59,3)*33.6003125</f>
+        <v>5.506104713575E-4</v>
       </c>
       <c r="N87" t="s">
         <v>286</v>
@@ -5553,13 +5562,13 @@
     </row>
     <row r="88" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A88" t="s">
-        <v>248</v>
+        <v>434</v>
       </c>
       <c r="B88" t="s">
-        <v>353</v>
+        <v>351</v>
       </c>
       <c r="C88" t="s">
-        <v>283</v>
+        <v>281</v>
       </c>
       <c r="D88">
         <v>0</v>
@@ -5589,22 +5598,22 @@
         <v>0</v>
       </c>
       <c r="M88">
-        <f>M87*4</f>
-        <v>4.40488377086E-3</v>
+        <f>M87*2</f>
+        <v>1.101220942715E-3</v>
       </c>
       <c r="N88" t="s">
-        <v>288</v>
+        <v>285</v>
       </c>
     </row>
     <row r="89" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A89" t="s">
-        <v>248</v>
+        <v>434</v>
       </c>
       <c r="B89" t="s">
-        <v>354</v>
+        <v>352</v>
       </c>
       <c r="C89" t="s">
-        <v>355</v>
+        <v>282</v>
       </c>
       <c r="D89">
         <v>0</v>
@@ -5634,22 +5643,22 @@
         <v>0</v>
       </c>
       <c r="M89">
-        <f>M88*2</f>
-        <v>8.8097675417200001E-3</v>
+        <f>M88*4</f>
+        <v>4.40488377086E-3</v>
       </c>
       <c r="N89" t="s">
-        <v>290</v>
+        <v>287</v>
       </c>
     </row>
     <row r="90" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A90" t="s">
-        <v>248</v>
+        <v>434</v>
       </c>
       <c r="B90" t="s">
-        <v>359</v>
+        <v>353</v>
       </c>
       <c r="C90" t="s">
-        <v>285</v>
+        <v>354</v>
       </c>
       <c r="D90">
         <v>0</v>
@@ -5679,8 +5688,8 @@
         <v>0</v>
       </c>
       <c r="M90">
-        <f>M89*4</f>
-        <v>3.523907016688E-2</v>
+        <f>M89*2</f>
+        <v>8.8097675417200001E-3</v>
       </c>
       <c r="N90" t="s">
         <v>289</v>
@@ -5688,22 +5697,22 @@
     </row>
     <row r="91" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A91" t="s">
-        <v>77</v>
+        <v>434</v>
       </c>
       <c r="B91" t="s">
-        <v>84</v>
+        <v>358</v>
       </c>
       <c r="C91" t="s">
-        <v>89</v>
+        <v>284</v>
       </c>
       <c r="D91">
         <v>0</v>
       </c>
       <c r="E91">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="F91">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G91">
         <v>0</v>
@@ -5724,11 +5733,11 @@
         <v>0</v>
       </c>
       <c r="M91">
-        <f>M94/7000</f>
-        <v>6.4798910000000008E-5</v>
+        <f>M90*4</f>
+        <v>3.523907016688E-2</v>
       </c>
       <c r="N91" t="s">
-        <v>190</v>
+        <v>288</v>
       </c>
     </row>
     <row r="92" spans="1:14" x14ac:dyDescent="0.3">
@@ -5736,10 +5745,10 @@
         <v>77</v>
       </c>
       <c r="B92" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="C92" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="D92">
         <v>0</v>
@@ -5769,11 +5778,11 @@
         <v>0</v>
       </c>
       <c r="M92">
-        <f>M94/256</f>
-        <v>1.7718451953125001E-3</v>
+        <f>M95/7000</f>
+        <v>6.4798910000000008E-5</v>
       </c>
       <c r="N92" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
     </row>
     <row r="93" spans="1:14" x14ac:dyDescent="0.3">
@@ -5781,10 +5790,10 @@
         <v>77</v>
       </c>
       <c r="B93" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="C93" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="D93">
         <v>0</v>
@@ -5814,11 +5823,11 @@
         <v>0</v>
       </c>
       <c r="M93">
-        <f>M94/16</f>
-        <v>2.8349523125000001E-2</v>
+        <f>M95/256</f>
+        <v>1.7718451953125001E-3</v>
       </c>
       <c r="N93" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
     </row>
     <row r="94" spans="1:14" x14ac:dyDescent="0.3">
@@ -5826,10 +5835,10 @@
         <v>77</v>
       </c>
       <c r="B94" t="s">
-        <v>136</v>
+        <v>86</v>
       </c>
       <c r="C94" t="s">
-        <v>204</v>
+        <v>91</v>
       </c>
       <c r="D94">
         <v>0</v>
@@ -5859,11 +5868,11 @@
         <v>0</v>
       </c>
       <c r="M94">
-        <f>0.45359237</f>
-        <v>0.45359237000000002</v>
+        <f>M95/16</f>
+        <v>2.8349523125000001E-2</v>
       </c>
       <c r="N94" t="s">
-        <v>257</v>
+        <v>192</v>
       </c>
     </row>
     <row r="95" spans="1:14" x14ac:dyDescent="0.3">
@@ -5871,10 +5880,10 @@
         <v>77</v>
       </c>
       <c r="B95" t="s">
-        <v>92</v>
+        <v>136</v>
       </c>
       <c r="C95" t="s">
-        <v>93</v>
+        <v>204</v>
       </c>
       <c r="D95">
         <v>0</v>
@@ -5904,11 +5913,11 @@
         <v>0</v>
       </c>
       <c r="M95">
-        <f>M94*14</f>
-        <v>6.3502931800000004</v>
+        <f>0.45359237</f>
+        <v>0.45359237000000002</v>
       </c>
       <c r="N95" t="s">
-        <v>193</v>
+        <v>256</v>
       </c>
     </row>
     <row r="96" spans="1:14" x14ac:dyDescent="0.3">
@@ -5916,10 +5925,10 @@
         <v>77</v>
       </c>
       <c r="B96" t="s">
-        <v>87</v>
+        <v>92</v>
       </c>
       <c r="C96" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="D96">
         <v>0</v>
@@ -5949,11 +5958,11 @@
         <v>0</v>
       </c>
       <c r="M96">
-        <f>M94*28</f>
-        <v>12.700586360000001</v>
+        <f>M95*14</f>
+        <v>6.3502931800000004</v>
       </c>
       <c r="N96" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
     </row>
     <row r="97" spans="1:14" x14ac:dyDescent="0.3">
@@ -5961,10 +5970,10 @@
         <v>77</v>
       </c>
       <c r="B97" t="s">
-        <v>348</v>
+        <v>87</v>
       </c>
       <c r="C97" t="s">
-        <v>252</v>
+        <v>94</v>
       </c>
       <c r="D97">
         <v>0</v>
@@ -5994,11 +6003,11 @@
         <v>0</v>
       </c>
       <c r="M97">
-        <f>M94*112</f>
-        <v>50.802345440000003</v>
+        <f>M95*28</f>
+        <v>12.700586360000001</v>
       </c>
       <c r="N97" t="s">
-        <v>253</v>
+        <v>194</v>
       </c>
     </row>
     <row r="98" spans="1:14" x14ac:dyDescent="0.3">
@@ -6009,7 +6018,7 @@
         <v>347</v>
       </c>
       <c r="C98" t="s">
-        <v>255</v>
+        <v>251</v>
       </c>
       <c r="D98">
         <v>0</v>
@@ -6039,22 +6048,22 @@
         <v>0</v>
       </c>
       <c r="M98">
-        <f>M97*20</f>
-        <v>1016.0469088000001</v>
+        <f>M95*112</f>
+        <v>50.802345440000003</v>
       </c>
       <c r="N98" t="s">
-        <v>254</v>
+        <v>252</v>
       </c>
     </row>
     <row r="99" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A99" t="s">
-        <v>248</v>
+        <v>77</v>
       </c>
       <c r="B99" t="s">
         <v>346</v>
       </c>
       <c r="C99" t="s">
-        <v>258</v>
+        <v>254</v>
       </c>
       <c r="D99">
         <v>0</v>
@@ -6084,22 +6093,22 @@
         <v>0</v>
       </c>
       <c r="M99">
-        <f>M94*100</f>
-        <v>45.359237</v>
+        <f>M98*20</f>
+        <v>1016.0469088000001</v>
       </c>
       <c r="N99" t="s">
-        <v>259</v>
+        <v>253</v>
       </c>
     </row>
     <row r="100" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A100" t="s">
-        <v>248</v>
+        <v>434</v>
       </c>
       <c r="B100" t="s">
         <v>345</v>
       </c>
       <c r="C100" t="s">
-        <v>256</v>
+        <v>257</v>
       </c>
       <c r="D100">
         <v>0</v>
@@ -6129,22 +6138,22 @@
         <v>0</v>
       </c>
       <c r="M100">
-        <f>M99*20</f>
-        <v>907.18474000000003</v>
+        <f>M95*100</f>
+        <v>45.359237</v>
       </c>
       <c r="N100" t="s">
-        <v>260</v>
+        <v>258</v>
       </c>
     </row>
     <row r="101" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A101" t="s">
-        <v>77</v>
+        <v>434</v>
       </c>
       <c r="B101" t="s">
-        <v>88</v>
+        <v>344</v>
       </c>
       <c r="C101" t="s">
-        <v>88</v>
+        <v>255</v>
       </c>
       <c r="D101">
         <v>0</v>
@@ -6174,11 +6183,11 @@
         <v>0</v>
       </c>
       <c r="M101">
-        <f>M45/M60*M94</f>
-        <v>14.593902937206368</v>
+        <f>M100*20</f>
+        <v>907.18474000000003</v>
       </c>
       <c r="N101" t="s">
-        <v>195</v>
+        <v>259</v>
       </c>
     </row>
     <row r="102" spans="1:14" x14ac:dyDescent="0.3">
@@ -6186,16 +6195,16 @@
         <v>77</v>
       </c>
       <c r="B102" t="s">
-        <v>134</v>
+        <v>88</v>
       </c>
       <c r="C102" t="s">
-        <v>135</v>
+        <v>88</v>
       </c>
       <c r="D102">
-        <v>-2</v>
+        <v>0</v>
       </c>
       <c r="E102">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F102">
         <v>1</v>
@@ -6219,11 +6228,11 @@
         <v>0</v>
       </c>
       <c r="M102">
-        <f>M45*M94</f>
-        <v>4.4482216152604996</v>
+        <f>M46/M61*M95</f>
+        <v>14.593902937206368</v>
       </c>
       <c r="N102" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
     </row>
     <row r="103" spans="1:14" x14ac:dyDescent="0.3">
@@ -6231,16 +6240,16 @@
         <v>77</v>
       </c>
       <c r="B103" t="s">
-        <v>216</v>
+        <v>134</v>
       </c>
       <c r="C103" t="s">
-        <v>217</v>
+        <v>135</v>
       </c>
       <c r="D103">
         <v>-2</v>
       </c>
       <c r="E103">
-        <v>-1</v>
+        <v>1</v>
       </c>
       <c r="F103">
         <v>1</v>
@@ -6264,11 +6273,11 @@
         <v>0</v>
       </c>
       <c r="M103">
-        <f>M102 / (M58 *M58)</f>
-        <v>6894.7572931683608</v>
+        <f>M46*M95</f>
+        <v>4.4482216152604996</v>
       </c>
       <c r="N103" t="s">
-        <v>218</v>
+        <v>196</v>
       </c>
     </row>
     <row r="104" spans="1:14" x14ac:dyDescent="0.3">
@@ -6276,16 +6285,16 @@
         <v>77</v>
       </c>
       <c r="B104" t="s">
-        <v>120</v>
+        <v>216</v>
       </c>
       <c r="C104" t="s">
-        <v>121</v>
+        <v>217</v>
       </c>
       <c r="D104">
-        <v>-3</v>
+        <v>-2</v>
       </c>
       <c r="E104">
-        <v>2</v>
+        <v>-1</v>
       </c>
       <c r="F104">
         <v>1</v>
@@ -6309,11 +6318,11 @@
         <v>0</v>
       </c>
       <c r="M104">
-        <f>(550 *M94*M45*M60)</f>
-        <v>745.69987158227002</v>
+        <f>M103 / (M59 *M59)</f>
+        <v>6894.7572931683608</v>
       </c>
       <c r="N104" t="s">
-        <v>131</v>
+        <v>218</v>
       </c>
     </row>
     <row r="105" spans="1:14" x14ac:dyDescent="0.3">
@@ -6321,25 +6330,25 @@
         <v>77</v>
       </c>
       <c r="B105" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
       <c r="C105" t="s">
-        <v>116</v>
+        <v>121</v>
       </c>
       <c r="D105">
-        <v>0</v>
+        <v>-3</v>
       </c>
       <c r="E105">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="F105">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G105">
         <v>0</v>
       </c>
       <c r="H105">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I105">
         <v>0</v>
@@ -6354,11 +6363,11 @@
         <v>0</v>
       </c>
       <c r="M105">
-        <f>5/9</f>
-        <v>0.55555555555555558</v>
+        <f>(550 *M95*M46*M61)</f>
+        <v>745.69987158227002</v>
       </c>
       <c r="N105" t="s">
-        <v>198</v>
+        <v>131</v>
       </c>
     </row>
     <row r="106" spans="1:14" x14ac:dyDescent="0.3">
@@ -6366,10 +6375,10 @@
         <v>77</v>
       </c>
       <c r="B106" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="C106" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="D106">
         <v>0</v>
@@ -6403,7 +6412,7 @@
         <v>0.55555555555555558</v>
       </c>
       <c r="N106" t="s">
-        <v>197</v>
+        <v>198</v>
       </c>
     </row>
     <row r="107" spans="1:14" x14ac:dyDescent="0.3">
@@ -6411,25 +6420,25 @@
         <v>77</v>
       </c>
       <c r="B107" t="s">
-        <v>338</v>
+        <v>123</v>
       </c>
       <c r="C107" t="s">
-        <v>201</v>
+        <v>117</v>
       </c>
       <c r="D107">
-        <v>-2</v>
+        <v>0</v>
       </c>
       <c r="E107">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="F107">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G107">
         <v>0</v>
       </c>
       <c r="H107">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I107">
         <v>0</v>
@@ -6444,10 +6453,11 @@
         <v>0</v>
       </c>
       <c r="M107">
-        <v>4.1840000000000002</v>
+        <f>5/9</f>
+        <v>0.55555555555555558</v>
       </c>
       <c r="N107" t="s">
-        <v>247</v>
+        <v>197</v>
       </c>
     </row>
     <row r="108" spans="1:14" x14ac:dyDescent="0.3">
@@ -6455,10 +6465,10 @@
         <v>77</v>
       </c>
       <c r="B108" t="s">
-        <v>339</v>
+        <v>337</v>
       </c>
       <c r="C108" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="D108">
         <v>-2</v>
@@ -6488,11 +6498,10 @@
         <v>0</v>
       </c>
       <c r="M108">
-        <f>M107/M4</f>
-        <v>4184</v>
+        <v>4.1840000000000002</v>
       </c>
       <c r="N108" t="s">
-        <v>203</v>
+        <v>247</v>
       </c>
     </row>
     <row r="109" spans="1:14" x14ac:dyDescent="0.3">
@@ -6500,10 +6509,10 @@
         <v>77</v>
       </c>
       <c r="B109" t="s">
-        <v>366</v>
+        <v>338</v>
       </c>
       <c r="C109" t="s">
-        <v>206</v>
+        <v>202</v>
       </c>
       <c r="D109">
         <v>-2</v>
@@ -6533,11 +6542,11 @@
         <v>0</v>
       </c>
       <c r="M109">
-        <f>4.1868</f>
-        <v>4.1867999999999999</v>
+        <f>M108/M4</f>
+        <v>4184</v>
       </c>
       <c r="N109" t="s">
-        <v>251</v>
+        <v>203</v>
       </c>
     </row>
     <row r="110" spans="1:14" x14ac:dyDescent="0.3">
@@ -6545,10 +6554,10 @@
         <v>77</v>
       </c>
       <c r="B110" t="s">
-        <v>367</v>
+        <v>365</v>
       </c>
       <c r="C110" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="D110">
         <v>-2</v>
@@ -6578,11 +6587,11 @@
         <v>0</v>
       </c>
       <c r="M110">
-        <f>M109/M4</f>
-        <v>4186.8</v>
+        <f>4.1868</f>
+        <v>4.1867999999999999</v>
       </c>
       <c r="N110" t="s">
-        <v>208</v>
+        <v>250</v>
       </c>
     </row>
     <row r="111" spans="1:14" x14ac:dyDescent="0.3">
@@ -6590,10 +6599,10 @@
         <v>77</v>
       </c>
       <c r="B111" t="s">
-        <v>340</v>
+        <v>366</v>
       </c>
       <c r="C111" t="s">
-        <v>200</v>
+        <v>207</v>
       </c>
       <c r="D111">
         <v>-2</v>
@@ -6623,11 +6632,11 @@
         <v>0</v>
       </c>
       <c r="M111">
-        <f>M108*M94*M105</f>
-        <v>1054.350264488889</v>
+        <f>M110/M4</f>
+        <v>4186.8</v>
       </c>
       <c r="N111" t="s">
-        <v>205</v>
+        <v>208</v>
       </c>
     </row>
     <row r="112" spans="1:14" x14ac:dyDescent="0.3">
@@ -6635,10 +6644,10 @@
         <v>77</v>
       </c>
       <c r="B112" t="s">
-        <v>368</v>
+        <v>339</v>
       </c>
       <c r="C112" t="s">
-        <v>209</v>
+        <v>200</v>
       </c>
       <c r="D112">
         <v>-2</v>
@@ -6668,11 +6677,11 @@
         <v>0</v>
       </c>
       <c r="M112">
-        <f>M110*M94*M105</f>
-        <v>1055.05585262</v>
+        <f>M109*M95*M106</f>
+        <v>1054.350264488889</v>
       </c>
       <c r="N112" t="s">
-        <v>210</v>
+        <v>205</v>
       </c>
     </row>
     <row r="113" spans="1:14" x14ac:dyDescent="0.3">
@@ -6680,10 +6689,10 @@
         <v>77</v>
       </c>
       <c r="B113" t="s">
-        <v>211</v>
+        <v>367</v>
       </c>
       <c r="C113" t="s">
-        <v>213</v>
+        <v>209</v>
       </c>
       <c r="D113">
         <v>-2</v>
@@ -6713,11 +6722,11 @@
         <v>0</v>
       </c>
       <c r="M113">
-        <f>M112*100000</f>
-        <v>105505585.26199999</v>
+        <f>M111*M95*M106</f>
+        <v>1055.05585262</v>
       </c>
       <c r="N113" t="s">
-        <v>215</v>
+        <v>210</v>
       </c>
     </row>
     <row r="114" spans="1:14" x14ac:dyDescent="0.3">
@@ -6725,10 +6734,10 @@
         <v>77</v>
       </c>
       <c r="B114" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="C114" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="D114">
         <v>-2</v>
@@ -6758,8 +6767,8 @@
         <v>0</v>
       </c>
       <c r="M114">
-        <f>M112*POWER(10,15)</f>
-        <v>1.05505585262E+18</v>
+        <f>M113*100000</f>
+        <v>105505585.26199999</v>
       </c>
       <c r="N114" t="s">
         <v>215</v>
@@ -6767,21 +6776,55 @@
     </row>
     <row r="115" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A115" t="s">
-        <v>375</v>
+        <v>77</v>
       </c>
       <c r="B115" t="s">
-        <v>378</v>
+        <v>212</v>
+      </c>
+      <c r="C115" t="s">
+        <v>214</v>
+      </c>
+      <c r="D115">
+        <v>-2</v>
+      </c>
+      <c r="E115">
+        <v>2</v>
+      </c>
+      <c r="F115">
+        <v>1</v>
+      </c>
+      <c r="G115">
+        <v>0</v>
+      </c>
+      <c r="H115">
+        <v>0</v>
+      </c>
+      <c r="I115">
+        <v>0</v>
+      </c>
+      <c r="J115">
+        <v>0</v>
+      </c>
+      <c r="K115">
+        <v>0</v>
+      </c>
+      <c r="L115">
+        <v>0</v>
       </c>
       <c r="M115">
-        <v>0</v>
+        <f>M113*POWER(10,15)</f>
+        <v>1.05505585262E+18</v>
+      </c>
+      <c r="N115" t="s">
+        <v>215</v>
       </c>
     </row>
     <row r="116" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A116" t="s">
-        <v>375</v>
+        <v>374</v>
       </c>
       <c r="B116" t="s">
-        <v>327</v>
+        <v>377</v>
       </c>
       <c r="M116">
         <v>0</v>
@@ -6789,10 +6832,10 @@
     </row>
     <row r="117" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A117" t="s">
-        <v>375</v>
+        <v>374</v>
       </c>
       <c r="B117" t="s">
-        <v>379</v>
+        <v>326</v>
       </c>
       <c r="M117">
         <v>0</v>
@@ -6800,35 +6843,35 @@
     </row>
     <row r="118" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A118" t="s">
-        <v>375</v>
+        <v>374</v>
       </c>
       <c r="B118" t="s">
-        <v>316</v>
+        <v>378</v>
       </c>
       <c r="M118">
         <v>0</v>
-      </c>
-      <c r="N118" t="s">
-        <v>411</v>
       </c>
     </row>
     <row r="119" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A119" t="s">
-        <v>375</v>
+        <v>374</v>
       </c>
       <c r="B119" t="s">
-        <v>380</v>
+        <v>315</v>
       </c>
       <c r="M119">
         <v>0</v>
+      </c>
+      <c r="N119" t="s">
+        <v>410</v>
       </c>
     </row>
     <row r="120" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A120" t="s">
-        <v>375</v>
+        <v>374</v>
       </c>
       <c r="B120" t="s">
-        <v>381</v>
+        <v>379</v>
       </c>
       <c r="M120">
         <v>0</v>
@@ -6836,245 +6879,215 @@
     </row>
     <row r="121" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A121" t="s">
-        <v>375</v>
+        <v>374</v>
       </c>
       <c r="B121" t="s">
-        <v>382</v>
+        <v>380</v>
       </c>
       <c r="M121">
         <v>0</v>
-      </c>
-      <c r="N121" t="s">
-        <v>416</v>
       </c>
     </row>
     <row r="122" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A122" t="s">
-        <v>375</v>
+        <v>374</v>
       </c>
       <c r="B122" t="s">
-        <v>383</v>
+        <v>381</v>
       </c>
       <c r="M122">
         <v>0</v>
       </c>
       <c r="N122" t="s">
-        <v>412</v>
+        <v>415</v>
       </c>
     </row>
     <row r="123" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A123" t="s">
-        <v>375</v>
+        <v>374</v>
       </c>
       <c r="B123" t="s">
-        <v>384</v>
-      </c>
-      <c r="D123">
-        <v>-3</v>
-      </c>
-      <c r="E123">
-        <v>2</v>
-      </c>
-      <c r="F123">
-        <v>1</v>
-      </c>
-      <c r="G123">
-        <v>0</v>
-      </c>
-      <c r="H123">
-        <v>0</v>
-      </c>
-      <c r="I123">
-        <v>0</v>
-      </c>
-      <c r="J123">
-        <v>0</v>
-      </c>
-      <c r="K123">
-        <v>0</v>
-      </c>
-      <c r="L123">
-        <v>0</v>
+        <v>382</v>
       </c>
       <c r="M123">
-        <v>-150</v>
+        <v>0</v>
       </c>
       <c r="N123" t="s">
-        <v>429</v>
+        <v>411</v>
       </c>
     </row>
     <row r="124" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A124" t="s">
-        <v>375</v>
+        <v>374</v>
       </c>
       <c r="B124" t="s">
-        <v>385</v>
+        <v>383</v>
+      </c>
+      <c r="D124">
+        <v>-3</v>
+      </c>
+      <c r="E124">
+        <v>2</v>
+      </c>
+      <c r="F124">
+        <v>1</v>
+      </c>
+      <c r="G124">
+        <v>0</v>
+      </c>
+      <c r="H124">
+        <v>0</v>
+      </c>
+      <c r="I124">
+        <v>0</v>
+      </c>
+      <c r="J124">
+        <v>0</v>
+      </c>
+      <c r="K124">
+        <v>0</v>
+      </c>
+      <c r="L124">
+        <v>0</v>
       </c>
       <c r="M124">
-        <v>0</v>
+        <v>-150</v>
       </c>
       <c r="N124" t="s">
-        <v>413</v>
+        <v>428</v>
       </c>
     </row>
     <row r="125" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A125" t="s">
-        <v>375</v>
+        <v>374</v>
       </c>
       <c r="B125" t="s">
-        <v>305</v>
+        <v>384</v>
       </c>
       <c r="M125">
         <v>0</v>
       </c>
       <c r="N125" t="s">
-        <v>414</v>
+        <v>412</v>
       </c>
     </row>
     <row r="126" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A126" t="s">
-        <v>375</v>
+        <v>374</v>
       </c>
       <c r="B126" t="s">
-        <v>386</v>
+        <v>304</v>
       </c>
       <c r="M126">
         <v>0</v>
       </c>
       <c r="N126" t="s">
-        <v>415</v>
+        <v>413</v>
       </c>
     </row>
     <row r="127" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A127" t="s">
-        <v>375</v>
+        <v>374</v>
       </c>
       <c r="B127" t="s">
-        <v>387</v>
+        <v>385</v>
       </c>
       <c r="M127">
         <v>0</v>
       </c>
       <c r="N127" t="s">
-        <v>417</v>
+        <v>414</v>
       </c>
     </row>
     <row r="128" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A128" t="s">
-        <v>375</v>
+        <v>374</v>
       </c>
       <c r="B128" t="s">
-        <v>24</v>
+        <v>386</v>
       </c>
       <c r="M128">
         <v>0</v>
       </c>
       <c r="N128" t="s">
-        <v>418</v>
+        <v>416</v>
       </c>
     </row>
     <row r="129" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A129" t="s">
-        <v>375</v>
+        <v>374</v>
       </c>
       <c r="B129" t="s">
-        <v>388</v>
-      </c>
-      <c r="D129">
-        <v>-3</v>
-      </c>
-      <c r="E129">
-        <v>2</v>
-      </c>
-      <c r="F129">
-        <v>1</v>
-      </c>
-      <c r="G129">
-        <v>0</v>
-      </c>
-      <c r="H129">
-        <v>0</v>
-      </c>
-      <c r="I129">
-        <v>0</v>
-      </c>
-      <c r="J129">
-        <v>0</v>
-      </c>
-      <c r="K129">
-        <v>0</v>
-      </c>
-      <c r="L129">
-        <v>0</v>
+        <v>24</v>
       </c>
       <c r="M129">
-        <v>30</v>
+        <v>0</v>
       </c>
       <c r="N129" t="s">
-        <v>428</v>
+        <v>417</v>
       </c>
     </row>
     <row r="130" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A130" t="s">
-        <v>375</v>
+        <v>374</v>
       </c>
       <c r="B130" t="s">
-        <v>389</v>
+        <v>387</v>
+      </c>
+      <c r="D130">
+        <v>-3</v>
+      </c>
+      <c r="E130">
+        <v>2</v>
+      </c>
+      <c r="F130">
+        <v>1</v>
+      </c>
+      <c r="G130">
+        <v>0</v>
+      </c>
+      <c r="H130">
+        <v>0</v>
+      </c>
+      <c r="I130">
+        <v>0</v>
+      </c>
+      <c r="J130">
+        <v>0</v>
+      </c>
+      <c r="K130">
+        <v>0</v>
+      </c>
+      <c r="L130">
+        <v>0</v>
       </c>
       <c r="M130">
-        <v>0</v>
+        <v>30</v>
       </c>
       <c r="N130" t="s">
-        <v>419</v>
+        <v>427</v>
       </c>
     </row>
     <row r="131" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A131" t="s">
-        <v>375</v>
+        <v>374</v>
       </c>
       <c r="B131" t="s">
-        <v>390</v>
-      </c>
-      <c r="D131">
-        <v>-3</v>
-      </c>
-      <c r="E131">
-        <v>2</v>
-      </c>
-      <c r="F131">
-        <v>1</v>
-      </c>
-      <c r="G131">
-        <v>0</v>
-      </c>
-      <c r="H131">
-        <v>0</v>
-      </c>
-      <c r="I131">
-        <v>0</v>
-      </c>
-      <c r="J131">
-        <v>0</v>
-      </c>
-      <c r="K131">
-        <v>0</v>
-      </c>
-      <c r="L131">
-        <v>0</v>
+        <v>388</v>
       </c>
       <c r="M131">
-        <v>-30</v>
+        <v>0</v>
       </c>
       <c r="N131" t="s">
-        <v>430</v>
+        <v>418</v>
       </c>
     </row>
     <row r="132" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A132" t="s">
-        <v>375</v>
+        <v>374</v>
       </c>
       <c r="B132" t="s">
-        <v>426</v>
+        <v>389</v>
       </c>
       <c r="D132">
         <v>-3</v>
@@ -7103,76 +7116,106 @@
       <c r="L132">
         <v>0</v>
       </c>
+      <c r="M132">
+        <v>-30</v>
+      </c>
+      <c r="N132" t="s">
+        <v>429</v>
+      </c>
     </row>
     <row r="133" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A133" t="s">
-        <v>375</v>
+        <v>374</v>
       </c>
       <c r="B133" t="s">
-        <v>391</v>
-      </c>
-      <c r="M133">
+        <v>425</v>
+      </c>
+      <c r="D133">
+        <v>-3</v>
+      </c>
+      <c r="E133">
+        <v>2</v>
+      </c>
+      <c r="F133">
+        <v>1</v>
+      </c>
+      <c r="G133">
+        <v>0</v>
+      </c>
+      <c r="H133">
+        <v>0</v>
+      </c>
+      <c r="I133">
+        <v>0</v>
+      </c>
+      <c r="J133">
+        <v>0</v>
+      </c>
+      <c r="K133">
+        <v>0</v>
+      </c>
+      <c r="L133">
         <v>0</v>
       </c>
     </row>
     <row r="134" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A134" t="s">
-        <v>375</v>
+        <v>374</v>
       </c>
       <c r="B134" t="s">
-        <v>392</v>
-      </c>
-      <c r="D134">
-        <v>-3</v>
-      </c>
-      <c r="E134">
-        <v>2</v>
-      </c>
-      <c r="F134">
-        <v>1</v>
-      </c>
-      <c r="G134">
-        <v>-1</v>
-      </c>
-      <c r="H134">
-        <v>0</v>
-      </c>
-      <c r="I134">
-        <v>0</v>
-      </c>
-      <c r="J134">
-        <v>0</v>
-      </c>
-      <c r="K134">
-        <v>0</v>
-      </c>
-      <c r="L134">
-        <v>0</v>
+        <v>390</v>
       </c>
       <c r="M134">
         <v>0</v>
-      </c>
-      <c r="N134" t="s">
-        <v>420</v>
       </c>
     </row>
     <row r="135" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A135" t="s">
-        <v>375</v>
+        <v>374</v>
       </c>
       <c r="B135" t="s">
-        <v>393</v>
+        <v>391</v>
+      </c>
+      <c r="D135">
+        <v>-3</v>
+      </c>
+      <c r="E135">
+        <v>2</v>
+      </c>
+      <c r="F135">
+        <v>1</v>
+      </c>
+      <c r="G135">
+        <v>-1</v>
+      </c>
+      <c r="H135">
+        <v>0</v>
+      </c>
+      <c r="I135">
+        <v>0</v>
+      </c>
+      <c r="J135">
+        <v>0</v>
+      </c>
+      <c r="K135">
+        <v>0</v>
+      </c>
+      <c r="L135">
+        <v>0</v>
       </c>
       <c r="M135">
         <v>0</v>
+      </c>
+      <c r="N135" t="s">
+        <v>419</v>
       </c>
     </row>
     <row r="136" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A136" t="s">
-        <v>375</v>
+        <v>374</v>
       </c>
       <c r="B136" t="s">
-        <v>394</v>
+        <v>392</v>
       </c>
       <c r="M136">
         <v>0</v>
@@ -7180,10 +7223,10 @@
     </row>
     <row r="137" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A137" t="s">
-        <v>375</v>
+        <v>374</v>
       </c>
       <c r="B137" t="s">
-        <v>395</v>
+        <v>393</v>
       </c>
       <c r="M137">
         <v>0</v>
@@ -7191,10 +7234,10 @@
     </row>
     <row r="138" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A138" t="s">
-        <v>375</v>
+        <v>374</v>
       </c>
       <c r="B138" t="s">
-        <v>396</v>
+        <v>394</v>
       </c>
       <c r="M138">
         <v>0</v>
@@ -7202,10 +7245,10 @@
     </row>
     <row r="139" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A139" t="s">
-        <v>375</v>
+        <v>374</v>
       </c>
       <c r="B139" t="s">
-        <v>397</v>
+        <v>395</v>
       </c>
       <c r="M139">
         <v>0</v>
@@ -7213,37 +7256,10 @@
     </row>
     <row r="140" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A140" t="s">
-        <v>375</v>
+        <v>374</v>
       </c>
       <c r="B140" t="s">
-        <v>398</v>
-      </c>
-      <c r="D140">
-        <v>0</v>
-      </c>
-      <c r="E140">
-        <v>2</v>
-      </c>
-      <c r="F140">
-        <v>0</v>
-      </c>
-      <c r="G140">
-        <v>0</v>
-      </c>
-      <c r="H140">
-        <v>0</v>
-      </c>
-      <c r="I140">
-        <v>0</v>
-      </c>
-      <c r="J140">
-        <v>0</v>
-      </c>
-      <c r="K140">
-        <v>0</v>
-      </c>
-      <c r="L140">
-        <v>0</v>
+        <v>396</v>
       </c>
       <c r="M140">
         <v>0</v>
@@ -7251,10 +7267,37 @@
     </row>
     <row r="141" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A141" t="s">
-        <v>375</v>
+        <v>374</v>
       </c>
       <c r="B141" t="s">
-        <v>399</v>
+        <v>397</v>
+      </c>
+      <c r="D141">
+        <v>0</v>
+      </c>
+      <c r="E141">
+        <v>2</v>
+      </c>
+      <c r="F141">
+        <v>0</v>
+      </c>
+      <c r="G141">
+        <v>0</v>
+      </c>
+      <c r="H141">
+        <v>0</v>
+      </c>
+      <c r="I141">
+        <v>0</v>
+      </c>
+      <c r="J141">
+        <v>0</v>
+      </c>
+      <c r="K141">
+        <v>0</v>
+      </c>
+      <c r="L141">
+        <v>0</v>
       </c>
       <c r="M141">
         <v>0</v>
@@ -7262,191 +7305,191 @@
     </row>
     <row r="142" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A142" t="s">
-        <v>375</v>
+        <v>374</v>
       </c>
       <c r="B142" t="s">
-        <v>400</v>
-      </c>
-      <c r="D142">
-        <v>-3</v>
-      </c>
-      <c r="E142">
-        <v>2</v>
-      </c>
-      <c r="F142">
-        <v>1</v>
-      </c>
-      <c r="G142">
-        <v>-1</v>
-      </c>
-      <c r="H142">
-        <v>0</v>
-      </c>
-      <c r="I142">
-        <v>0</v>
-      </c>
-      <c r="J142">
-        <v>0</v>
-      </c>
-      <c r="K142">
-        <v>0</v>
-      </c>
-      <c r="L142">
-        <v>0</v>
+        <v>398</v>
       </c>
       <c r="M142">
         <v>0</v>
-      </c>
-      <c r="N142" t="s">
-        <v>424</v>
       </c>
     </row>
     <row r="143" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A143" t="s">
-        <v>375</v>
+        <v>374</v>
       </c>
       <c r="B143" t="s">
-        <v>401</v>
+        <v>399</v>
+      </c>
+      <c r="D143">
+        <v>-3</v>
+      </c>
+      <c r="E143">
+        <v>2</v>
+      </c>
+      <c r="F143">
+        <v>1</v>
+      </c>
+      <c r="G143">
+        <v>-1</v>
+      </c>
+      <c r="H143">
+        <v>0</v>
+      </c>
+      <c r="I143">
+        <v>0</v>
+      </c>
+      <c r="J143">
+        <v>0</v>
+      </c>
+      <c r="K143">
+        <v>0</v>
+      </c>
+      <c r="L143">
+        <v>0</v>
       </c>
       <c r="M143">
         <v>0</v>
+      </c>
+      <c r="N143" t="s">
+        <v>423</v>
       </c>
     </row>
     <row r="144" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A144" t="s">
-        <v>375</v>
+        <v>374</v>
       </c>
       <c r="B144" t="s">
-        <v>402</v>
-      </c>
-      <c r="D144">
-        <v>-3</v>
-      </c>
-      <c r="E144">
-        <v>2</v>
-      </c>
-      <c r="F144">
-        <v>1</v>
-      </c>
-      <c r="G144">
-        <v>-1</v>
-      </c>
-      <c r="H144">
-        <v>0</v>
-      </c>
-      <c r="I144">
-        <v>0</v>
-      </c>
-      <c r="J144">
-        <v>0</v>
-      </c>
-      <c r="K144">
-        <v>0</v>
-      </c>
-      <c r="L144">
-        <v>0</v>
+        <v>400</v>
       </c>
       <c r="M144">
         <v>0</v>
-      </c>
-      <c r="N144" t="s">
-        <v>427</v>
       </c>
     </row>
     <row r="145" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A145" t="s">
-        <v>375</v>
+        <v>374</v>
       </c>
       <c r="B145" t="s">
-        <v>403</v>
+        <v>401</v>
+      </c>
+      <c r="D145">
+        <v>-3</v>
+      </c>
+      <c r="E145">
+        <v>2</v>
+      </c>
+      <c r="F145">
+        <v>1</v>
+      </c>
+      <c r="G145">
+        <v>-1</v>
+      </c>
+      <c r="H145">
+        <v>0</v>
+      </c>
+      <c r="I145">
+        <v>0</v>
+      </c>
+      <c r="J145">
+        <v>0</v>
+      </c>
+      <c r="K145">
+        <v>0</v>
+      </c>
+      <c r="L145">
+        <v>0</v>
       </c>
       <c r="M145">
         <v>0</v>
+      </c>
+      <c r="N145" t="s">
+        <v>426</v>
       </c>
     </row>
     <row r="146" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A146" t="s">
-        <v>375</v>
+        <v>374</v>
       </c>
       <c r="B146" t="s">
-        <v>404</v>
+        <v>402</v>
       </c>
       <c r="M146">
         <v>0</v>
-      </c>
-      <c r="N146" t="s">
-        <v>425</v>
       </c>
     </row>
     <row r="147" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A147" t="s">
-        <v>375</v>
+        <v>374</v>
       </c>
       <c r="B147" t="s">
-        <v>405</v>
+        <v>403</v>
       </c>
       <c r="M147">
         <v>0</v>
+      </c>
+      <c r="N147" t="s">
+        <v>424</v>
       </c>
     </row>
     <row r="148" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A148" t="s">
-        <v>375</v>
+        <v>374</v>
       </c>
       <c r="B148" t="s">
-        <v>25</v>
-      </c>
-      <c r="D148">
-        <v>-3</v>
-      </c>
-      <c r="E148">
-        <v>2</v>
-      </c>
-      <c r="F148">
-        <v>1</v>
-      </c>
-      <c r="G148">
-        <v>0</v>
-      </c>
-      <c r="H148">
-        <v>0</v>
-      </c>
-      <c r="I148">
-        <v>0</v>
-      </c>
-      <c r="J148">
-        <v>0</v>
-      </c>
-      <c r="K148">
-        <v>0</v>
-      </c>
-      <c r="L148">
-        <v>0</v>
+        <v>404</v>
       </c>
       <c r="M148">
         <v>0</v>
-      </c>
-      <c r="N148" t="s">
-        <v>431</v>
       </c>
     </row>
     <row r="149" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A149" t="s">
-        <v>375</v>
+        <v>374</v>
       </c>
       <c r="B149" t="s">
-        <v>406</v>
+        <v>25</v>
+      </c>
+      <c r="D149">
+        <v>-3</v>
+      </c>
+      <c r="E149">
+        <v>2</v>
+      </c>
+      <c r="F149">
+        <v>1</v>
+      </c>
+      <c r="G149">
+        <v>0</v>
+      </c>
+      <c r="H149">
+        <v>0</v>
+      </c>
+      <c r="I149">
+        <v>0</v>
+      </c>
+      <c r="J149">
+        <v>0</v>
+      </c>
+      <c r="K149">
+        <v>0</v>
+      </c>
+      <c r="L149">
+        <v>0</v>
       </c>
       <c r="M149">
         <v>0</v>
+      </c>
+      <c r="N149" t="s">
+        <v>430</v>
       </c>
     </row>
     <row r="150" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A150" t="s">
-        <v>375</v>
+        <v>374</v>
       </c>
       <c r="B150" t="s">
-        <v>407</v>
+        <v>405</v>
       </c>
       <c r="M150">
         <v>0</v>
@@ -7454,10 +7497,10 @@
     </row>
     <row r="151" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A151" t="s">
-        <v>375</v>
+        <v>374</v>
       </c>
       <c r="B151" t="s">
-        <v>423</v>
+        <v>406</v>
       </c>
       <c r="M151">
         <v>0</v>
@@ -7465,60 +7508,33 @@
     </row>
     <row r="152" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A152" t="s">
-        <v>375</v>
+        <v>374</v>
       </c>
       <c r="B152" t="s">
         <v>422</v>
       </c>
-      <c r="D152">
-        <v>-3</v>
-      </c>
-      <c r="E152">
-        <v>1</v>
-      </c>
-      <c r="F152">
-        <v>1</v>
-      </c>
-      <c r="G152">
-        <v>-1</v>
-      </c>
-      <c r="H152">
-        <v>0</v>
-      </c>
-      <c r="I152">
-        <v>0</v>
-      </c>
-      <c r="J152">
-        <v>0</v>
-      </c>
-      <c r="K152">
-        <v>0</v>
-      </c>
-      <c r="L152">
-        <v>0</v>
-      </c>
       <c r="M152">
         <v>0</v>
       </c>
     </row>
     <row r="153" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A153" t="s">
-        <v>375</v>
+        <v>374</v>
       </c>
       <c r="B153" t="s">
-        <v>408</v>
+        <v>421</v>
       </c>
       <c r="D153">
+        <v>-3</v>
+      </c>
+      <c r="E153">
+        <v>1</v>
+      </c>
+      <c r="F153">
+        <v>1</v>
+      </c>
+      <c r="G153">
         <v>-1</v>
-      </c>
-      <c r="E153">
-        <v>0</v>
-      </c>
-      <c r="F153">
-        <v>0</v>
-      </c>
-      <c r="G153">
-        <v>0</v>
       </c>
       <c r="H153">
         <v>0</v>
@@ -7541,13 +7557,13 @@
     </row>
     <row r="154" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A154" t="s">
-        <v>375</v>
+        <v>374</v>
       </c>
       <c r="B154" t="s">
-        <v>409</v>
+        <v>407</v>
       </c>
       <c r="D154">
-        <v>0</v>
+        <v>-1</v>
       </c>
       <c r="E154">
         <v>0</v>
@@ -7559,7 +7575,7 @@
         <v>0</v>
       </c>
       <c r="H154">
-        <v>-1</v>
+        <v>0</v>
       </c>
       <c r="I154">
         <v>0</v>
@@ -7579,26 +7595,26 @@
     </row>
     <row r="155" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A155" t="s">
-        <v>375</v>
+        <v>374</v>
       </c>
       <c r="B155" t="s">
-        <v>410</v>
+        <v>408</v>
       </c>
       <c r="D155">
         <v>0</v>
       </c>
       <c r="E155">
+        <v>0</v>
+      </c>
+      <c r="F155">
+        <v>0</v>
+      </c>
+      <c r="G155">
+        <v>0</v>
+      </c>
+      <c r="H155">
         <v>-1</v>
       </c>
-      <c r="F155">
-        <v>0</v>
-      </c>
-      <c r="G155">
-        <v>0</v>
-      </c>
-      <c r="H155">
-        <v>0</v>
-      </c>
       <c r="I155">
         <v>0</v>
       </c>
@@ -7612,6 +7628,44 @@
         <v>0</v>
       </c>
       <c r="M155">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="156" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A156" t="s">
+        <v>374</v>
+      </c>
+      <c r="B156" t="s">
+        <v>409</v>
+      </c>
+      <c r="D156">
+        <v>0</v>
+      </c>
+      <c r="E156">
+        <v>-1</v>
+      </c>
+      <c r="F156">
+        <v>0</v>
+      </c>
+      <c r="G156">
+        <v>0</v>
+      </c>
+      <c r="H156">
+        <v>0</v>
+      </c>
+      <c r="I156">
+        <v>0</v>
+      </c>
+      <c r="J156">
+        <v>0</v>
+      </c>
+      <c r="K156">
+        <v>0</v>
+      </c>
+      <c r="L156">
+        <v>0</v>
+      </c>
+      <c r="M156">
         <v>0</v>
       </c>
     </row>
@@ -7636,7 +7690,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EDB7BAAD-9B17-4BFB-BDE6-C10D563716CF}">
   <dimension ref="A1:D23"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A12" sqref="A12"/>
     </sheetView>
   </sheetViews>
@@ -7653,7 +7707,7 @@
         <v>1</v>
       </c>
       <c r="D1" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.3">
@@ -7661,10 +7715,10 @@
         <v>95</v>
       </c>
       <c r="B2" t="s">
+        <v>295</v>
+      </c>
+      <c r="C2" t="s">
         <v>296</v>
-      </c>
-      <c r="C2" t="s">
-        <v>297</v>
       </c>
       <c r="D2">
         <v>24</v>
@@ -7675,10 +7729,10 @@
         <v>95</v>
       </c>
       <c r="B3" t="s">
+        <v>297</v>
+      </c>
+      <c r="C3" t="s">
         <v>298</v>
-      </c>
-      <c r="C3" t="s">
-        <v>299</v>
       </c>
       <c r="D3">
         <v>21</v>
@@ -7689,10 +7743,10 @@
         <v>95</v>
       </c>
       <c r="B4" t="s">
+        <v>299</v>
+      </c>
+      <c r="C4" t="s">
         <v>300</v>
-      </c>
-      <c r="C4" t="s">
-        <v>301</v>
       </c>
       <c r="D4">
         <v>18</v>
@@ -7703,10 +7757,10 @@
         <v>95</v>
       </c>
       <c r="B5" t="s">
+        <v>301</v>
+      </c>
+      <c r="C5" t="s">
         <v>302</v>
-      </c>
-      <c r="C5" t="s">
-        <v>303</v>
       </c>
       <c r="D5">
         <v>15</v>
@@ -7720,7 +7774,7 @@
         <v>32</v>
       </c>
       <c r="C6" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
       <c r="D6">
         <v>12</v>
@@ -7731,10 +7785,10 @@
         <v>95</v>
       </c>
       <c r="B7" t="s">
+        <v>304</v>
+      </c>
+      <c r="C7" t="s">
         <v>305</v>
-      </c>
-      <c r="C7" t="s">
-        <v>306</v>
       </c>
       <c r="D7">
         <v>9</v>
@@ -7745,10 +7799,10 @@
         <v>95</v>
       </c>
       <c r="B8" t="s">
+        <v>306</v>
+      </c>
+      <c r="C8" t="s">
         <v>307</v>
-      </c>
-      <c r="C8" t="s">
-        <v>308</v>
       </c>
       <c r="D8">
         <v>6</v>
@@ -7759,10 +7813,10 @@
         <v>95</v>
       </c>
       <c r="B9" t="s">
+        <v>308</v>
+      </c>
+      <c r="C9" t="s">
         <v>309</v>
-      </c>
-      <c r="C9" t="s">
-        <v>310</v>
       </c>
       <c r="D9">
         <v>3</v>
@@ -7776,7 +7830,7 @@
         <v>65</v>
       </c>
       <c r="C10" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
       <c r="D10">
         <v>2</v>
@@ -7787,10 +7841,10 @@
         <v>95</v>
       </c>
       <c r="B11" t="s">
+        <v>311</v>
+      </c>
+      <c r="C11" t="s">
         <v>312</v>
-      </c>
-      <c r="C11" t="s">
-        <v>313</v>
       </c>
       <c r="D11">
         <v>1</v>
@@ -7809,10 +7863,10 @@
         <v>95</v>
       </c>
       <c r="B13" t="s">
+        <v>313</v>
+      </c>
+      <c r="C13" t="s">
         <v>314</v>
-      </c>
-      <c r="C13" t="s">
-        <v>315</v>
       </c>
       <c r="D13">
         <v>-1</v>
@@ -7823,10 +7877,10 @@
         <v>95</v>
       </c>
       <c r="B14" t="s">
+        <v>315</v>
+      </c>
+      <c r="C14" t="s">
         <v>316</v>
-      </c>
-      <c r="C14" t="s">
-        <v>317</v>
       </c>
       <c r="D14">
         <v>-2</v>
@@ -7840,7 +7894,7 @@
         <v>3</v>
       </c>
       <c r="C15" t="s">
-        <v>318</v>
+        <v>317</v>
       </c>
       <c r="D15">
         <v>-3</v>
@@ -7851,10 +7905,10 @@
         <v>95</v>
       </c>
       <c r="B16" t="s">
+        <v>318</v>
+      </c>
+      <c r="C16" t="s">
         <v>319</v>
-      </c>
-      <c r="C16" t="s">
-        <v>320</v>
       </c>
       <c r="D16">
         <v>-6</v>
@@ -7865,10 +7919,10 @@
         <v>95</v>
       </c>
       <c r="B17" t="s">
+        <v>320</v>
+      </c>
+      <c r="C17" t="s">
         <v>321</v>
-      </c>
-      <c r="C17" t="s">
-        <v>322</v>
       </c>
       <c r="D17">
         <v>-9</v>
@@ -7879,10 +7933,10 @@
         <v>95</v>
       </c>
       <c r="B18" t="s">
+        <v>322</v>
+      </c>
+      <c r="C18" t="s">
         <v>323</v>
-      </c>
-      <c r="C18" t="s">
-        <v>324</v>
       </c>
       <c r="D18">
         <v>-12</v>
@@ -7893,10 +7947,10 @@
         <v>95</v>
       </c>
       <c r="B19" t="s">
+        <v>324</v>
+      </c>
+      <c r="C19" t="s">
         <v>325</v>
-      </c>
-      <c r="C19" t="s">
-        <v>326</v>
       </c>
       <c r="D19">
         <v>-15</v>
@@ -7907,10 +7961,10 @@
         <v>95</v>
       </c>
       <c r="B20" t="s">
+        <v>326</v>
+      </c>
+      <c r="C20" t="s">
         <v>327</v>
-      </c>
-      <c r="C20" t="s">
-        <v>328</v>
       </c>
       <c r="D20">
         <v>-18</v>
@@ -7921,10 +7975,10 @@
         <v>95</v>
       </c>
       <c r="B21" t="s">
+        <v>328</v>
+      </c>
+      <c r="C21" t="s">
         <v>329</v>
-      </c>
-      <c r="C21" t="s">
-        <v>330</v>
       </c>
       <c r="D21">
         <v>-21</v>
@@ -7935,10 +7989,10 @@
         <v>95</v>
       </c>
       <c r="B22" t="s">
+        <v>330</v>
+      </c>
+      <c r="C22" t="s">
         <v>331</v>
-      </c>
-      <c r="C22" t="s">
-        <v>332</v>
       </c>
       <c r="D22">
         <v>-24</v>
@@ -7946,13 +8000,13 @@
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
+        <v>374</v>
+      </c>
+      <c r="B23" t="s">
         <v>375</v>
       </c>
-      <c r="B23" t="s">
+      <c r="C23" t="s">
         <v>376</v>
-      </c>
-      <c r="C23" t="s">
-        <v>377</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Not passing, checkpoint for new Quantity objects
</commit_message>
<xml_diff>
--- a/src/carpy/utility/data/quantities.xlsx
+++ b/src/carpy/utility/data/quantities.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25601"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27328"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://sotonac-my.sharepoint.com/personal/yr3g17_soton_ac_uk/Documents/Documents/Python/carpy/src/carpy/utility/data/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\yr3g17\PycharmProjects\carpy\src\carpy\utility\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="934" documentId="13_ncr:1_{848856CE-4ADE-4AE2-9F79-561287E38E1C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{6DD52F89-8BDB-4BCF-9746-9DC57D68CA16}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7F33FFD5-518D-4FE3-B688-95659F3C90BE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-107" yWindow="-107" windowWidth="20847" windowHeight="11208" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="dimensions" sheetId="1" r:id="rId1"/>
@@ -34,8 +34,42 @@
 </workbook>
 </file>
 
+<file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
+  <authors>
+    <author>Yaseen Reza</author>
+  </authors>
+  <commentList>
+    <comment ref="M4" authorId="0" shapeId="0" xr:uid="{F244A028-3DD0-4250-8F9E-A6C66ED0A1E6}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>Yaseen Reza:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+I realise this looks out of place compared to everything else, but it's a necessary exception for the code - a byproduct of the kilogram being the standard measurement of mass (and not the gram)</t>
+        </r>
+      </text>
+    </comment>
+  </commentList>
+</comments>
+</file>
+
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="637" uniqueCount="435">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="644" uniqueCount="441">
   <si>
     <t>Symbol</t>
   </si>
@@ -628,731 +662,762 @@
     <t>newtons to a pound-force</t>
   </si>
   <si>
-    <t>change in kelvin to degree Rankine</t>
-  </si>
-  <si>
     <t>change in degree Celsius to degree Farenheit</t>
   </si>
   <si>
+    <t>thermochemical british thermal unit</t>
+  </si>
+  <si>
+    <t>thermochemical (small) calorie</t>
+  </si>
+  <si>
+    <t>thermochemical (large) calorie</t>
+  </si>
+  <si>
+    <t>joules to the ISO thermochemical large calorie</t>
+  </si>
+  <si>
+    <t>pound (mass)</t>
+  </si>
+  <si>
+    <t>Exact definition, 1 kcal_th/(lb degF)</t>
+  </si>
+  <si>
+    <t>international steam table (small) calorie</t>
+  </si>
+  <si>
+    <t>international steam table (large) calorie</t>
+  </si>
+  <si>
+    <t>joules to the international steam table large calorie</t>
+  </si>
+  <si>
+    <t>international steam table british thermal unit</t>
+  </si>
+  <si>
+    <t>Exact definition, 1 kcal_it/(lb degF)</t>
+  </si>
+  <si>
+    <t>therm</t>
+  </si>
+  <si>
+    <t>quad</t>
+  </si>
+  <si>
+    <t>100,000 british thermal units</t>
+  </si>
+  <si>
+    <t>10^15 british thermal units</t>
+  </si>
+  <si>
+    <t>joules to an international steam table british thermal unit</t>
+  </si>
+  <si>
+    <t>psi</t>
+  </si>
+  <si>
+    <t>pound-force per square inch</t>
+  </si>
+  <si>
+    <t>pascal to a pound per square inch</t>
+  </si>
+  <si>
+    <t>metric</t>
+  </si>
+  <si>
+    <t>bar</t>
+  </si>
+  <si>
+    <t>mbar</t>
+  </si>
+  <si>
+    <t>dbar</t>
+  </si>
+  <si>
+    <t>millibar</t>
+  </si>
+  <si>
+    <t>decibar</t>
+  </si>
+  <si>
+    <t>pascal to a bar</t>
+  </si>
+  <si>
+    <t>pascal to a decibar</t>
+  </si>
+  <si>
+    <t>pascal to a millibar</t>
+  </si>
+  <si>
+    <t>miscellaneous</t>
+  </si>
+  <si>
+    <t>atm</t>
+  </si>
+  <si>
+    <t>atmospheric pressure</t>
+  </si>
+  <si>
+    <t>mmHg</t>
+  </si>
+  <si>
+    <t>millimetres of mercury</t>
+  </si>
+  <si>
+    <t>Exact definition, pascal</t>
+  </si>
+  <si>
+    <t>Exact definition, joules</t>
+  </si>
+  <si>
+    <t>torr</t>
+  </si>
+  <si>
+    <t>Torr</t>
+  </si>
+  <si>
+    <t>mTorr</t>
+  </si>
+  <si>
+    <t>millitorr</t>
+  </si>
+  <si>
+    <t>pascal to a millitorr</t>
+  </si>
+  <si>
+    <t>inHg</t>
+  </si>
+  <si>
+    <t>inches of mercury</t>
+  </si>
+  <si>
+    <t>pascal to a inch of mercury</t>
+  </si>
+  <si>
+    <t>ly</t>
+  </si>
+  <si>
+    <t>pc</t>
+  </si>
+  <si>
+    <t>parsec</t>
+  </si>
+  <si>
+    <t>metres to a parsec</t>
+  </si>
+  <si>
+    <t>Exact definition, joules to the ISO thermochemical small calorie</t>
+  </si>
+  <si>
+    <t>Exact definition, metres cubed to an imperial gallon</t>
+  </si>
+  <si>
+    <t>Exact definition, metres cubed to a U.S. gallon</t>
+  </si>
+  <si>
+    <t>Exact definition, joules to the international steam table small calorie (1956)</t>
+  </si>
+  <si>
+    <t>long hundredweight</t>
+  </si>
+  <si>
+    <t>kilograms to a long hundredweight</t>
+  </si>
+  <si>
+    <t>kilograms to a long ton (UK)</t>
+  </si>
+  <si>
+    <t>long ton</t>
+  </si>
+  <si>
+    <t>short ton</t>
+  </si>
+  <si>
+    <t>Exact definition, kilograms to a pound</t>
+  </si>
+  <si>
+    <t>US hundredweight</t>
+  </si>
+  <si>
+    <t>kilograms to a US hundredweight</t>
+  </si>
+  <si>
+    <t>kilograms to a short ton (US)</t>
+  </si>
+  <si>
+    <t>U.S. gallon</t>
+  </si>
+  <si>
+    <t>U.S. pottle</t>
+  </si>
+  <si>
+    <t>U.S. quart</t>
+  </si>
+  <si>
+    <t>U.S. fluid ounce</t>
+  </si>
+  <si>
+    <t>U.S. gill</t>
+  </si>
+  <si>
+    <t>U.S. pint</t>
+  </si>
+  <si>
+    <t>metres cubed to a U.S. pottle</t>
+  </si>
+  <si>
+    <t>metres cubed to a U.S. fluid ounce</t>
+  </si>
+  <si>
+    <t>metres cubed to a U.S. gill</t>
+  </si>
+  <si>
+    <t>metres cubed to a U.S. pint</t>
+  </si>
+  <si>
+    <t>metres cubed to a U.S. quart</t>
+  </si>
+  <si>
+    <t>tbsp</t>
+  </si>
+  <si>
+    <t>tsp</t>
+  </si>
+  <si>
+    <t>teaspoon</t>
+  </si>
+  <si>
+    <t>tablespoon</t>
+  </si>
+  <si>
+    <t>cup</t>
+  </si>
+  <si>
+    <t>metres cubed to a cup</t>
+  </si>
+  <si>
+    <t>metres cubed to a teaspoon</t>
+  </si>
+  <si>
+    <t>metres cubed to a tablespoon</t>
+  </si>
+  <si>
+    <t>pk</t>
+  </si>
+  <si>
+    <t>U.S. dry pint</t>
+  </si>
+  <si>
+    <t>U.S. dry quart</t>
+  </si>
+  <si>
+    <t>U.S. dry gallon</t>
+  </si>
+  <si>
+    <t>peck</t>
+  </si>
+  <si>
+    <t>bushel</t>
+  </si>
+  <si>
+    <t>metres cubed to a U.S. dry quart</t>
+  </si>
+  <si>
+    <t>Exact definition, 33.6003125 cubic inches to a U.S. dry pint</t>
+  </si>
+  <si>
+    <t>metres cubed to a U.S. dry gallon</t>
+  </si>
+  <si>
+    <t>metres cubed to a dry bushel</t>
+  </si>
+  <si>
+    <t>metres cubed to a dry peck</t>
+  </si>
+  <si>
+    <t>light year</t>
+  </si>
+  <si>
+    <t>metres to a light year</t>
+  </si>
+  <si>
+    <t>kgf,kgF,kp</t>
+  </si>
+  <si>
+    <t>kilogram-force (kilopond)</t>
+  </si>
+  <si>
+    <t>Exponent</t>
+  </si>
+  <si>
+    <t>Y</t>
+  </si>
+  <si>
+    <t>yotta</t>
+  </si>
+  <si>
+    <t>Z</t>
+  </si>
+  <si>
+    <t>zetta</t>
+  </si>
+  <si>
+    <t>E</t>
+  </si>
+  <si>
+    <t>exa</t>
+  </si>
+  <si>
+    <t>P</t>
+  </si>
+  <si>
+    <t>peta</t>
+  </si>
+  <si>
+    <t>tera</t>
+  </si>
+  <si>
+    <t>G</t>
+  </si>
+  <si>
+    <t>giga</t>
+  </si>
+  <si>
+    <t>M</t>
+  </si>
+  <si>
+    <t>mega</t>
+  </si>
+  <si>
+    <t>k</t>
+  </si>
+  <si>
+    <t>kilo</t>
+  </si>
+  <si>
+    <t>hecto</t>
+  </si>
+  <si>
+    <t>da</t>
+  </si>
+  <si>
+    <t>deca</t>
+  </si>
+  <si>
+    <t>d</t>
+  </si>
+  <si>
+    <t>deci</t>
+  </si>
+  <si>
+    <t>c</t>
+  </si>
+  <si>
+    <t>centi</t>
+  </si>
+  <si>
+    <t>milli</t>
+  </si>
+  <si>
+    <t>u</t>
+  </si>
+  <si>
+    <t>micro</t>
+  </si>
+  <si>
+    <t>n</t>
+  </si>
+  <si>
+    <t>nano</t>
+  </si>
+  <si>
+    <t>p</t>
+  </si>
+  <si>
+    <t>pico</t>
+  </si>
+  <si>
+    <t>f</t>
+  </si>
+  <si>
+    <t>femto</t>
+  </si>
+  <si>
+    <t>a</t>
+  </si>
+  <si>
+    <t>atto</t>
+  </si>
+  <si>
+    <t>z</t>
+  </si>
+  <si>
+    <t>zepto</t>
+  </si>
+  <si>
+    <t>y</t>
+  </si>
+  <si>
+    <t>yocto</t>
+  </si>
+  <si>
+    <t>gi</t>
+  </si>
+  <si>
+    <t>pt</t>
+  </si>
+  <si>
+    <t>qt</t>
+  </si>
+  <si>
+    <t>gal</t>
+  </si>
+  <si>
+    <t>pot</t>
+  </si>
+  <si>
+    <t>cal</t>
+  </si>
+  <si>
+    <t>kcal</t>
+  </si>
+  <si>
+    <t>Btu,BTU</t>
+  </si>
+  <si>
+    <t>arcmin</t>
+  </si>
+  <si>
+    <t>arcsec</t>
+  </si>
+  <si>
+    <t>in</t>
+  </si>
+  <si>
+    <t>ft</t>
+  </si>
+  <si>
+    <t>ton(short)</t>
+  </si>
+  <si>
+    <t>cwt(short)</t>
+  </si>
+  <si>
+    <t>ton(long)</t>
+  </si>
+  <si>
+    <t>cwt(long)</t>
+  </si>
+  <si>
+    <t>Symbol(s)</t>
+  </si>
+  <si>
+    <t>hh</t>
+  </si>
+  <si>
+    <t>pt(dry)</t>
+  </si>
+  <si>
+    <t>qt(dry)</t>
+  </si>
+  <si>
+    <t>gal(dry)</t>
+  </si>
+  <si>
+    <t>pk(dry)</t>
+  </si>
+  <si>
+    <t>U.S. dry peck</t>
+  </si>
+  <si>
+    <t>fl.dr</t>
+  </si>
+  <si>
+    <t>U.S. fluid dram</t>
+  </si>
+  <si>
+    <t>metres cubed to a U.S. fluid dram</t>
+  </si>
+  <si>
+    <t>bsh,bu</t>
+  </si>
+  <si>
+    <t>metres cubed to a peck</t>
+  </si>
+  <si>
+    <t>metres cubed to a bushel</t>
+  </si>
+  <si>
+    <t>nmi,M,NM</t>
+  </si>
+  <si>
+    <t>dyn</t>
+  </si>
+  <si>
+    <t>dyne</t>
+  </si>
+  <si>
+    <t>newtons to a dyne</t>
+  </si>
+  <si>
+    <t>cal(IT)</t>
+  </si>
+  <si>
+    <t>kcal(IT)</t>
+  </si>
+  <si>
+    <t>Btu(IT),BTU(IT)</t>
+  </si>
+  <si>
+    <t>rps,RPS</t>
+  </si>
+  <si>
+    <t>rpm,RPM</t>
+  </si>
+  <si>
+    <t>revolutions per minute</t>
+  </si>
+  <si>
+    <t>revolutions per second</t>
+  </si>
+  <si>
+    <t>radians per second to revolutions per second</t>
+  </si>
+  <si>
+    <t>radians per second to revolutions per minute</t>
+  </si>
+  <si>
+    <t>Bel</t>
+  </si>
+  <si>
+    <t>dB</t>
+  </si>
+  <si>
+    <t>decibel</t>
+  </si>
+  <si>
+    <t>A,(A)</t>
+  </si>
+  <si>
+    <t>B,(B)</t>
+  </si>
+  <si>
+    <t>C,(C)</t>
+  </si>
+  <si>
+    <t>D,DB(D)</t>
+  </si>
+  <si>
+    <t>d,(dipole)</t>
+  </si>
+  <si>
+    <t>e</t>
+  </si>
+  <si>
+    <t>f,(fW)</t>
+  </si>
+  <si>
+    <t>FS</t>
+  </si>
+  <si>
+    <t>i,(isotropic)</t>
+  </si>
+  <si>
+    <t>iC</t>
+  </si>
+  <si>
+    <t>k,(kW)</t>
+  </si>
+  <si>
+    <t>K,(K)</t>
+  </si>
+  <si>
+    <t>m,(mW)</t>
+  </si>
+  <si>
+    <t>m0s</t>
+  </si>
+  <si>
+    <t>mV,(mV_{RMS})</t>
+  </si>
+  <si>
+    <t>o</t>
+  </si>
+  <si>
+    <t>O,ov,(overload)</t>
+  </si>
+  <si>
+    <t>q</t>
+  </si>
+  <si>
+    <t>r</t>
+  </si>
+  <si>
+    <t>rn,rnC</t>
+  </si>
+  <si>
+    <t>sm</t>
+  </si>
+  <si>
+    <t>TP</t>
+  </si>
+  <si>
+    <t>u,v</t>
+  </si>
+  <si>
+    <t>u0s</t>
+  </si>
+  <si>
+    <t>uV</t>
+  </si>
+  <si>
+    <t>uV/m</t>
+  </si>
+  <si>
+    <t>V,(V_{RMS})</t>
+  </si>
+  <si>
+    <t>VU</t>
+  </si>
+  <si>
+    <t>Wm^{-2}Hz^{-1}</t>
+  </si>
+  <si>
+    <t>Z,(Z)</t>
+  </si>
+  <si>
+    <t>-Hz,(Hz)</t>
+  </si>
+  <si>
+    <t>/K,(K^{-1})</t>
+  </si>
+  <si>
+    <t>m^{-1},(m^{-1})</t>
+  </si>
+  <si>
+    <t>relative to carrier</t>
+  </si>
+  <si>
+    <t>electrical</t>
+  </si>
+  <si>
+    <t>full scale</t>
+  </si>
+  <si>
+    <t>G-weighted spectrum</t>
+  </si>
+  <si>
+    <t>isotropic antenna gain</t>
+  </si>
+  <si>
+    <t>dipole antenna gain</t>
+  </si>
+  <si>
+    <t>isotropic circularly polarized antenna gain</t>
+  </si>
+  <si>
+    <t>relative to 1 joule</t>
+  </si>
+  <si>
+    <t>relative to kelvin</t>
+  </si>
+  <si>
+    <t>relative to 1 mV across 75 ohm</t>
+  </si>
+  <si>
+    <t>uV/m,(muV/m),mu</t>
+  </si>
+  <si>
+    <t>uV,(muV_{RMS})</t>
+  </si>
+  <si>
+    <t>RMS voltage relative to sqrt(0.6) V</t>
+  </si>
+  <si>
+    <t>voltage relative to 1 volt, regardless of impedance</t>
+  </si>
+  <si>
+    <t>m0</t>
+  </si>
+  <si>
+    <t>voltage relative to 1 microvolt</t>
+  </si>
+  <si>
+    <t>dB shift of 1 watt to 1 kilowatt</t>
+  </si>
+  <si>
+    <t>dB shift of 1 watt to 1 femtowatt</t>
+  </si>
+  <si>
+    <t>dB shift of 1 watt to 1 milliwatt</t>
+  </si>
+  <si>
+    <t>dB shift of 1 watt to 1 watt</t>
+  </si>
+  <si>
+    <t>ml,mL</t>
+  </si>
+  <si>
+    <t>millilitre</t>
+  </si>
+  <si>
+    <t>metres cubed to a millilitre</t>
+  </si>
+  <si>
+    <t>USC</t>
+  </si>
+  <si>
     <t>kilograms to a gram</t>
   </si>
   <si>
-    <t>thermochemical british thermal unit</t>
-  </si>
-  <si>
-    <t>thermochemical (small) calorie</t>
-  </si>
-  <si>
-    <t>thermochemical (large) calorie</t>
-  </si>
-  <si>
-    <t>joules to the ISO thermochemical large calorie</t>
-  </si>
-  <si>
-    <t>pound (mass)</t>
-  </si>
-  <si>
-    <t>Exact definition, 1 kcal_th/(lb degF)</t>
-  </si>
-  <si>
-    <t>international steam table (small) calorie</t>
-  </si>
-  <si>
-    <t>international steam table (large) calorie</t>
-  </si>
-  <si>
-    <t>joules to the international steam table large calorie</t>
-  </si>
-  <si>
-    <t>international steam table british thermal unit</t>
-  </si>
-  <si>
-    <t>Exact definition, 1 kcal_it/(lb degF)</t>
-  </si>
-  <si>
-    <t>therm</t>
-  </si>
-  <si>
-    <t>quad</t>
-  </si>
-  <si>
-    <t>100,000 british thermal units</t>
-  </si>
-  <si>
-    <t>10^15 british thermal units</t>
-  </si>
-  <si>
-    <t>joules to an international steam table british thermal unit</t>
-  </si>
-  <si>
-    <t>psi</t>
-  </si>
-  <si>
-    <t>pound-force per square inch</t>
-  </si>
-  <si>
-    <t>pascal to a pound per square inch</t>
-  </si>
-  <si>
-    <t>metric</t>
-  </si>
-  <si>
-    <t>bar</t>
-  </si>
-  <si>
-    <t>mbar</t>
-  </si>
-  <si>
-    <t>dbar</t>
-  </si>
-  <si>
-    <t>millibar</t>
-  </si>
-  <si>
-    <t>decibar</t>
-  </si>
-  <si>
-    <t>pascal to a bar</t>
-  </si>
-  <si>
-    <t>pascal to a decibar</t>
-  </si>
-  <si>
-    <t>pascal to a millibar</t>
-  </si>
-  <si>
-    <t>miscellaneous</t>
-  </si>
-  <si>
-    <t>atm</t>
-  </si>
-  <si>
-    <t>atmospheric pressure</t>
-  </si>
-  <si>
-    <t>mmHg</t>
-  </si>
-  <si>
-    <t>millimetres of mercury</t>
-  </si>
-  <si>
-    <t>Exact definition, pascal</t>
-  </si>
-  <si>
-    <t>Exact definition, joules</t>
-  </si>
-  <si>
-    <t>torr</t>
-  </si>
-  <si>
-    <t>Torr</t>
-  </si>
-  <si>
-    <t>mTorr</t>
-  </si>
-  <si>
-    <t>millitorr</t>
-  </si>
-  <si>
-    <t>pascal to a millitorr</t>
-  </si>
-  <si>
-    <t>inHg</t>
-  </si>
-  <si>
-    <t>inches of mercury</t>
-  </si>
-  <si>
-    <t>pascal to a inch of mercury</t>
-  </si>
-  <si>
-    <t>ly</t>
-  </si>
-  <si>
-    <t>pc</t>
-  </si>
-  <si>
-    <t>parsec</t>
-  </si>
-  <si>
-    <t>metres to a parsec</t>
-  </si>
-  <si>
-    <t>Exact definition, joules to the ISO thermochemical small calorie</t>
-  </si>
-  <si>
-    <t>Exact definition, metres cubed to an imperial gallon</t>
-  </si>
-  <si>
-    <t>Exact definition, metres cubed to a U.S. gallon</t>
-  </si>
-  <si>
-    <t>Exact definition, joules to the international steam table small calorie (1956)</t>
-  </si>
-  <si>
-    <t>long hundredweight</t>
-  </si>
-  <si>
-    <t>kilograms to a long hundredweight</t>
-  </si>
-  <si>
-    <t>kilograms to a long ton (UK)</t>
-  </si>
-  <si>
-    <t>long ton</t>
-  </si>
-  <si>
-    <t>short ton</t>
-  </si>
-  <si>
-    <t>Exact definition, kilograms to a pound</t>
-  </si>
-  <si>
-    <t>US hundredweight</t>
-  </si>
-  <si>
-    <t>kilograms to a US hundredweight</t>
-  </si>
-  <si>
-    <t>kilograms to a short ton (US)</t>
-  </si>
-  <si>
-    <t>U.S. gallon</t>
-  </si>
-  <si>
-    <t>U.S. pottle</t>
-  </si>
-  <si>
-    <t>U.S. quart</t>
-  </si>
-  <si>
-    <t>U.S. fluid ounce</t>
-  </si>
-  <si>
-    <t>U.S. gill</t>
-  </si>
-  <si>
-    <t>U.S. pint</t>
-  </si>
-  <si>
-    <t>metres cubed to a U.S. pottle</t>
-  </si>
-  <si>
-    <t>metres cubed to a U.S. fluid ounce</t>
-  </si>
-  <si>
-    <t>metres cubed to a U.S. gill</t>
-  </si>
-  <si>
-    <t>metres cubed to a U.S. pint</t>
-  </si>
-  <si>
-    <t>metres cubed to a U.S. quart</t>
-  </si>
-  <si>
-    <t>tbsp</t>
-  </si>
-  <si>
-    <t>tsp</t>
-  </si>
-  <si>
-    <t>teaspoon</t>
-  </si>
-  <si>
-    <t>tablespoon</t>
-  </si>
-  <si>
-    <t>cup</t>
-  </si>
-  <si>
-    <t>metres cubed to a cup</t>
-  </si>
-  <si>
-    <t>metres cubed to a teaspoon</t>
-  </si>
-  <si>
-    <t>metres cubed to a tablespoon</t>
-  </si>
-  <si>
-    <t>pk</t>
-  </si>
-  <si>
-    <t>U.S. dry pint</t>
-  </si>
-  <si>
-    <t>U.S. dry quart</t>
-  </si>
-  <si>
-    <t>U.S. dry gallon</t>
-  </si>
-  <si>
-    <t>peck</t>
-  </si>
-  <si>
-    <t>bushel</t>
-  </si>
-  <si>
-    <t>metres cubed to a U.S. dry quart</t>
-  </si>
-  <si>
-    <t>Exact definition, 33.6003125 cubic inches to a U.S. dry pint</t>
-  </si>
-  <si>
-    <t>metres cubed to a U.S. dry gallon</t>
-  </si>
-  <si>
-    <t>metres cubed to a dry bushel</t>
-  </si>
-  <si>
-    <t>metres cubed to a dry peck</t>
-  </si>
-  <si>
-    <t>light year</t>
-  </si>
-  <si>
-    <t>metres to a light year</t>
-  </si>
-  <si>
-    <t>kgf,kgF,kp</t>
-  </si>
-  <si>
-    <t>kilogram-force (kilopond)</t>
-  </si>
-  <si>
-    <t>Exponent</t>
-  </si>
-  <si>
-    <t>Y</t>
-  </si>
-  <si>
-    <t>yotta</t>
-  </si>
-  <si>
-    <t>Z</t>
-  </si>
-  <si>
-    <t>zetta</t>
-  </si>
-  <si>
-    <t>E</t>
-  </si>
-  <si>
-    <t>exa</t>
-  </si>
-  <si>
-    <t>P</t>
-  </si>
-  <si>
-    <t>peta</t>
-  </si>
-  <si>
-    <t>tera</t>
-  </si>
-  <si>
-    <t>G</t>
-  </si>
-  <si>
-    <t>giga</t>
-  </si>
-  <si>
-    <t>M</t>
-  </si>
-  <si>
-    <t>mega</t>
-  </si>
-  <si>
-    <t>k</t>
-  </si>
-  <si>
-    <t>kilo</t>
-  </si>
-  <si>
-    <t>hecto</t>
-  </si>
-  <si>
-    <t>da</t>
-  </si>
-  <si>
-    <t>deca</t>
-  </si>
-  <si>
-    <t>d</t>
-  </si>
-  <si>
-    <t>deci</t>
-  </si>
-  <si>
-    <t>c</t>
-  </si>
-  <si>
-    <t>centi</t>
-  </si>
-  <si>
-    <t>milli</t>
-  </si>
-  <si>
-    <t>u</t>
-  </si>
-  <si>
-    <t>micro</t>
-  </si>
-  <si>
-    <t>n</t>
-  </si>
-  <si>
-    <t>nano</t>
-  </si>
-  <si>
-    <t>p</t>
-  </si>
-  <si>
-    <t>pico</t>
-  </si>
-  <si>
-    <t>f</t>
-  </si>
-  <si>
-    <t>femto</t>
-  </si>
-  <si>
-    <t>a</t>
-  </si>
-  <si>
-    <t>atto</t>
-  </si>
-  <si>
-    <t>z</t>
-  </si>
-  <si>
-    <t>zepto</t>
-  </si>
-  <si>
-    <t>y</t>
-  </si>
-  <si>
-    <t>yocto</t>
-  </si>
-  <si>
-    <t>gi</t>
-  </si>
-  <si>
-    <t>pt</t>
-  </si>
-  <si>
-    <t>qt</t>
-  </si>
-  <si>
-    <t>gal</t>
-  </si>
-  <si>
-    <t>pot</t>
-  </si>
-  <si>
-    <t>cal</t>
-  </si>
-  <si>
-    <t>kcal</t>
-  </si>
-  <si>
-    <t>Btu,BTU</t>
-  </si>
-  <si>
-    <t>arcmin</t>
-  </si>
-  <si>
-    <t>arcsec</t>
-  </si>
-  <si>
-    <t>in</t>
-  </si>
-  <si>
-    <t>ft</t>
-  </si>
-  <si>
-    <t>ton(short)</t>
-  </si>
-  <si>
-    <t>cwt(short)</t>
-  </si>
-  <si>
-    <t>ton(long)</t>
-  </si>
-  <si>
-    <t>cwt(long)</t>
-  </si>
-  <si>
-    <t>Symbol(s)</t>
-  </si>
-  <si>
-    <t>hh</t>
-  </si>
-  <si>
-    <t>pt(dry)</t>
-  </si>
-  <si>
-    <t>qt(dry)</t>
-  </si>
-  <si>
-    <t>gal(dry)</t>
-  </si>
-  <si>
-    <t>pk(dry)</t>
-  </si>
-  <si>
-    <t>U.S. dry peck</t>
-  </si>
-  <si>
-    <t>fl.dr</t>
-  </si>
-  <si>
-    <t>U.S. fluid dram</t>
-  </si>
-  <si>
-    <t>metres cubed to a U.S. fluid dram</t>
-  </si>
-  <si>
-    <t>bsh,bu</t>
-  </si>
-  <si>
-    <t>metres cubed to a peck</t>
-  </si>
-  <si>
-    <t>metres cubed to a bushel</t>
-  </si>
-  <si>
-    <t>nmi,M,NM</t>
-  </si>
-  <si>
-    <t>dyn</t>
-  </si>
-  <si>
-    <t>dyne</t>
-  </si>
-  <si>
-    <t>newtons to a dyne</t>
-  </si>
-  <si>
-    <t>cal(IT)</t>
-  </si>
-  <si>
-    <t>kcal(IT)</t>
-  </si>
-  <si>
-    <t>Btu(IT),BTU(IT)</t>
-  </si>
-  <si>
-    <t>rps,RPS</t>
-  </si>
-  <si>
-    <t>rpm,RPM</t>
-  </si>
-  <si>
-    <t>revolutions per minute</t>
-  </si>
-  <si>
-    <t>revolutions per second</t>
-  </si>
-  <si>
-    <t>radians per second to revolutions per second</t>
-  </si>
-  <si>
-    <t>radians per second to revolutions per minute</t>
-  </si>
-  <si>
-    <t>Bel</t>
-  </si>
-  <si>
-    <t>dB</t>
-  </si>
-  <si>
-    <t>decibel</t>
-  </si>
-  <si>
-    <t>A,(A)</t>
-  </si>
-  <si>
-    <t>B,(B)</t>
-  </si>
-  <si>
-    <t>C,(C)</t>
-  </si>
-  <si>
-    <t>D,DB(D)</t>
-  </si>
-  <si>
-    <t>d,(dipole)</t>
-  </si>
-  <si>
-    <t>e</t>
-  </si>
-  <si>
-    <t>f,(fW)</t>
-  </si>
-  <si>
-    <t>FS</t>
-  </si>
-  <si>
-    <t>i,(isotropic)</t>
-  </si>
-  <si>
-    <t>iC</t>
-  </si>
-  <si>
-    <t>k,(kW)</t>
-  </si>
-  <si>
-    <t>K,(K)</t>
-  </si>
-  <si>
-    <t>m,(mW)</t>
-  </si>
-  <si>
-    <t>m0s</t>
-  </si>
-  <si>
-    <t>mV,(mV_{RMS})</t>
-  </si>
-  <si>
-    <t>o</t>
-  </si>
-  <si>
-    <t>O,ov,(overload)</t>
-  </si>
-  <si>
-    <t>q</t>
-  </si>
-  <si>
-    <t>r</t>
-  </si>
-  <si>
-    <t>rn,rnC</t>
-  </si>
-  <si>
-    <t>sm</t>
-  </si>
-  <si>
-    <t>TP</t>
-  </si>
-  <si>
-    <t>u,v</t>
-  </si>
-  <si>
-    <t>u0s</t>
-  </si>
-  <si>
-    <t>uV</t>
-  </si>
-  <si>
-    <t>uV/m</t>
-  </si>
-  <si>
-    <t>V,(V_{RMS})</t>
-  </si>
-  <si>
-    <t>VU</t>
-  </si>
-  <si>
-    <t>Wm^{-2}Hz^{-1}</t>
-  </si>
-  <si>
-    <t>Z,(Z)</t>
-  </si>
-  <si>
-    <t>-Hz,(Hz)</t>
-  </si>
-  <si>
-    <t>/K,(K^{-1})</t>
-  </si>
-  <si>
-    <t>m^{-1},(m^{-1})</t>
-  </si>
-  <si>
-    <t>relative to carrier</t>
-  </si>
-  <si>
-    <t>electrical</t>
-  </si>
-  <si>
-    <t>full scale</t>
-  </si>
-  <si>
-    <t>G-weighted spectrum</t>
-  </si>
-  <si>
-    <t>isotropic antenna gain</t>
-  </si>
-  <si>
-    <t>dipole antenna gain</t>
-  </si>
-  <si>
-    <t>isotropic circularly polarized antenna gain</t>
-  </si>
-  <si>
-    <t>relative to 1 joule</t>
-  </si>
-  <si>
-    <t>relative to kelvin</t>
-  </si>
-  <si>
-    <t>relative to 1 mV across 75 ohm</t>
-  </si>
-  <si>
-    <t>transform</t>
-  </si>
-  <si>
-    <t>uV/m,(muV/m),mu</t>
-  </si>
-  <si>
-    <t>uV,(muV_{RMS})</t>
-  </si>
-  <si>
-    <t>RMS voltage relative to sqrt(0.6) V</t>
-  </si>
-  <si>
-    <t>voltage relative to 1 volt, regardless of impedance</t>
-  </si>
-  <si>
-    <t>m0</t>
-  </si>
-  <si>
-    <t>voltage relative to 1 microvolt</t>
-  </si>
-  <si>
-    <t>dB shift of 1 watt to 1 kilowatt</t>
-  </si>
-  <si>
-    <t>dB shift of 1 watt to 1 femtowatt</t>
-  </si>
-  <si>
-    <t>dB shift of 1 watt to 1 milliwatt</t>
-  </si>
-  <si>
-    <t>dB shift of 1 watt to 1 watt</t>
-  </si>
-  <si>
-    <t>ml,mL</t>
-  </si>
-  <si>
-    <t>millilitre</t>
-  </si>
-  <si>
-    <t>metres cubed to a millilitre</t>
-  </si>
-  <si>
-    <t>USC</t>
+    <t>Kelvin to a Rankine</t>
+  </si>
+  <si>
+    <t>factor</t>
+  </si>
+  <si>
+    <t>miles per hour</t>
+  </si>
+  <si>
+    <t>metres per second to a mph</t>
+  </si>
+  <si>
+    <t>mph,m.p.h,MPH,mi/h</t>
+  </si>
+  <si>
+    <t>kph,km/h,km/hr</t>
+  </si>
+  <si>
+    <t>kilometres per hour</t>
+  </si>
+  <si>
+    <t>meters per second to a kph</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="9"/>
+      <color indexed="81"/>
+      <name val="Tahoma"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="9"/>
+      <color indexed="81"/>
+      <name val="Tahoma"/>
+      <charset val="1"/>
     </font>
   </fonts>
   <fills count="2">
@@ -1658,27 +1723,29 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:N156"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:N158"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A101" sqref="A101"/>
+      <pane ySplit="1" topLeftCell="A146" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="M162" sqref="M162"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="2" max="2" width="11.59765625" customWidth="1"/>
-    <col min="3" max="3" width="13.69921875" customWidth="1"/>
-    <col min="4" max="5" width="2.5" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="2.69921875" bestFit="1" customWidth="1"/>
-    <col min="7" max="8" width="2.5" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="4.09765625" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="2.796875" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="3.69921875" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="2.3984375" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="11.8984375" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="65.5" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="12.44140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="18.44140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="38" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="2.6640625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="2.44140625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="2.6640625" bestFit="1" customWidth="1"/>
+    <col min="7" max="8" width="2.44140625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="4.109375" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="2.77734375" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="3.6640625" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="2.44140625" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="11.88671875" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="65.44140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:14" x14ac:dyDescent="0.3">
@@ -1686,7 +1753,7 @@
         <v>76</v>
       </c>
       <c r="B1" t="s">
-        <v>348</v>
+        <v>346</v>
       </c>
       <c r="C1" t="s">
         <v>1</v>
@@ -1719,7 +1786,7 @@
         <v>18</v>
       </c>
       <c r="M1" t="s">
-        <v>420</v>
+        <v>434</v>
       </c>
       <c r="N1" t="s">
         <v>130</v>
@@ -1854,7 +1921,7 @@
         <v>1E-3</v>
       </c>
       <c r="N4" t="s">
-        <v>199</v>
+        <v>432</v>
       </c>
     </row>
     <row r="5" spans="1:14" x14ac:dyDescent="0.3">
@@ -3003,7 +3070,7 @@
     </row>
     <row r="31" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A31" t="s">
-        <v>219</v>
+        <v>217</v>
       </c>
       <c r="B31" t="s">
         <v>96</v>
@@ -3048,7 +3115,7 @@
     </row>
     <row r="32" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A32" t="s">
-        <v>219</v>
+        <v>217</v>
       </c>
       <c r="B32" t="s">
         <v>126</v>
@@ -3093,7 +3160,7 @@
     </row>
     <row r="33" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A33" t="s">
-        <v>219</v>
+        <v>217</v>
       </c>
       <c r="B33" t="s">
         <v>127</v>
@@ -3138,7 +3205,7 @@
     </row>
     <row r="34" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A34" t="s">
-        <v>219</v>
+        <v>217</v>
       </c>
       <c r="B34" t="s">
         <v>119</v>
@@ -3182,13 +3249,13 @@
     </row>
     <row r="35" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A35" t="s">
-        <v>219</v>
+        <v>217</v>
       </c>
       <c r="B35" t="s">
-        <v>243</v>
+        <v>241</v>
       </c>
       <c r="C35" t="s">
-        <v>290</v>
+        <v>288</v>
       </c>
       <c r="D35">
         <v>0</v>
@@ -3222,18 +3289,18 @@
         <v>9460750000000000</v>
       </c>
       <c r="N35" t="s">
-        <v>291</v>
+        <v>289</v>
       </c>
     </row>
     <row r="36" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A36" t="s">
-        <v>219</v>
+        <v>217</v>
       </c>
       <c r="B36" t="s">
-        <v>244</v>
+        <v>242</v>
       </c>
       <c r="C36" t="s">
-        <v>245</v>
+        <v>243</v>
       </c>
       <c r="D36">
         <v>0</v>
@@ -3267,12 +3334,12 @@
         <v>3.0856775814671916E+16</v>
       </c>
       <c r="N36" t="s">
-        <v>246</v>
+        <v>244</v>
       </c>
     </row>
     <row r="37" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A37" t="s">
-        <v>219</v>
+        <v>217</v>
       </c>
       <c r="B37" t="s">
         <v>97</v>
@@ -3317,10 +3384,10 @@
     </row>
     <row r="38" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A38" t="s">
-        <v>219</v>
+        <v>217</v>
       </c>
       <c r="B38" s="1" t="s">
-        <v>340</v>
+        <v>338</v>
       </c>
       <c r="C38" t="s">
         <v>107</v>
@@ -3362,10 +3429,10 @@
     </row>
     <row r="39" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A39" t="s">
-        <v>219</v>
+        <v>217</v>
       </c>
       <c r="B39" t="s">
-        <v>341</v>
+        <v>339</v>
       </c>
       <c r="C39" t="s">
         <v>108</v>
@@ -3407,7 +3474,7 @@
     </row>
     <row r="40" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A40" t="s">
-        <v>219</v>
+        <v>217</v>
       </c>
       <c r="B40" t="s">
         <v>98</v>
@@ -3452,7 +3519,7 @@
     </row>
     <row r="41" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A41" t="s">
-        <v>219</v>
+        <v>217</v>
       </c>
       <c r="B41" t="s">
         <v>99</v>
@@ -3496,13 +3563,13 @@
     </row>
     <row r="42" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A42" t="s">
-        <v>219</v>
+        <v>217</v>
       </c>
       <c r="B42" t="s">
-        <v>431</v>
+        <v>428</v>
       </c>
       <c r="C42" t="s">
-        <v>432</v>
+        <v>429</v>
       </c>
       <c r="D42">
         <v>0</v>
@@ -3536,12 +3603,12 @@
         <v>9.9999999999999995E-7</v>
       </c>
       <c r="N42" t="s">
-        <v>433</v>
+        <v>430</v>
       </c>
     </row>
     <row r="43" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A43" t="s">
-        <v>219</v>
+        <v>217</v>
       </c>
       <c r="B43" t="s">
         <v>125</v>
@@ -3585,7 +3652,7 @@
     </row>
     <row r="44" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A44" t="s">
-        <v>219</v>
+        <v>217</v>
       </c>
       <c r="B44" t="s">
         <v>100</v>
@@ -3630,13 +3697,13 @@
     </row>
     <row r="45" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A45" t="s">
-        <v>219</v>
+        <v>217</v>
       </c>
       <c r="B45" t="s">
-        <v>362</v>
+        <v>360</v>
       </c>
       <c r="C45" t="s">
-        <v>363</v>
+        <v>361</v>
       </c>
       <c r="D45">
         <v>-2</v>
@@ -3669,18 +3736,18 @@
         <v>1.0000000000000001E-5</v>
       </c>
       <c r="N45" t="s">
-        <v>364</v>
+        <v>362</v>
       </c>
     </row>
     <row r="46" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A46" t="s">
-        <v>219</v>
+        <v>217</v>
       </c>
       <c r="B46" t="s">
-        <v>292</v>
+        <v>290</v>
       </c>
       <c r="C46" t="s">
-        <v>293</v>
+        <v>291</v>
       </c>
       <c r="D46">
         <v>-2</v>
@@ -3719,13 +3786,13 @@
     </row>
     <row r="47" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A47" t="s">
+        <v>217</v>
+      </c>
+      <c r="B47" t="s">
         <v>219</v>
       </c>
-      <c r="B47" t="s">
+      <c r="C47" t="s">
         <v>221</v>
-      </c>
-      <c r="C47" t="s">
-        <v>223</v>
       </c>
       <c r="D47">
         <v>-2</v>
@@ -3759,18 +3826,18 @@
         <v>100</v>
       </c>
       <c r="N47" t="s">
-        <v>227</v>
+        <v>225</v>
       </c>
     </row>
     <row r="48" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A48" t="s">
-        <v>219</v>
+        <v>217</v>
       </c>
       <c r="B48" t="s">
-        <v>220</v>
+        <v>218</v>
       </c>
       <c r="C48" t="s">
-        <v>220</v>
+        <v>218</v>
       </c>
       <c r="D48">
         <v>-2</v>
@@ -3804,18 +3871,18 @@
         <v>100000</v>
       </c>
       <c r="N48" t="s">
-        <v>225</v>
+        <v>223</v>
       </c>
     </row>
     <row r="49" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A49" t="s">
-        <v>219</v>
+        <v>217</v>
       </c>
       <c r="B49" t="s">
+        <v>220</v>
+      </c>
+      <c r="C49" t="s">
         <v>222</v>
-      </c>
-      <c r="C49" t="s">
-        <v>224</v>
       </c>
       <c r="D49">
         <v>-2</v>
@@ -3849,12 +3916,12 @@
         <v>1000000</v>
       </c>
       <c r="N49" t="s">
-        <v>226</v>
+        <v>224</v>
       </c>
     </row>
     <row r="50" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A50" t="s">
-        <v>219</v>
+        <v>217</v>
       </c>
       <c r="B50" t="s">
         <v>101</v>
@@ -3894,18 +3961,18 @@
         <v>1.6021766340000001E-19</v>
       </c>
       <c r="N50" t="s">
-        <v>234</v>
+        <v>232</v>
       </c>
     </row>
     <row r="51" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A51" t="s">
+        <v>226</v>
+      </c>
+      <c r="B51" t="s">
+        <v>227</v>
+      </c>
+      <c r="C51" t="s">
         <v>228</v>
-      </c>
-      <c r="B51" t="s">
-        <v>229</v>
-      </c>
-      <c r="C51" t="s">
-        <v>230</v>
       </c>
       <c r="D51">
         <v>-2</v>
@@ -3938,18 +4005,18 @@
         <v>101325</v>
       </c>
       <c r="N51" t="s">
-        <v>233</v>
+        <v>231</v>
       </c>
     </row>
     <row r="52" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A52" t="s">
-        <v>228</v>
+        <v>226</v>
       </c>
       <c r="B52" t="s">
-        <v>231</v>
+        <v>229</v>
       </c>
       <c r="C52" t="s">
-        <v>232</v>
+        <v>230</v>
       </c>
       <c r="D52">
         <v>-2</v>
@@ -3982,18 +4049,18 @@
         <v>133.32238741500001</v>
       </c>
       <c r="N52" t="s">
-        <v>233</v>
+        <v>231</v>
       </c>
     </row>
     <row r="53" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A53" t="s">
-        <v>228</v>
+        <v>226</v>
       </c>
       <c r="B53" t="s">
-        <v>240</v>
+        <v>238</v>
       </c>
       <c r="C53" t="s">
-        <v>241</v>
+        <v>239</v>
       </c>
       <c r="D53">
         <v>-2</v>
@@ -4027,18 +4094,18 @@
         <v>3386.3886403410002</v>
       </c>
       <c r="N53" t="s">
-        <v>242</v>
+        <v>240</v>
       </c>
     </row>
     <row r="54" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A54" t="s">
-        <v>228</v>
+        <v>226</v>
       </c>
       <c r="B54" t="s">
-        <v>237</v>
+        <v>235</v>
       </c>
       <c r="C54" t="s">
-        <v>238</v>
+        <v>236</v>
       </c>
       <c r="D54">
         <v>-2</v>
@@ -4072,18 +4139,18 @@
         <v>0.13332236842105263</v>
       </c>
       <c r="N54" t="s">
-        <v>239</v>
+        <v>237</v>
       </c>
     </row>
     <row r="55" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A55" t="s">
-        <v>228</v>
+        <v>226</v>
       </c>
       <c r="B55" t="s">
-        <v>236</v>
+        <v>234</v>
       </c>
       <c r="C55" t="s">
-        <v>235</v>
+        <v>233</v>
       </c>
       <c r="D55">
         <v>-2</v>
@@ -4117,18 +4184,18 @@
         <v>133.32236842105263</v>
       </c>
       <c r="N55" t="s">
-        <v>233</v>
+        <v>231</v>
       </c>
     </row>
     <row r="56" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A56" t="s">
-        <v>228</v>
+        <v>226</v>
       </c>
       <c r="B56" t="s">
-        <v>368</v>
+        <v>366</v>
       </c>
       <c r="C56" t="s">
-        <v>371</v>
+        <v>369</v>
       </c>
       <c r="D56">
         <v>-1</v>
@@ -4162,18 +4229,18 @@
         <v>6.2831853071795862</v>
       </c>
       <c r="N56" t="s">
-        <v>372</v>
+        <v>370</v>
       </c>
     </row>
     <row r="57" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A57" t="s">
-        <v>228</v>
+        <v>226</v>
       </c>
       <c r="B57" t="s">
-        <v>369</v>
+        <v>367</v>
       </c>
       <c r="C57" t="s">
-        <v>370</v>
+        <v>368</v>
       </c>
       <c r="D57">
         <v>-1</v>
@@ -4207,7 +4274,7 @@
         <v>0.10471975511965977</v>
       </c>
       <c r="N57" t="s">
-        <v>373</v>
+        <v>371</v>
       </c>
     </row>
     <row r="58" spans="1:14" x14ac:dyDescent="0.3">
@@ -4260,7 +4327,7 @@
         <v>77</v>
       </c>
       <c r="B59" t="s">
-        <v>342</v>
+        <v>340</v>
       </c>
       <c r="C59" t="s">
         <v>58</v>
@@ -4305,7 +4372,7 @@
         <v>77</v>
       </c>
       <c r="B60" t="s">
-        <v>349</v>
+        <v>347</v>
       </c>
       <c r="C60" t="s">
         <v>63</v>
@@ -4350,7 +4417,7 @@
         <v>77</v>
       </c>
       <c r="B61" t="s">
-        <v>343</v>
+        <v>341</v>
       </c>
       <c r="C61" t="s">
         <v>59</v>
@@ -4665,7 +4732,7 @@
         <v>77</v>
       </c>
       <c r="B68" t="s">
-        <v>361</v>
+        <v>359</v>
       </c>
       <c r="C68" t="s">
         <v>75</v>
@@ -4800,7 +4867,7 @@
         <v>77</v>
       </c>
       <c r="B71" t="s">
-        <v>332</v>
+        <v>330</v>
       </c>
       <c r="C71" t="s">
         <v>80</v>
@@ -4845,10 +4912,10 @@
         <v>77</v>
       </c>
       <c r="B72" t="s">
-        <v>315</v>
+        <v>313</v>
       </c>
       <c r="C72" t="s">
-        <v>275</v>
+        <v>273</v>
       </c>
       <c r="D72">
         <v>0</v>
@@ -4882,7 +4949,7 @@
         <v>2.8413062500000006E-4</v>
       </c>
       <c r="N72" t="s">
-        <v>276</v>
+        <v>274</v>
       </c>
     </row>
     <row r="73" spans="1:14" x14ac:dyDescent="0.3">
@@ -4890,7 +4957,7 @@
         <v>77</v>
       </c>
       <c r="B73" t="s">
-        <v>333</v>
+        <v>331</v>
       </c>
       <c r="C73" t="s">
         <v>81</v>
@@ -4935,7 +5002,7 @@
         <v>77</v>
       </c>
       <c r="B74" t="s">
-        <v>334</v>
+        <v>332</v>
       </c>
       <c r="C74" t="s">
         <v>82</v>
@@ -4980,7 +5047,7 @@
         <v>77</v>
       </c>
       <c r="B75" t="s">
-        <v>335</v>
+        <v>333</v>
       </c>
       <c r="C75" t="s">
         <v>83</v>
@@ -5017,7 +5084,7 @@
         <v>4.5460900000000009E-3</v>
       </c>
       <c r="N75" t="s">
-        <v>248</v>
+        <v>246</v>
       </c>
     </row>
     <row r="76" spans="1:14" x14ac:dyDescent="0.3">
@@ -5025,10 +5092,10 @@
         <v>77</v>
       </c>
       <c r="B76" t="s">
-        <v>279</v>
+        <v>277</v>
       </c>
       <c r="C76" t="s">
-        <v>283</v>
+        <v>281</v>
       </c>
       <c r="D76">
         <v>0</v>
@@ -5062,7 +5129,7 @@
         <v>9.0921800000000018E-3</v>
       </c>
       <c r="N76" t="s">
-        <v>359</v>
+        <v>357</v>
       </c>
     </row>
     <row r="77" spans="1:14" x14ac:dyDescent="0.3">
@@ -5070,10 +5137,10 @@
         <v>77</v>
       </c>
       <c r="B77" t="s">
-        <v>358</v>
+        <v>356</v>
       </c>
       <c r="C77" t="s">
-        <v>284</v>
+        <v>282</v>
       </c>
       <c r="D77">
         <v>0</v>
@@ -5107,18 +5174,18 @@
         <v>3.6368720000000007E-2</v>
       </c>
       <c r="N77" t="s">
-        <v>360</v>
+        <v>358</v>
       </c>
     </row>
     <row r="78" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A78" t="s">
-        <v>434</v>
+        <v>431</v>
       </c>
       <c r="B78" t="s">
-        <v>272</v>
+        <v>270</v>
       </c>
       <c r="C78" t="s">
-        <v>273</v>
+        <v>271</v>
       </c>
       <c r="D78">
         <v>0</v>
@@ -5152,18 +5219,18 @@
         <v>4.9289215937500005E-6</v>
       </c>
       <c r="N78" t="s">
-        <v>277</v>
+        <v>275</v>
       </c>
     </row>
     <row r="79" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A79" t="s">
-        <v>434</v>
+        <v>431</v>
       </c>
       <c r="B79" t="s">
-        <v>271</v>
+        <v>269</v>
       </c>
       <c r="C79" t="s">
-        <v>274</v>
+        <v>272</v>
       </c>
       <c r="D79">
         <v>0</v>
@@ -5197,18 +5264,18 @@
         <v>1.4786764781250001E-5</v>
       </c>
       <c r="N79" t="s">
-        <v>278</v>
+        <v>276</v>
       </c>
     </row>
     <row r="80" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A80" t="s">
-        <v>434</v>
+        <v>431</v>
       </c>
       <c r="B80" t="s">
-        <v>355</v>
+        <v>353</v>
       </c>
       <c r="C80" t="s">
-        <v>356</v>
+        <v>354</v>
       </c>
       <c r="D80">
         <v>0</v>
@@ -5242,18 +5309,18 @@
         <v>3.6966911953125001E-6</v>
       </c>
       <c r="N80" t="s">
-        <v>357</v>
+        <v>355</v>
       </c>
     </row>
     <row r="81" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A81" t="s">
-        <v>434</v>
+        <v>431</v>
       </c>
       <c r="B81" t="s">
         <v>78</v>
       </c>
       <c r="C81" t="s">
-        <v>263</v>
+        <v>261</v>
       </c>
       <c r="D81">
         <v>0</v>
@@ -5287,18 +5354,18 @@
         <v>2.9573529562500001E-5</v>
       </c>
       <c r="N81" t="s">
-        <v>267</v>
+        <v>265</v>
       </c>
     </row>
     <row r="82" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A82" t="s">
-        <v>434</v>
+        <v>431</v>
       </c>
       <c r="B82" t="s">
-        <v>332</v>
+        <v>330</v>
       </c>
       <c r="C82" t="s">
-        <v>264</v>
+        <v>262</v>
       </c>
       <c r="D82">
         <v>0</v>
@@ -5332,18 +5399,18 @@
         <v>9.4635294600000004E-4</v>
       </c>
       <c r="N82" t="s">
-        <v>268</v>
+        <v>266</v>
       </c>
     </row>
     <row r="83" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A83" t="s">
-        <v>434</v>
+        <v>431</v>
       </c>
       <c r="B83" t="s">
-        <v>333</v>
+        <v>331</v>
       </c>
       <c r="C83" t="s">
-        <v>265</v>
+        <v>263</v>
       </c>
       <c r="D83">
         <v>0</v>
@@ -5377,18 +5444,18 @@
         <v>4.7317647300000002E-4</v>
       </c>
       <c r="N83" t="s">
-        <v>269</v>
+        <v>267</v>
       </c>
     </row>
     <row r="84" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A84" t="s">
-        <v>434</v>
+        <v>431</v>
       </c>
       <c r="B84" t="s">
-        <v>334</v>
+        <v>332</v>
       </c>
       <c r="C84" t="s">
-        <v>262</v>
+        <v>260</v>
       </c>
       <c r="D84">
         <v>0</v>
@@ -5422,18 +5489,18 @@
         <v>9.4635294600000004E-4</v>
       </c>
       <c r="N84" t="s">
-        <v>270</v>
+        <v>268</v>
       </c>
     </row>
     <row r="85" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A85" t="s">
-        <v>434</v>
+        <v>431</v>
       </c>
       <c r="B85" t="s">
-        <v>336</v>
+        <v>334</v>
       </c>
       <c r="C85" t="s">
-        <v>261</v>
+        <v>259</v>
       </c>
       <c r="D85">
         <v>0</v>
@@ -5467,18 +5534,18 @@
         <v>1.8927058920000001E-3</v>
       </c>
       <c r="N85" t="s">
-        <v>266</v>
+        <v>264</v>
       </c>
     </row>
     <row r="86" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A86" t="s">
-        <v>434</v>
+        <v>431</v>
       </c>
       <c r="B86" t="s">
-        <v>335</v>
+        <v>333</v>
       </c>
       <c r="C86" t="s">
-        <v>260</v>
+        <v>258</v>
       </c>
       <c r="D86">
         <v>0</v>
@@ -5512,18 +5579,18 @@
         <v>3.7854117840000001E-3</v>
       </c>
       <c r="N86" t="s">
-        <v>249</v>
+        <v>247</v>
       </c>
     </row>
     <row r="87" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A87" t="s">
-        <v>434</v>
+        <v>431</v>
       </c>
       <c r="B87" t="s">
-        <v>350</v>
+        <v>348</v>
       </c>
       <c r="C87" t="s">
-        <v>280</v>
+        <v>278</v>
       </c>
       <c r="D87">
         <v>0</v>
@@ -5557,18 +5624,18 @@
         <v>5.506104713575E-4</v>
       </c>
       <c r="N87" t="s">
-        <v>286</v>
+        <v>284</v>
       </c>
     </row>
     <row r="88" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A88" t="s">
-        <v>434</v>
+        <v>431</v>
       </c>
       <c r="B88" t="s">
-        <v>351</v>
+        <v>349</v>
       </c>
       <c r="C88" t="s">
-        <v>281</v>
+        <v>279</v>
       </c>
       <c r="D88">
         <v>0</v>
@@ -5602,18 +5669,18 @@
         <v>1.101220942715E-3</v>
       </c>
       <c r="N88" t="s">
-        <v>285</v>
+        <v>283</v>
       </c>
     </row>
     <row r="89" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A89" t="s">
-        <v>434</v>
+        <v>431</v>
       </c>
       <c r="B89" t="s">
-        <v>352</v>
+        <v>350</v>
       </c>
       <c r="C89" t="s">
-        <v>282</v>
+        <v>280</v>
       </c>
       <c r="D89">
         <v>0</v>
@@ -5647,18 +5714,18 @@
         <v>4.40488377086E-3</v>
       </c>
       <c r="N89" t="s">
-        <v>287</v>
+        <v>285</v>
       </c>
     </row>
     <row r="90" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A90" t="s">
-        <v>434</v>
+        <v>431</v>
       </c>
       <c r="B90" t="s">
-        <v>353</v>
+        <v>351</v>
       </c>
       <c r="C90" t="s">
-        <v>354</v>
+        <v>352</v>
       </c>
       <c r="D90">
         <v>0</v>
@@ -5692,18 +5759,18 @@
         <v>8.8097675417200001E-3</v>
       </c>
       <c r="N90" t="s">
-        <v>289</v>
+        <v>287</v>
       </c>
     </row>
     <row r="91" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A91" t="s">
-        <v>434</v>
+        <v>431</v>
       </c>
       <c r="B91" t="s">
-        <v>358</v>
+        <v>356</v>
       </c>
       <c r="C91" t="s">
-        <v>284</v>
+        <v>282</v>
       </c>
       <c r="D91">
         <v>0</v>
@@ -5737,7 +5804,7 @@
         <v>3.523907016688E-2</v>
       </c>
       <c r="N91" t="s">
-        <v>288</v>
+        <v>286</v>
       </c>
     </row>
     <row r="92" spans="1:14" x14ac:dyDescent="0.3">
@@ -5883,7 +5950,7 @@
         <v>136</v>
       </c>
       <c r="C95" t="s">
-        <v>204</v>
+        <v>202</v>
       </c>
       <c r="D95">
         <v>0</v>
@@ -5917,7 +5984,7 @@
         <v>0.45359237000000002</v>
       </c>
       <c r="N95" t="s">
-        <v>256</v>
+        <v>254</v>
       </c>
     </row>
     <row r="96" spans="1:14" x14ac:dyDescent="0.3">
@@ -6015,10 +6082,10 @@
         <v>77</v>
       </c>
       <c r="B98" t="s">
-        <v>347</v>
+        <v>345</v>
       </c>
       <c r="C98" t="s">
-        <v>251</v>
+        <v>249</v>
       </c>
       <c r="D98">
         <v>0</v>
@@ -6052,7 +6119,7 @@
         <v>50.802345440000003</v>
       </c>
       <c r="N98" t="s">
-        <v>252</v>
+        <v>250</v>
       </c>
     </row>
     <row r="99" spans="1:14" x14ac:dyDescent="0.3">
@@ -6060,10 +6127,10 @@
         <v>77</v>
       </c>
       <c r="B99" t="s">
-        <v>346</v>
+        <v>344</v>
       </c>
       <c r="C99" t="s">
-        <v>254</v>
+        <v>252</v>
       </c>
       <c r="D99">
         <v>0</v>
@@ -6097,18 +6164,18 @@
         <v>1016.0469088000001</v>
       </c>
       <c r="N99" t="s">
-        <v>253</v>
+        <v>251</v>
       </c>
     </row>
     <row r="100" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A100" t="s">
-        <v>434</v>
+        <v>431</v>
       </c>
       <c r="B100" t="s">
-        <v>345</v>
+        <v>343</v>
       </c>
       <c r="C100" t="s">
-        <v>257</v>
+        <v>255</v>
       </c>
       <c r="D100">
         <v>0</v>
@@ -6142,18 +6209,18 @@
         <v>45.359237</v>
       </c>
       <c r="N100" t="s">
-        <v>258</v>
+        <v>256</v>
       </c>
     </row>
     <row r="101" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A101" t="s">
-        <v>434</v>
+        <v>431</v>
       </c>
       <c r="B101" t="s">
-        <v>344</v>
+        <v>342</v>
       </c>
       <c r="C101" t="s">
-        <v>255</v>
+        <v>253</v>
       </c>
       <c r="D101">
         <v>0</v>
@@ -6187,7 +6254,7 @@
         <v>907.18474000000003</v>
       </c>
       <c r="N101" t="s">
-        <v>259</v>
+        <v>257</v>
       </c>
     </row>
     <row r="102" spans="1:14" x14ac:dyDescent="0.3">
@@ -6285,10 +6352,10 @@
         <v>77</v>
       </c>
       <c r="B104" t="s">
-        <v>216</v>
+        <v>214</v>
       </c>
       <c r="C104" t="s">
-        <v>217</v>
+        <v>215</v>
       </c>
       <c r="D104">
         <v>-2</v>
@@ -6322,7 +6389,7 @@
         <v>6894.7572931683608</v>
       </c>
       <c r="N104" t="s">
-        <v>218</v>
+        <v>216</v>
       </c>
     </row>
     <row r="105" spans="1:14" x14ac:dyDescent="0.3">
@@ -6412,7 +6479,7 @@
         <v>0.55555555555555558</v>
       </c>
       <c r="N106" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
     </row>
     <row r="107" spans="1:14" x14ac:dyDescent="0.3">
@@ -6457,7 +6524,7 @@
         <v>0.55555555555555558</v>
       </c>
       <c r="N107" t="s">
-        <v>197</v>
+        <v>433</v>
       </c>
     </row>
     <row r="108" spans="1:14" x14ac:dyDescent="0.3">
@@ -6465,10 +6532,10 @@
         <v>77</v>
       </c>
       <c r="B108" t="s">
-        <v>337</v>
+        <v>335</v>
       </c>
       <c r="C108" t="s">
-        <v>201</v>
+        <v>199</v>
       </c>
       <c r="D108">
         <v>-2</v>
@@ -6501,7 +6568,7 @@
         <v>4.1840000000000002</v>
       </c>
       <c r="N108" t="s">
-        <v>247</v>
+        <v>245</v>
       </c>
     </row>
     <row r="109" spans="1:14" x14ac:dyDescent="0.3">
@@ -6509,10 +6576,10 @@
         <v>77</v>
       </c>
       <c r="B109" t="s">
-        <v>338</v>
+        <v>336</v>
       </c>
       <c r="C109" t="s">
-        <v>202</v>
+        <v>200</v>
       </c>
       <c r="D109">
         <v>-2</v>
@@ -6542,11 +6609,11 @@
         <v>0</v>
       </c>
       <c r="M109">
-        <f>M108/M4</f>
+        <f>M108 * (10^prefixes!$D$9)</f>
         <v>4184</v>
       </c>
       <c r="N109" t="s">
-        <v>203</v>
+        <v>201</v>
       </c>
     </row>
     <row r="110" spans="1:14" x14ac:dyDescent="0.3">
@@ -6554,10 +6621,10 @@
         <v>77</v>
       </c>
       <c r="B110" t="s">
-        <v>365</v>
+        <v>363</v>
       </c>
       <c r="C110" t="s">
-        <v>206</v>
+        <v>204</v>
       </c>
       <c r="D110">
         <v>-2</v>
@@ -6591,7 +6658,7 @@
         <v>4.1867999999999999</v>
       </c>
       <c r="N110" t="s">
-        <v>250</v>
+        <v>248</v>
       </c>
     </row>
     <row r="111" spans="1:14" x14ac:dyDescent="0.3">
@@ -6599,10 +6666,10 @@
         <v>77</v>
       </c>
       <c r="B111" t="s">
-        <v>366</v>
+        <v>364</v>
       </c>
       <c r="C111" t="s">
-        <v>207</v>
+        <v>205</v>
       </c>
       <c r="D111">
         <v>-2</v>
@@ -6632,11 +6699,11 @@
         <v>0</v>
       </c>
       <c r="M111">
-        <f>M110/M4</f>
+        <f>M110 * (10^prefixes!$D$9)</f>
         <v>4186.8</v>
       </c>
       <c r="N111" t="s">
-        <v>208</v>
+        <v>206</v>
       </c>
     </row>
     <row r="112" spans="1:14" x14ac:dyDescent="0.3">
@@ -6644,10 +6711,10 @@
         <v>77</v>
       </c>
       <c r="B112" t="s">
-        <v>339</v>
+        <v>337</v>
       </c>
       <c r="C112" t="s">
-        <v>200</v>
+        <v>198</v>
       </c>
       <c r="D112">
         <v>-2</v>
@@ -6681,7 +6748,7 @@
         <v>1054.350264488889</v>
       </c>
       <c r="N112" t="s">
-        <v>205</v>
+        <v>203</v>
       </c>
     </row>
     <row r="113" spans="1:14" x14ac:dyDescent="0.3">
@@ -6689,10 +6756,10 @@
         <v>77</v>
       </c>
       <c r="B113" t="s">
-        <v>367</v>
+        <v>365</v>
       </c>
       <c r="C113" t="s">
-        <v>209</v>
+        <v>207</v>
       </c>
       <c r="D113">
         <v>-2</v>
@@ -6726,7 +6793,7 @@
         <v>1055.05585262</v>
       </c>
       <c r="N113" t="s">
-        <v>210</v>
+        <v>208</v>
       </c>
     </row>
     <row r="114" spans="1:14" x14ac:dyDescent="0.3">
@@ -6734,10 +6801,10 @@
         <v>77</v>
       </c>
       <c r="B114" t="s">
+        <v>209</v>
+      </c>
+      <c r="C114" t="s">
         <v>211</v>
-      </c>
-      <c r="C114" t="s">
-        <v>213</v>
       </c>
       <c r="D114">
         <v>-2</v>
@@ -6771,7 +6838,7 @@
         <v>105505585.26199999</v>
       </c>
       <c r="N114" t="s">
-        <v>215</v>
+        <v>213</v>
       </c>
     </row>
     <row r="115" spans="1:14" x14ac:dyDescent="0.3">
@@ -6779,10 +6846,10 @@
         <v>77</v>
       </c>
       <c r="B115" t="s">
+        <v>210</v>
+      </c>
+      <c r="C115" t="s">
         <v>212</v>
-      </c>
-      <c r="C115" t="s">
-        <v>214</v>
       </c>
       <c r="D115">
         <v>-2</v>
@@ -6816,15 +6883,15 @@
         <v>1.05505585262E+18</v>
       </c>
       <c r="N115" t="s">
-        <v>215</v>
+        <v>213</v>
       </c>
     </row>
     <row r="116" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A116" t="s">
-        <v>374</v>
+        <v>372</v>
       </c>
       <c r="B116" t="s">
-        <v>377</v>
+        <v>375</v>
       </c>
       <c r="M116">
         <v>0</v>
@@ -6832,10 +6899,10 @@
     </row>
     <row r="117" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A117" t="s">
-        <v>374</v>
+        <v>372</v>
       </c>
       <c r="B117" t="s">
-        <v>326</v>
+        <v>324</v>
       </c>
       <c r="M117">
         <v>0</v>
@@ -6843,10 +6910,10 @@
     </row>
     <row r="118" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A118" t="s">
-        <v>374</v>
+        <v>372</v>
       </c>
       <c r="B118" t="s">
-        <v>378</v>
+        <v>376</v>
       </c>
       <c r="M118">
         <v>0</v>
@@ -6854,24 +6921,24 @@
     </row>
     <row r="119" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A119" t="s">
-        <v>374</v>
+        <v>372</v>
       </c>
       <c r="B119" t="s">
-        <v>315</v>
+        <v>313</v>
       </c>
       <c r="M119">
         <v>0</v>
       </c>
       <c r="N119" t="s">
-        <v>410</v>
+        <v>408</v>
       </c>
     </row>
     <row r="120" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A120" t="s">
-        <v>374</v>
+        <v>372</v>
       </c>
       <c r="B120" t="s">
-        <v>379</v>
+        <v>377</v>
       </c>
       <c r="M120">
         <v>0</v>
@@ -6879,10 +6946,10 @@
     </row>
     <row r="121" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A121" t="s">
-        <v>374</v>
+        <v>372</v>
       </c>
       <c r="B121" t="s">
-        <v>380</v>
+        <v>378</v>
       </c>
       <c r="M121">
         <v>0</v>
@@ -6890,38 +6957,38 @@
     </row>
     <row r="122" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A122" t="s">
-        <v>374</v>
+        <v>372</v>
       </c>
       <c r="B122" t="s">
-        <v>381</v>
+        <v>379</v>
       </c>
       <c r="M122">
         <v>0</v>
       </c>
       <c r="N122" t="s">
-        <v>415</v>
+        <v>413</v>
       </c>
     </row>
     <row r="123" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A123" t="s">
-        <v>374</v>
+        <v>372</v>
       </c>
       <c r="B123" t="s">
-        <v>382</v>
+        <v>380</v>
       </c>
       <c r="M123">
         <v>0</v>
       </c>
       <c r="N123" t="s">
-        <v>411</v>
+        <v>409</v>
       </c>
     </row>
     <row r="124" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A124" t="s">
-        <v>374</v>
+        <v>372</v>
       </c>
       <c r="B124" t="s">
-        <v>383</v>
+        <v>381</v>
       </c>
       <c r="D124">
         <v>-3</v>
@@ -6954,68 +7021,68 @@
         <v>-150</v>
       </c>
       <c r="N124" t="s">
-        <v>428</v>
+        <v>425</v>
       </c>
     </row>
     <row r="125" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A125" t="s">
-        <v>374</v>
+        <v>372</v>
       </c>
       <c r="B125" t="s">
-        <v>384</v>
+        <v>382</v>
       </c>
       <c r="M125">
         <v>0</v>
       </c>
       <c r="N125" t="s">
-        <v>412</v>
+        <v>410</v>
       </c>
     </row>
     <row r="126" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A126" t="s">
-        <v>374</v>
+        <v>372</v>
       </c>
       <c r="B126" t="s">
-        <v>304</v>
+        <v>302</v>
       </c>
       <c r="M126">
         <v>0</v>
       </c>
       <c r="N126" t="s">
-        <v>413</v>
+        <v>411</v>
       </c>
     </row>
     <row r="127" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A127" t="s">
-        <v>374</v>
+        <v>372</v>
       </c>
       <c r="B127" t="s">
-        <v>385</v>
+        <v>383</v>
       </c>
       <c r="M127">
         <v>0</v>
       </c>
       <c r="N127" t="s">
-        <v>414</v>
+        <v>412</v>
       </c>
     </row>
     <row r="128" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A128" t="s">
-        <v>374</v>
+        <v>372</v>
       </c>
       <c r="B128" t="s">
-        <v>386</v>
+        <v>384</v>
       </c>
       <c r="M128">
         <v>0</v>
       </c>
       <c r="N128" t="s">
-        <v>416</v>
+        <v>414</v>
       </c>
     </row>
     <row r="129" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A129" t="s">
-        <v>374</v>
+        <v>372</v>
       </c>
       <c r="B129" t="s">
         <v>24</v>
@@ -7024,15 +7091,15 @@
         <v>0</v>
       </c>
       <c r="N129" t="s">
-        <v>417</v>
+        <v>415</v>
       </c>
     </row>
     <row r="130" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A130" t="s">
-        <v>374</v>
+        <v>372</v>
       </c>
       <c r="B130" t="s">
-        <v>387</v>
+        <v>385</v>
       </c>
       <c r="D130">
         <v>-3</v>
@@ -7065,29 +7132,29 @@
         <v>30</v>
       </c>
       <c r="N130" t="s">
-        <v>427</v>
+        <v>424</v>
       </c>
     </row>
     <row r="131" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A131" t="s">
-        <v>374</v>
+        <v>372</v>
       </c>
       <c r="B131" t="s">
-        <v>388</v>
+        <v>386</v>
       </c>
       <c r="M131">
         <v>0</v>
       </c>
       <c r="N131" t="s">
-        <v>418</v>
+        <v>416</v>
       </c>
     </row>
     <row r="132" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A132" t="s">
-        <v>374</v>
+        <v>372</v>
       </c>
       <c r="B132" t="s">
-        <v>389</v>
+        <v>387</v>
       </c>
       <c r="D132">
         <v>-3</v>
@@ -7120,15 +7187,15 @@
         <v>-30</v>
       </c>
       <c r="N132" t="s">
-        <v>429</v>
+        <v>426</v>
       </c>
     </row>
     <row r="133" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A133" t="s">
-        <v>374</v>
+        <v>372</v>
       </c>
       <c r="B133" t="s">
-        <v>425</v>
+        <v>422</v>
       </c>
       <c r="D133">
         <v>-3</v>
@@ -7160,10 +7227,10 @@
     </row>
     <row r="134" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A134" t="s">
-        <v>374</v>
+        <v>372</v>
       </c>
       <c r="B134" t="s">
-        <v>390</v>
+        <v>388</v>
       </c>
       <c r="M134">
         <v>0</v>
@@ -7171,10 +7238,10 @@
     </row>
     <row r="135" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A135" t="s">
-        <v>374</v>
+        <v>372</v>
       </c>
       <c r="B135" t="s">
-        <v>391</v>
+        <v>389</v>
       </c>
       <c r="D135">
         <v>-3</v>
@@ -7207,15 +7274,15 @@
         <v>0</v>
       </c>
       <c r="N135" t="s">
-        <v>419</v>
+        <v>417</v>
       </c>
     </row>
     <row r="136" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A136" t="s">
-        <v>374</v>
+        <v>372</v>
       </c>
       <c r="B136" t="s">
-        <v>392</v>
+        <v>390</v>
       </c>
       <c r="M136">
         <v>0</v>
@@ -7223,10 +7290,10 @@
     </row>
     <row r="137" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A137" t="s">
-        <v>374</v>
+        <v>372</v>
       </c>
       <c r="B137" t="s">
-        <v>393</v>
+        <v>391</v>
       </c>
       <c r="M137">
         <v>0</v>
@@ -7234,10 +7301,10 @@
     </row>
     <row r="138" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A138" t="s">
-        <v>374</v>
+        <v>372</v>
       </c>
       <c r="B138" t="s">
-        <v>394</v>
+        <v>392</v>
       </c>
       <c r="M138">
         <v>0</v>
@@ -7245,10 +7312,10 @@
     </row>
     <row r="139" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A139" t="s">
-        <v>374</v>
+        <v>372</v>
       </c>
       <c r="B139" t="s">
-        <v>395</v>
+        <v>393</v>
       </c>
       <c r="M139">
         <v>0</v>
@@ -7256,10 +7323,10 @@
     </row>
     <row r="140" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A140" t="s">
-        <v>374</v>
+        <v>372</v>
       </c>
       <c r="B140" t="s">
-        <v>396</v>
+        <v>394</v>
       </c>
       <c r="M140">
         <v>0</v>
@@ -7267,10 +7334,10 @@
     </row>
     <row r="141" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A141" t="s">
-        <v>374</v>
+        <v>372</v>
       </c>
       <c r="B141" t="s">
-        <v>397</v>
+        <v>395</v>
       </c>
       <c r="D141">
         <v>0</v>
@@ -7305,10 +7372,10 @@
     </row>
     <row r="142" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A142" t="s">
-        <v>374</v>
+        <v>372</v>
       </c>
       <c r="B142" t="s">
-        <v>398</v>
+        <v>396</v>
       </c>
       <c r="M142">
         <v>0</v>
@@ -7316,10 +7383,10 @@
     </row>
     <row r="143" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A143" t="s">
-        <v>374</v>
+        <v>372</v>
       </c>
       <c r="B143" t="s">
-        <v>399</v>
+        <v>397</v>
       </c>
       <c r="D143">
         <v>-3</v>
@@ -7352,15 +7419,15 @@
         <v>0</v>
       </c>
       <c r="N143" t="s">
-        <v>423</v>
+        <v>420</v>
       </c>
     </row>
     <row r="144" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A144" t="s">
-        <v>374</v>
+        <v>372</v>
       </c>
       <c r="B144" t="s">
-        <v>400</v>
+        <v>398</v>
       </c>
       <c r="M144">
         <v>0</v>
@@ -7368,10 +7435,10 @@
     </row>
     <row r="145" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A145" t="s">
-        <v>374</v>
+        <v>372</v>
       </c>
       <c r="B145" t="s">
-        <v>401</v>
+        <v>399</v>
       </c>
       <c r="D145">
         <v>-3</v>
@@ -7404,15 +7471,15 @@
         <v>0</v>
       </c>
       <c r="N145" t="s">
-        <v>426</v>
+        <v>423</v>
       </c>
     </row>
     <row r="146" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A146" t="s">
-        <v>374</v>
+        <v>372</v>
       </c>
       <c r="B146" t="s">
-        <v>402</v>
+        <v>400</v>
       </c>
       <c r="M146">
         <v>0</v>
@@ -7420,24 +7487,24 @@
     </row>
     <row r="147" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A147" t="s">
-        <v>374</v>
+        <v>372</v>
       </c>
       <c r="B147" t="s">
-        <v>403</v>
+        <v>401</v>
       </c>
       <c r="M147">
         <v>0</v>
       </c>
       <c r="N147" t="s">
-        <v>424</v>
+        <v>421</v>
       </c>
     </row>
     <row r="148" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A148" t="s">
-        <v>374</v>
+        <v>372</v>
       </c>
       <c r="B148" t="s">
-        <v>404</v>
+        <v>402</v>
       </c>
       <c r="M148">
         <v>0</v>
@@ -7445,7 +7512,7 @@
     </row>
     <row r="149" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A149" t="s">
-        <v>374</v>
+        <v>372</v>
       </c>
       <c r="B149" t="s">
         <v>25</v>
@@ -7481,15 +7548,15 @@
         <v>0</v>
       </c>
       <c r="N149" t="s">
-        <v>430</v>
+        <v>427</v>
       </c>
     </row>
     <row r="150" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A150" t="s">
-        <v>374</v>
+        <v>372</v>
       </c>
       <c r="B150" t="s">
-        <v>405</v>
+        <v>403</v>
       </c>
       <c r="M150">
         <v>0</v>
@@ -7497,10 +7564,10 @@
     </row>
     <row r="151" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A151" t="s">
-        <v>374</v>
+        <v>372</v>
       </c>
       <c r="B151" t="s">
-        <v>406</v>
+        <v>404</v>
       </c>
       <c r="M151">
         <v>0</v>
@@ -7508,10 +7575,10 @@
     </row>
     <row r="152" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A152" t="s">
-        <v>374</v>
+        <v>372</v>
       </c>
       <c r="B152" t="s">
-        <v>422</v>
+        <v>419</v>
       </c>
       <c r="M152">
         <v>0</v>
@@ -7519,10 +7586,10 @@
     </row>
     <row r="153" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A153" t="s">
-        <v>374</v>
+        <v>372</v>
       </c>
       <c r="B153" t="s">
-        <v>421</v>
+        <v>418</v>
       </c>
       <c r="D153">
         <v>-3</v>
@@ -7557,10 +7624,10 @@
     </row>
     <row r="154" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A154" t="s">
-        <v>374</v>
+        <v>372</v>
       </c>
       <c r="B154" t="s">
-        <v>407</v>
+        <v>405</v>
       </c>
       <c r="D154">
         <v>-1</v>
@@ -7595,10 +7662,10 @@
     </row>
     <row r="155" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A155" t="s">
-        <v>374</v>
+        <v>372</v>
       </c>
       <c r="B155" t="s">
-        <v>408</v>
+        <v>406</v>
       </c>
       <c r="D155">
         <v>0</v>
@@ -7633,10 +7700,10 @@
     </row>
     <row r="156" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A156" t="s">
-        <v>374</v>
+        <v>372</v>
       </c>
       <c r="B156" t="s">
-        <v>409</v>
+        <v>407</v>
       </c>
       <c r="D156">
         <v>0</v>
@@ -7667,6 +7734,96 @@
       </c>
       <c r="M156">
         <v>0</v>
+      </c>
+    </row>
+    <row r="157" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A157" t="s">
+        <v>77</v>
+      </c>
+      <c r="B157" t="s">
+        <v>437</v>
+      </c>
+      <c r="C157" t="s">
+        <v>435</v>
+      </c>
+      <c r="D157">
+        <v>-1</v>
+      </c>
+      <c r="E157">
+        <v>1</v>
+      </c>
+      <c r="F157">
+        <v>0</v>
+      </c>
+      <c r="G157">
+        <v>0</v>
+      </c>
+      <c r="H157">
+        <v>0</v>
+      </c>
+      <c r="I157">
+        <v>0</v>
+      </c>
+      <c r="J157">
+        <v>0</v>
+      </c>
+      <c r="K157">
+        <v>0</v>
+      </c>
+      <c r="L157">
+        <v>0</v>
+      </c>
+      <c r="M157">
+        <f>M65/M32</f>
+        <v>0.44703999999999994</v>
+      </c>
+      <c r="N157" t="s">
+        <v>436</v>
+      </c>
+    </row>
+    <row r="158" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A158" t="s">
+        <v>226</v>
+      </c>
+      <c r="B158" t="s">
+        <v>438</v>
+      </c>
+      <c r="C158" t="s">
+        <v>439</v>
+      </c>
+      <c r="D158">
+        <v>-1</v>
+      </c>
+      <c r="E158">
+        <v>1</v>
+      </c>
+      <c r="F158">
+        <v>0</v>
+      </c>
+      <c r="G158">
+        <v>0</v>
+      </c>
+      <c r="H158">
+        <v>0</v>
+      </c>
+      <c r="I158">
+        <v>0</v>
+      </c>
+      <c r="J158">
+        <v>0</v>
+      </c>
+      <c r="K158">
+        <v>0</v>
+      </c>
+      <c r="L158">
+        <v>0</v>
+      </c>
+      <c r="M158">
+        <f>M3 *(10^prefixes!$D$9)/M32</f>
+        <v>0.27777777777777779</v>
+      </c>
+      <c r="N158" t="s">
+        <v>440</v>
       </c>
     </row>
   </sheetData>
@@ -7683,6 +7840,7 @@
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <legacyDrawing r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -7694,7 +7852,7 @@
       <selection activeCell="A12" sqref="A12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
@@ -7707,7 +7865,7 @@
         <v>1</v>
       </c>
       <c r="D1" t="s">
-        <v>294</v>
+        <v>292</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.3">
@@ -7715,10 +7873,10 @@
         <v>95</v>
       </c>
       <c r="B2" t="s">
-        <v>295</v>
+        <v>293</v>
       </c>
       <c r="C2" t="s">
-        <v>296</v>
+        <v>294</v>
       </c>
       <c r="D2">
         <v>24</v>
@@ -7729,10 +7887,10 @@
         <v>95</v>
       </c>
       <c r="B3" t="s">
-        <v>297</v>
+        <v>295</v>
       </c>
       <c r="C3" t="s">
-        <v>298</v>
+        <v>296</v>
       </c>
       <c r="D3">
         <v>21</v>
@@ -7743,10 +7901,10 @@
         <v>95</v>
       </c>
       <c r="B4" t="s">
-        <v>299</v>
+        <v>297</v>
       </c>
       <c r="C4" t="s">
-        <v>300</v>
+        <v>298</v>
       </c>
       <c r="D4">
         <v>18</v>
@@ -7757,10 +7915,10 @@
         <v>95</v>
       </c>
       <c r="B5" t="s">
-        <v>301</v>
+        <v>299</v>
       </c>
       <c r="C5" t="s">
-        <v>302</v>
+        <v>300</v>
       </c>
       <c r="D5">
         <v>15</v>
@@ -7774,7 +7932,7 @@
         <v>32</v>
       </c>
       <c r="C6" t="s">
-        <v>303</v>
+        <v>301</v>
       </c>
       <c r="D6">
         <v>12</v>
@@ -7785,10 +7943,10 @@
         <v>95</v>
       </c>
       <c r="B7" t="s">
-        <v>304</v>
+        <v>302</v>
       </c>
       <c r="C7" t="s">
-        <v>305</v>
+        <v>303</v>
       </c>
       <c r="D7">
         <v>9</v>
@@ -7799,10 +7957,10 @@
         <v>95</v>
       </c>
       <c r="B8" t="s">
-        <v>306</v>
+        <v>304</v>
       </c>
       <c r="C8" t="s">
-        <v>307</v>
+        <v>305</v>
       </c>
       <c r="D8">
         <v>6</v>
@@ -7813,10 +7971,10 @@
         <v>95</v>
       </c>
       <c r="B9" t="s">
-        <v>308</v>
+        <v>306</v>
       </c>
       <c r="C9" t="s">
-        <v>309</v>
+        <v>307</v>
       </c>
       <c r="D9">
         <v>3</v>
@@ -7830,7 +7988,7 @@
         <v>65</v>
       </c>
       <c r="C10" t="s">
-        <v>310</v>
+        <v>308</v>
       </c>
       <c r="D10">
         <v>2</v>
@@ -7841,19 +7999,16 @@
         <v>95</v>
       </c>
       <c r="B11" t="s">
-        <v>311</v>
+        <v>309</v>
       </c>
       <c r="C11" t="s">
-        <v>312</v>
+        <v>310</v>
       </c>
       <c r="D11">
         <v>1</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A12" t="s">
-        <v>95</v>
-      </c>
       <c r="D12">
         <v>0</v>
       </c>
@@ -7863,10 +8018,10 @@
         <v>95</v>
       </c>
       <c r="B13" t="s">
-        <v>313</v>
+        <v>311</v>
       </c>
       <c r="C13" t="s">
-        <v>314</v>
+        <v>312</v>
       </c>
       <c r="D13">
         <v>-1</v>
@@ -7877,10 +8032,10 @@
         <v>95</v>
       </c>
       <c r="B14" t="s">
-        <v>315</v>
+        <v>313</v>
       </c>
       <c r="C14" t="s">
-        <v>316</v>
+        <v>314</v>
       </c>
       <c r="D14">
         <v>-2</v>
@@ -7894,7 +8049,7 @@
         <v>3</v>
       </c>
       <c r="C15" t="s">
-        <v>317</v>
+        <v>315</v>
       </c>
       <c r="D15">
         <v>-3</v>
@@ -7905,10 +8060,10 @@
         <v>95</v>
       </c>
       <c r="B16" t="s">
-        <v>318</v>
+        <v>316</v>
       </c>
       <c r="C16" t="s">
-        <v>319</v>
+        <v>317</v>
       </c>
       <c r="D16">
         <v>-6</v>
@@ -7919,10 +8074,10 @@
         <v>95</v>
       </c>
       <c r="B17" t="s">
-        <v>320</v>
+        <v>318</v>
       </c>
       <c r="C17" t="s">
-        <v>321</v>
+        <v>319</v>
       </c>
       <c r="D17">
         <v>-9</v>
@@ -7933,10 +8088,10 @@
         <v>95</v>
       </c>
       <c r="B18" t="s">
-        <v>322</v>
+        <v>320</v>
       </c>
       <c r="C18" t="s">
-        <v>323</v>
+        <v>321</v>
       </c>
       <c r="D18">
         <v>-12</v>
@@ -7947,10 +8102,10 @@
         <v>95</v>
       </c>
       <c r="B19" t="s">
-        <v>324</v>
+        <v>322</v>
       </c>
       <c r="C19" t="s">
-        <v>325</v>
+        <v>323</v>
       </c>
       <c r="D19">
         <v>-15</v>
@@ -7961,10 +8116,10 @@
         <v>95</v>
       </c>
       <c r="B20" t="s">
-        <v>326</v>
+        <v>324</v>
       </c>
       <c r="C20" t="s">
-        <v>327</v>
+        <v>325</v>
       </c>
       <c r="D20">
         <v>-18</v>
@@ -7975,10 +8130,10 @@
         <v>95</v>
       </c>
       <c r="B21" t="s">
-        <v>328</v>
+        <v>326</v>
       </c>
       <c r="C21" t="s">
-        <v>329</v>
+        <v>327</v>
       </c>
       <c r="D21">
         <v>-21</v>
@@ -7989,10 +8144,10 @@
         <v>95</v>
       </c>
       <c r="B22" t="s">
-        <v>330</v>
+        <v>328</v>
       </c>
       <c r="C22" t="s">
-        <v>331</v>
+        <v>329</v>
       </c>
       <c r="D22">
         <v>-24</v>
@@ -8000,13 +8155,13 @@
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
+        <v>372</v>
+      </c>
+      <c r="B23" t="s">
+        <v>373</v>
+      </c>
+      <c r="C23" t="s">
         <v>374</v>
-      </c>
-      <c r="B23" t="s">
-        <v>375</v>
-      </c>
-      <c r="C23" t="s">
-        <v>376</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Initial commit of powerplant IO types
</commit_message>
<xml_diff>
--- a/src/carpy/utility/data/quantities.xlsx
+++ b/src/carpy/utility/data/quantities.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\yr3g17\PycharmProjects\carpy\src\carpy\utility\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7F33FFD5-518D-4FE3-B688-95659F3C90BE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E1D4C2FC-21FF-43A6-ADC4-A936D334C31C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -69,7 +69,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="644" uniqueCount="441">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="656" uniqueCount="450">
   <si>
     <t>Symbol</t>
   </si>
@@ -158,9 +158,6 @@
     <t>F</t>
   </si>
   <si>
-    <t>O</t>
-  </si>
-  <si>
     <t>S</t>
   </si>
   <si>
@@ -1392,6 +1389,36 @@
   </si>
   <si>
     <t>meters per second to a kph</t>
+  </si>
+  <si>
+    <t>O,ohm</t>
+  </si>
+  <si>
+    <t>VA</t>
+  </si>
+  <si>
+    <t>volt ampere</t>
+  </si>
+  <si>
+    <t>volt ampere reactive</t>
+  </si>
+  <si>
+    <t>1 volt ampere (measures apparent power)</t>
+  </si>
+  <si>
+    <t>var</t>
+  </si>
+  <si>
+    <t>1 volt ampere-reactive (measures reactive power)</t>
+  </si>
+  <si>
+    <t>kVA</t>
+  </si>
+  <si>
+    <t>kilovolt ampere</t>
+  </si>
+  <si>
+    <t>VA to kVA</t>
   </si>
 </sst>
 </file>
@@ -1724,11 +1751,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:N158"/>
+  <dimension ref="A1:N161"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A146" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="M162" sqref="M162"/>
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="G19" sqref="G19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1750,10 +1777,10 @@
   <sheetData>
     <row r="1" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="B1" t="s">
-        <v>346</v>
+        <v>345</v>
       </c>
       <c r="C1" t="s">
         <v>1</v>
@@ -1786,15 +1813,15 @@
         <v>18</v>
       </c>
       <c r="M1" t="s">
-        <v>434</v>
+        <v>433</v>
       </c>
       <c r="N1" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
     </row>
     <row r="2" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="B2" t="s">
         <v>2</v>
@@ -1833,12 +1860,12 @@
         <v>1</v>
       </c>
       <c r="N2" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
     </row>
     <row r="3" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="B3" t="s">
         <v>3</v>
@@ -1877,18 +1904,18 @@
         <v>1</v>
       </c>
       <c r="N3" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
     </row>
     <row r="4" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="B4" t="s">
+        <v>113</v>
+      </c>
+      <c r="C4" t="s">
         <v>114</v>
-      </c>
-      <c r="C4" t="s">
-        <v>115</v>
       </c>
       <c r="D4">
         <v>0</v>
@@ -1921,12 +1948,12 @@
         <v>1E-3</v>
       </c>
       <c r="N4" t="s">
-        <v>432</v>
+        <v>431</v>
       </c>
     </row>
     <row r="5" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="B5" t="s">
         <v>5</v>
@@ -1965,12 +1992,12 @@
         <v>1</v>
       </c>
       <c r="N5" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
     </row>
     <row r="6" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="B6" t="s">
         <v>6</v>
@@ -2009,12 +2036,12 @@
         <v>1</v>
       </c>
       <c r="N6" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
     </row>
     <row r="7" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="B7" t="s">
         <v>7</v>
@@ -2053,12 +2080,12 @@
         <v>1</v>
       </c>
       <c r="N7" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
     </row>
     <row r="8" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="B8" t="s">
         <v>8</v>
@@ -2097,12 +2124,12 @@
         <v>1</v>
       </c>
       <c r="N8" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
     </row>
     <row r="9" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="B9" t="s">
         <v>15</v>
@@ -2141,12 +2168,12 @@
         <v>1</v>
       </c>
       <c r="N9" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
     </row>
     <row r="10" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="B10" t="s">
         <v>18</v>
@@ -2185,12 +2212,12 @@
         <v>1</v>
       </c>
       <c r="N10" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
     </row>
     <row r="11" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="B11" t="s">
         <v>19</v>
@@ -2229,12 +2256,12 @@
         <v>1</v>
       </c>
       <c r="N11" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
     </row>
     <row r="12" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="B12" t="s">
         <v>21</v>
@@ -2273,18 +2300,18 @@
         <v>1</v>
       </c>
       <c r="N12" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
     </row>
     <row r="13" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="B13" t="s">
         <v>23</v>
       </c>
       <c r="C13" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="D13">
         <v>-2</v>
@@ -2317,18 +2344,18 @@
         <v>1</v>
       </c>
       <c r="N13" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
     </row>
     <row r="14" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="B14" t="s">
         <v>24</v>
       </c>
       <c r="C14" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="D14">
         <v>-2</v>
@@ -2361,18 +2388,18 @@
         <v>1</v>
       </c>
       <c r="N14" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
     </row>
     <row r="15" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="B15" t="s">
         <v>25</v>
       </c>
       <c r="C15" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="D15">
         <v>-3</v>
@@ -2405,18 +2432,18 @@
         <v>1</v>
       </c>
       <c r="N15" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
     </row>
     <row r="16" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="B16" t="s">
         <v>27</v>
       </c>
       <c r="C16" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="D16">
         <v>1</v>
@@ -2449,18 +2476,18 @@
         <v>1</v>
       </c>
       <c r="N16" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
     </row>
     <row r="17" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="B17" t="s">
         <v>26</v>
       </c>
       <c r="C17" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="D17">
         <v>-3</v>
@@ -2493,18 +2520,18 @@
         <v>1</v>
       </c>
       <c r="N17" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
     </row>
     <row r="18" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="B18" t="s">
         <v>28</v>
       </c>
       <c r="C18" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="D18">
         <v>4</v>
@@ -2537,18 +2564,18 @@
         <v>1</v>
       </c>
       <c r="N18" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
     </row>
     <row r="19" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="B19" t="s">
-        <v>29</v>
+        <v>440</v>
       </c>
       <c r="C19" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="D19">
         <v>-3</v>
@@ -2581,18 +2608,18 @@
         <v>1</v>
       </c>
       <c r="N19" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
     </row>
     <row r="20" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="B20" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="C20" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="D20">
         <v>3</v>
@@ -2625,18 +2652,18 @@
         <v>1</v>
       </c>
       <c r="N20" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
     </row>
     <row r="21" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="B21" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C21" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="D21">
         <v>-2</v>
@@ -2669,18 +2696,18 @@
         <v>1</v>
       </c>
       <c r="N21" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
     </row>
     <row r="22" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="B22" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C22" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="D22">
         <v>-2</v>
@@ -2713,18 +2740,18 @@
         <v>1</v>
       </c>
       <c r="N22" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
     </row>
     <row r="23" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="B23" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="C23" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="D23">
         <v>-2</v>
@@ -2757,18 +2784,18 @@
         <v>1</v>
       </c>
       <c r="N23" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
     </row>
     <row r="24" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="B24" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="C24" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="D24">
         <v>0</v>
@@ -2801,18 +2828,18 @@
         <v>1</v>
       </c>
       <c r="N24" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
     </row>
     <row r="25" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="B25" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="C25" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="D25">
         <v>0</v>
@@ -2845,18 +2872,18 @@
         <v>1</v>
       </c>
       <c r="N25" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
     </row>
     <row r="26" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="B26" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="C26" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="D26">
         <v>0</v>
@@ -2889,18 +2916,18 @@
         <v>1</v>
       </c>
       <c r="N26" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
     </row>
     <row r="27" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="B27" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="C27" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="D27">
         <v>-1</v>
@@ -2933,18 +2960,18 @@
         <v>1</v>
       </c>
       <c r="N27" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
     </row>
     <row r="28" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="B28" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="C28" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="D28">
         <v>-2</v>
@@ -2977,18 +3004,18 @@
         <v>1</v>
       </c>
       <c r="N28" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
     </row>
     <row r="29" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A29" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="B29" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="C29" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="D29">
         <v>-2</v>
@@ -3021,18 +3048,18 @@
         <v>1</v>
       </c>
       <c r="N29" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
     </row>
     <row r="30" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A30" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="B30" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="C30" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="D30">
         <v>-1</v>
@@ -3065,18 +3092,18 @@
         <v>1</v>
       </c>
       <c r="N30" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
     </row>
     <row r="31" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A31" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="B31" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="C31" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="D31">
         <v>1</v>
@@ -3110,18 +3137,18 @@
         <v>60</v>
       </c>
       <c r="N31" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
     </row>
     <row r="32" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A32" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="B32" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="C32" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="D32">
         <v>1</v>
@@ -3155,18 +3182,18 @@
         <v>3600</v>
       </c>
       <c r="N32" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
     </row>
     <row r="33" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A33" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="B33" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="C33" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="D33">
         <v>1</v>
@@ -3200,18 +3227,18 @@
         <v>86400</v>
       </c>
       <c r="N33" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
     </row>
     <row r="34" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A34" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="B34" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="C34" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="D34">
         <v>0</v>
@@ -3244,18 +3271,18 @@
         <v>149597870700</v>
       </c>
       <c r="N34" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
     </row>
     <row r="35" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A35" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="B35" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
       <c r="C35" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
       <c r="D35">
         <v>0</v>
@@ -3289,18 +3316,18 @@
         <v>9460750000000000</v>
       </c>
       <c r="N35" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
     </row>
     <row r="36" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A36" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="B36" t="s">
+        <v>241</v>
+      </c>
+      <c r="C36" t="s">
         <v>242</v>
-      </c>
-      <c r="C36" t="s">
-        <v>243</v>
       </c>
       <c r="D36">
         <v>0</v>
@@ -3334,18 +3361,18 @@
         <v>3.0856775814671916E+16</v>
       </c>
       <c r="N36" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
     </row>
     <row r="37" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A37" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="B37" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="C37" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="D37">
         <v>0</v>
@@ -3379,18 +3406,18 @@
         <v>1.7453292519943295E-2</v>
       </c>
       <c r="N37" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
     </row>
     <row r="38" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A38" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="B38" s="1" t="s">
-        <v>338</v>
+        <v>337</v>
       </c>
       <c r="C38" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="D38">
         <v>0</v>
@@ -3424,18 +3451,18 @@
         <v>2.9088820866572158E-4</v>
       </c>
       <c r="N38" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
     </row>
     <row r="39" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A39" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="B39" t="s">
-        <v>339</v>
+        <v>338</v>
       </c>
       <c r="C39" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="D39">
         <v>0</v>
@@ -3469,18 +3496,18 @@
         <v>4.8481368110953598E-6</v>
       </c>
       <c r="N39" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
     </row>
     <row r="40" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A40" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="B40" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="C40" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="D40">
         <v>0</v>
@@ -3514,18 +3541,18 @@
         <v>10000</v>
       </c>
       <c r="N40" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
     </row>
     <row r="41" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A41" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="B41" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="C41" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="D41">
         <v>0</v>
@@ -3558,18 +3585,18 @@
         <v>1E-3</v>
       </c>
       <c r="N41" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
     </row>
     <row r="42" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A42" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="B42" t="s">
+        <v>427</v>
+      </c>
+      <c r="C42" t="s">
         <v>428</v>
-      </c>
-      <c r="C42" t="s">
-        <v>429</v>
       </c>
       <c r="D42">
         <v>0</v>
@@ -3603,18 +3630,18 @@
         <v>9.9999999999999995E-7</v>
       </c>
       <c r="N42" t="s">
-        <v>430</v>
+        <v>429</v>
       </c>
     </row>
     <row r="43" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A43" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="B43" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="C43" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="D43">
         <v>0</v>
@@ -3647,18 +3674,18 @@
         <v>1000</v>
       </c>
       <c r="N43" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
     </row>
     <row r="44" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A44" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="B44" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="C44" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="D44">
         <v>0</v>
@@ -3692,18 +3719,18 @@
         <v>1.6605390666E-27</v>
       </c>
       <c r="N44" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
     </row>
     <row r="45" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A45" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="B45" t="s">
+        <v>359</v>
+      </c>
+      <c r="C45" t="s">
         <v>360</v>
-      </c>
-      <c r="C45" t="s">
-        <v>361</v>
       </c>
       <c r="D45">
         <v>-2</v>
@@ -3736,18 +3763,18 @@
         <v>1.0000000000000001E-5</v>
       </c>
       <c r="N45" t="s">
-        <v>362</v>
+        <v>361</v>
       </c>
     </row>
     <row r="46" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A46" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="B46" t="s">
+        <v>289</v>
+      </c>
+      <c r="C46" t="s">
         <v>290</v>
-      </c>
-      <c r="C46" t="s">
-        <v>291</v>
       </c>
       <c r="D46">
         <v>-2</v>
@@ -3781,18 +3808,18 @@
         <v>9.8066499999999994</v>
       </c>
       <c r="N46" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
     </row>
     <row r="47" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A47" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="B47" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="C47" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="D47">
         <v>-2</v>
@@ -3826,18 +3853,18 @@
         <v>100</v>
       </c>
       <c r="N47" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
     </row>
     <row r="48" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A48" t="s">
+        <v>216</v>
+      </c>
+      <c r="B48" t="s">
         <v>217</v>
       </c>
-      <c r="B48" t="s">
-        <v>218</v>
-      </c>
       <c r="C48" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="D48">
         <v>-2</v>
@@ -3871,18 +3898,18 @@
         <v>100000</v>
       </c>
       <c r="N48" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
     </row>
     <row r="49" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A49" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="B49" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="C49" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="D49">
         <v>-2</v>
@@ -3916,18 +3943,18 @@
         <v>1000000</v>
       </c>
       <c r="N49" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
     </row>
     <row r="50" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A50" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="B50" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="C50" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="D50">
         <v>-2</v>
@@ -3961,18 +3988,18 @@
         <v>1.6021766340000001E-19</v>
       </c>
       <c r="N50" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
     </row>
     <row r="51" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A51" t="s">
+        <v>225</v>
+      </c>
+      <c r="B51" t="s">
         <v>226</v>
       </c>
-      <c r="B51" t="s">
+      <c r="C51" t="s">
         <v>227</v>
-      </c>
-      <c r="C51" t="s">
-        <v>228</v>
       </c>
       <c r="D51">
         <v>-2</v>
@@ -4005,18 +4032,18 @@
         <v>101325</v>
       </c>
       <c r="N51" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
     </row>
     <row r="52" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A52" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="B52" t="s">
+        <v>228</v>
+      </c>
+      <c r="C52" t="s">
         <v>229</v>
-      </c>
-      <c r="C52" t="s">
-        <v>230</v>
       </c>
       <c r="D52">
         <v>-2</v>
@@ -4049,18 +4076,18 @@
         <v>133.32238741500001</v>
       </c>
       <c r="N52" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
     </row>
     <row r="53" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A53" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="B53" t="s">
+        <v>237</v>
+      </c>
+      <c r="C53" t="s">
         <v>238</v>
-      </c>
-      <c r="C53" t="s">
-        <v>239</v>
       </c>
       <c r="D53">
         <v>-2</v>
@@ -4094,18 +4121,18 @@
         <v>3386.3886403410002</v>
       </c>
       <c r="N53" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
     </row>
     <row r="54" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A54" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="B54" t="s">
+        <v>234</v>
+      </c>
+      <c r="C54" t="s">
         <v>235</v>
-      </c>
-      <c r="C54" t="s">
-        <v>236</v>
       </c>
       <c r="D54">
         <v>-2</v>
@@ -4139,18 +4166,18 @@
         <v>0.13332236842105263</v>
       </c>
       <c r="N54" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
     </row>
     <row r="55" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A55" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="B55" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="C55" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="D55">
         <v>-2</v>
@@ -4184,18 +4211,18 @@
         <v>133.32236842105263</v>
       </c>
       <c r="N55" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
     </row>
     <row r="56" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A56" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="B56" t="s">
-        <v>366</v>
+        <v>365</v>
       </c>
       <c r="C56" t="s">
-        <v>369</v>
+        <v>368</v>
       </c>
       <c r="D56">
         <v>-1</v>
@@ -4229,18 +4256,18 @@
         <v>6.2831853071795862</v>
       </c>
       <c r="N56" t="s">
-        <v>370</v>
+        <v>369</v>
       </c>
     </row>
     <row r="57" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A57" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="B57" t="s">
+        <v>366</v>
+      </c>
+      <c r="C57" t="s">
         <v>367</v>
-      </c>
-      <c r="C57" t="s">
-        <v>368</v>
       </c>
       <c r="D57">
         <v>-1</v>
@@ -4274,18 +4301,18 @@
         <v>0.10471975511965977</v>
       </c>
       <c r="N57" t="s">
-        <v>371</v>
+        <v>370</v>
       </c>
     </row>
     <row r="58" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A58" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="B58" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="C58" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="D58">
         <v>0</v>
@@ -4319,18 +4346,18 @@
         <v>2.5399999999999997E-5</v>
       </c>
       <c r="N58" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
     </row>
     <row r="59" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A59" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="B59" t="s">
-        <v>340</v>
+        <v>339</v>
       </c>
       <c r="C59" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="D59">
         <v>0</v>
@@ -4364,18 +4391,18 @@
         <v>2.5399999999999999E-2</v>
       </c>
       <c r="N59" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
     </row>
     <row r="60" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A60" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="B60" t="s">
-        <v>347</v>
+        <v>346</v>
       </c>
       <c r="C60" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="D60">
         <v>0</v>
@@ -4409,18 +4436,18 @@
         <v>0.10159999999999998</v>
       </c>
       <c r="N60" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
     </row>
     <row r="61" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A61" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="B61" t="s">
-        <v>341</v>
+        <v>340</v>
       </c>
       <c r="C61" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="D61">
         <v>0</v>
@@ -4454,18 +4481,18 @@
         <v>0.30479999999999996</v>
       </c>
       <c r="N61" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
     </row>
     <row r="62" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A62" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="B62" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="C62" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="D62">
         <v>0</v>
@@ -4499,18 +4526,18 @@
         <v>0.91439999999999988</v>
       </c>
       <c r="N62" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
     </row>
     <row r="63" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A63" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="B63" t="s">
+        <v>65</v>
+      </c>
+      <c r="C63" t="s">
         <v>66</v>
-      </c>
-      <c r="C63" t="s">
-        <v>67</v>
       </c>
       <c r="D63">
         <v>0</v>
@@ -4544,18 +4571,18 @@
         <v>20.116799999999998</v>
       </c>
       <c r="N63" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
     </row>
     <row r="64" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A64" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="B64" t="s">
+        <v>67</v>
+      </c>
+      <c r="C64" t="s">
         <v>68</v>
-      </c>
-      <c r="C64" t="s">
-        <v>69</v>
       </c>
       <c r="D64">
         <v>0</v>
@@ -4589,18 +4616,18 @@
         <v>201.16799999999998</v>
       </c>
       <c r="N64" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
     </row>
     <row r="65" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A65" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="B65" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="C65" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="D65">
         <v>0</v>
@@ -4634,18 +4661,18 @@
         <v>1609.3439999999998</v>
       </c>
       <c r="N65" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
     </row>
     <row r="66" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A66" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="B66" t="s">
+        <v>70</v>
+      </c>
+      <c r="C66" t="s">
         <v>71</v>
-      </c>
-      <c r="C66" t="s">
-        <v>72</v>
       </c>
       <c r="D66">
         <v>0</v>
@@ -4679,18 +4706,18 @@
         <v>4828.0319999999992</v>
       </c>
       <c r="N66" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
     </row>
     <row r="67" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A67" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="B67" t="s">
+        <v>72</v>
+      </c>
+      <c r="C67" t="s">
         <v>73</v>
-      </c>
-      <c r="C67" t="s">
-        <v>74</v>
       </c>
       <c r="D67">
         <v>0</v>
@@ -4724,18 +4751,18 @@
         <v>1.8520000000000001</v>
       </c>
       <c r="N67" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
     </row>
     <row r="68" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A68" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="B68" t="s">
-        <v>359</v>
+        <v>358</v>
       </c>
       <c r="C68" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="D68">
         <v>0</v>
@@ -4769,18 +4796,18 @@
         <v>1852</v>
       </c>
       <c r="N68" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
     </row>
     <row r="69" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A69" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="B69" t="s">
+        <v>127</v>
+      </c>
+      <c r="C69" t="s">
         <v>128</v>
-      </c>
-      <c r="C69" t="s">
-        <v>129</v>
       </c>
       <c r="D69">
         <v>-1</v>
@@ -4814,18 +4841,18 @@
         <v>0.51444444444444448</v>
       </c>
       <c r="N69" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
     </row>
     <row r="70" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A70" t="s">
+        <v>76</v>
+      </c>
+      <c r="B70" t="s">
         <v>77</v>
       </c>
-      <c r="B70" t="s">
+      <c r="C70" t="s">
         <v>78</v>
-      </c>
-      <c r="C70" t="s">
-        <v>79</v>
       </c>
       <c r="D70">
         <v>0</v>
@@ -4859,18 +4886,18 @@
         <v>2.8413062500000005E-5</v>
       </c>
       <c r="N70" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
     </row>
     <row r="71" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A71" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="B71" t="s">
-        <v>330</v>
+        <v>329</v>
       </c>
       <c r="C71" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="D71">
         <v>0</v>
@@ -4904,18 +4931,18 @@
         <v>1.4206531250000003E-4</v>
       </c>
       <c r="N71" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
     </row>
     <row r="72" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A72" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="B72" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
       <c r="C72" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
       <c r="D72">
         <v>0</v>
@@ -4949,18 +4976,18 @@
         <v>2.8413062500000006E-4</v>
       </c>
       <c r="N72" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
     </row>
     <row r="73" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A73" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="B73" t="s">
-        <v>331</v>
+        <v>330</v>
       </c>
       <c r="C73" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="D73">
         <v>0</v>
@@ -4994,18 +5021,18 @@
         <v>5.6826125000000011E-4</v>
       </c>
       <c r="N73" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
     </row>
     <row r="74" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A74" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="B74" t="s">
-        <v>332</v>
+        <v>331</v>
       </c>
       <c r="C74" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="D74">
         <v>0</v>
@@ -5039,18 +5066,18 @@
         <v>1.1365225000000002E-3</v>
       </c>
       <c r="N74" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
     </row>
     <row r="75" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A75" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="B75" t="s">
-        <v>333</v>
+        <v>332</v>
       </c>
       <c r="C75" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="D75">
         <v>0</v>
@@ -5084,18 +5111,18 @@
         <v>4.5460900000000009E-3</v>
       </c>
       <c r="N75" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
     </row>
     <row r="76" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A76" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="B76" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
       <c r="C76" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
       <c r="D76">
         <v>0</v>
@@ -5129,18 +5156,18 @@
         <v>9.0921800000000018E-3</v>
       </c>
       <c r="N76" t="s">
-        <v>357</v>
+        <v>356</v>
       </c>
     </row>
     <row r="77" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A77" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="B77" t="s">
-        <v>356</v>
+        <v>355</v>
       </c>
       <c r="C77" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
       <c r="D77">
         <v>0</v>
@@ -5174,18 +5201,18 @@
         <v>3.6368720000000007E-2</v>
       </c>
       <c r="N77" t="s">
-        <v>358</v>
+        <v>357</v>
       </c>
     </row>
     <row r="78" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A78" t="s">
-        <v>431</v>
+        <v>430</v>
       </c>
       <c r="B78" t="s">
+        <v>269</v>
+      </c>
+      <c r="C78" t="s">
         <v>270</v>
-      </c>
-      <c r="C78" t="s">
-        <v>271</v>
       </c>
       <c r="D78">
         <v>0</v>
@@ -5219,18 +5246,18 @@
         <v>4.9289215937500005E-6</v>
       </c>
       <c r="N78" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
     </row>
     <row r="79" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A79" t="s">
-        <v>431</v>
+        <v>430</v>
       </c>
       <c r="B79" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
       <c r="C79" t="s">
-        <v>272</v>
+        <v>271</v>
       </c>
       <c r="D79">
         <v>0</v>
@@ -5264,18 +5291,18 @@
         <v>1.4786764781250001E-5</v>
       </c>
       <c r="N79" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
     </row>
     <row r="80" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A80" t="s">
-        <v>431</v>
+        <v>430</v>
       </c>
       <c r="B80" t="s">
+        <v>352</v>
+      </c>
+      <c r="C80" t="s">
         <v>353</v>
-      </c>
-      <c r="C80" t="s">
-        <v>354</v>
       </c>
       <c r="D80">
         <v>0</v>
@@ -5309,18 +5336,18 @@
         <v>3.6966911953125001E-6</v>
       </c>
       <c r="N80" t="s">
-        <v>355</v>
+        <v>354</v>
       </c>
     </row>
     <row r="81" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A81" t="s">
-        <v>431</v>
+        <v>430</v>
       </c>
       <c r="B81" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="C81" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
       <c r="D81">
         <v>0</v>
@@ -5354,18 +5381,18 @@
         <v>2.9573529562500001E-5</v>
       </c>
       <c r="N81" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
     </row>
     <row r="82" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A82" t="s">
-        <v>431</v>
+        <v>430</v>
       </c>
       <c r="B82" t="s">
-        <v>330</v>
+        <v>329</v>
       </c>
       <c r="C82" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
       <c r="D82">
         <v>0</v>
@@ -5399,18 +5426,18 @@
         <v>9.4635294600000004E-4</v>
       </c>
       <c r="N82" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
     </row>
     <row r="83" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A83" t="s">
-        <v>431</v>
+        <v>430</v>
       </c>
       <c r="B83" t="s">
-        <v>331</v>
+        <v>330</v>
       </c>
       <c r="C83" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
       <c r="D83">
         <v>0</v>
@@ -5444,18 +5471,18 @@
         <v>4.7317647300000002E-4</v>
       </c>
       <c r="N83" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
     </row>
     <row r="84" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A84" t="s">
-        <v>431</v>
+        <v>430</v>
       </c>
       <c r="B84" t="s">
-        <v>332</v>
+        <v>331</v>
       </c>
       <c r="C84" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="D84">
         <v>0</v>
@@ -5489,18 +5516,18 @@
         <v>9.4635294600000004E-4</v>
       </c>
       <c r="N84" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
     </row>
     <row r="85" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A85" t="s">
-        <v>431</v>
+        <v>430</v>
       </c>
       <c r="B85" t="s">
-        <v>334</v>
+        <v>333</v>
       </c>
       <c r="C85" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
       <c r="D85">
         <v>0</v>
@@ -5534,18 +5561,18 @@
         <v>1.8927058920000001E-3</v>
       </c>
       <c r="N85" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
     </row>
     <row r="86" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A86" t="s">
-        <v>431</v>
+        <v>430</v>
       </c>
       <c r="B86" t="s">
-        <v>333</v>
+        <v>332</v>
       </c>
       <c r="C86" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
       <c r="D86">
         <v>0</v>
@@ -5579,18 +5606,18 @@
         <v>3.7854117840000001E-3</v>
       </c>
       <c r="N86" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
     </row>
     <row r="87" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A87" t="s">
-        <v>431</v>
+        <v>430</v>
       </c>
       <c r="B87" t="s">
-        <v>348</v>
+        <v>347</v>
       </c>
       <c r="C87" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
       <c r="D87">
         <v>0</v>
@@ -5624,18 +5651,18 @@
         <v>5.506104713575E-4</v>
       </c>
       <c r="N87" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
     </row>
     <row r="88" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A88" t="s">
-        <v>431</v>
+        <v>430</v>
       </c>
       <c r="B88" t="s">
-        <v>349</v>
+        <v>348</v>
       </c>
       <c r="C88" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
       <c r="D88">
         <v>0</v>
@@ -5669,18 +5696,18 @@
         <v>1.101220942715E-3</v>
       </c>
       <c r="N88" t="s">
-        <v>283</v>
+        <v>282</v>
       </c>
     </row>
     <row r="89" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A89" t="s">
-        <v>431</v>
+        <v>430</v>
       </c>
       <c r="B89" t="s">
-        <v>350</v>
+        <v>349</v>
       </c>
       <c r="C89" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
       <c r="D89">
         <v>0</v>
@@ -5714,18 +5741,18 @@
         <v>4.40488377086E-3</v>
       </c>
       <c r="N89" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
     </row>
     <row r="90" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A90" t="s">
-        <v>431</v>
+        <v>430</v>
       </c>
       <c r="B90" t="s">
+        <v>350</v>
+      </c>
+      <c r="C90" t="s">
         <v>351</v>
-      </c>
-      <c r="C90" t="s">
-        <v>352</v>
       </c>
       <c r="D90">
         <v>0</v>
@@ -5759,18 +5786,18 @@
         <v>8.8097675417200001E-3</v>
       </c>
       <c r="N90" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
     </row>
     <row r="91" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A91" t="s">
-        <v>431</v>
+        <v>430</v>
       </c>
       <c r="B91" t="s">
-        <v>356</v>
+        <v>355</v>
       </c>
       <c r="C91" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
       <c r="D91">
         <v>0</v>
@@ -5804,18 +5831,18 @@
         <v>3.523907016688E-2</v>
       </c>
       <c r="N91" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
     </row>
     <row r="92" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A92" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="B92" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="C92" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="D92">
         <v>0</v>
@@ -5849,18 +5876,18 @@
         <v>6.4798910000000008E-5</v>
       </c>
       <c r="N92" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
     </row>
     <row r="93" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A93" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="B93" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="C93" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="D93">
         <v>0</v>
@@ -5894,18 +5921,18 @@
         <v>1.7718451953125001E-3</v>
       </c>
       <c r="N93" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
     </row>
     <row r="94" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A94" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="B94" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="C94" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="D94">
         <v>0</v>
@@ -5939,18 +5966,18 @@
         <v>2.8349523125000001E-2</v>
       </c>
       <c r="N94" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
     </row>
     <row r="95" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A95" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="B95" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="C95" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="D95">
         <v>0</v>
@@ -5984,18 +6011,18 @@
         <v>0.45359237000000002</v>
       </c>
       <c r="N95" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
     </row>
     <row r="96" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A96" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="B96" t="s">
+        <v>91</v>
+      </c>
+      <c r="C96" t="s">
         <v>92</v>
-      </c>
-      <c r="C96" t="s">
-        <v>93</v>
       </c>
       <c r="D96">
         <v>0</v>
@@ -6029,18 +6056,18 @@
         <v>6.3502931800000004</v>
       </c>
       <c r="N96" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
     </row>
     <row r="97" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A97" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="B97" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="C97" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="D97">
         <v>0</v>
@@ -6074,18 +6101,18 @@
         <v>12.700586360000001</v>
       </c>
       <c r="N97" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
     </row>
     <row r="98" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A98" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="B98" t="s">
-        <v>345</v>
+        <v>344</v>
       </c>
       <c r="C98" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
       <c r="D98">
         <v>0</v>
@@ -6119,18 +6146,18 @@
         <v>50.802345440000003</v>
       </c>
       <c r="N98" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
     </row>
     <row r="99" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A99" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="B99" t="s">
-        <v>344</v>
+        <v>343</v>
       </c>
       <c r="C99" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="D99">
         <v>0</v>
@@ -6164,18 +6191,18 @@
         <v>1016.0469088000001</v>
       </c>
       <c r="N99" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
     </row>
     <row r="100" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A100" t="s">
-        <v>431</v>
+        <v>430</v>
       </c>
       <c r="B100" t="s">
-        <v>343</v>
+        <v>342</v>
       </c>
       <c r="C100" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
       <c r="D100">
         <v>0</v>
@@ -6209,18 +6236,18 @@
         <v>45.359237</v>
       </c>
       <c r="N100" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
     </row>
     <row r="101" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A101" t="s">
-        <v>431</v>
+        <v>430</v>
       </c>
       <c r="B101" t="s">
-        <v>342</v>
+        <v>341</v>
       </c>
       <c r="C101" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="D101">
         <v>0</v>
@@ -6254,18 +6281,18 @@
         <v>907.18474000000003</v>
       </c>
       <c r="N101" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
     </row>
     <row r="102" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A102" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="B102" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="C102" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="D102">
         <v>0</v>
@@ -6299,18 +6326,18 @@
         <v>14.593902937206368</v>
       </c>
       <c r="N102" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
     </row>
     <row r="103" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A103" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="B103" t="s">
+        <v>133</v>
+      </c>
+      <c r="C103" t="s">
         <v>134</v>
-      </c>
-      <c r="C103" t="s">
-        <v>135</v>
       </c>
       <c r="D103">
         <v>-2</v>
@@ -6344,18 +6371,18 @@
         <v>4.4482216152604996</v>
       </c>
       <c r="N103" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
     </row>
     <row r="104" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A104" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="B104" t="s">
+        <v>213</v>
+      </c>
+      <c r="C104" t="s">
         <v>214</v>
-      </c>
-      <c r="C104" t="s">
-        <v>215</v>
       </c>
       <c r="D104">
         <v>-2</v>
@@ -6389,18 +6416,18 @@
         <v>6894.7572931683608</v>
       </c>
       <c r="N104" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
     </row>
     <row r="105" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A105" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="B105" t="s">
+        <v>119</v>
+      </c>
+      <c r="C105" t="s">
         <v>120</v>
-      </c>
-      <c r="C105" t="s">
-        <v>121</v>
       </c>
       <c r="D105">
         <v>-3</v>
@@ -6434,18 +6461,18 @@
         <v>745.69987158227002</v>
       </c>
       <c r="N105" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
     </row>
     <row r="106" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A106" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="B106" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="C106" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="D106">
         <v>0</v>
@@ -6479,18 +6506,18 @@
         <v>0.55555555555555558</v>
       </c>
       <c r="N106" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
     </row>
     <row r="107" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A107" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="B107" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="C107" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="D107">
         <v>0</v>
@@ -6524,18 +6551,18 @@
         <v>0.55555555555555558</v>
       </c>
       <c r="N107" t="s">
-        <v>433</v>
+        <v>432</v>
       </c>
     </row>
     <row r="108" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A108" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="B108" t="s">
-        <v>335</v>
+        <v>334</v>
       </c>
       <c r="C108" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="D108">
         <v>-2</v>
@@ -6568,18 +6595,18 @@
         <v>4.1840000000000002</v>
       </c>
       <c r="N108" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
     </row>
     <row r="109" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A109" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="B109" t="s">
-        <v>336</v>
+        <v>335</v>
       </c>
       <c r="C109" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="D109">
         <v>-2</v>
@@ -6613,18 +6640,18 @@
         <v>4184</v>
       </c>
       <c r="N109" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
     </row>
     <row r="110" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A110" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="B110" t="s">
-        <v>363</v>
+        <v>362</v>
       </c>
       <c r="C110" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="D110">
         <v>-2</v>
@@ -6658,18 +6685,18 @@
         <v>4.1867999999999999</v>
       </c>
       <c r="N110" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
     </row>
     <row r="111" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A111" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="B111" t="s">
-        <v>364</v>
+        <v>363</v>
       </c>
       <c r="C111" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="D111">
         <v>-2</v>
@@ -6703,18 +6730,18 @@
         <v>4186.8</v>
       </c>
       <c r="N111" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
     </row>
     <row r="112" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A112" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="B112" t="s">
-        <v>337</v>
+        <v>336</v>
       </c>
       <c r="C112" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="D112">
         <v>-2</v>
@@ -6748,18 +6775,18 @@
         <v>1054.350264488889</v>
       </c>
       <c r="N112" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
     </row>
     <row r="113" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A113" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="B113" t="s">
-        <v>365</v>
+        <v>364</v>
       </c>
       <c r="C113" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="D113">
         <v>-2</v>
@@ -6793,18 +6820,18 @@
         <v>1055.05585262</v>
       </c>
       <c r="N113" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
     </row>
     <row r="114" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A114" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="B114" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="C114" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="D114">
         <v>-2</v>
@@ -6838,18 +6865,18 @@
         <v>105505585.26199999</v>
       </c>
       <c r="N114" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
     </row>
     <row r="115" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A115" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="B115" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="C115" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="D115">
         <v>-2</v>
@@ -6883,15 +6910,15 @@
         <v>1.05505585262E+18</v>
       </c>
       <c r="N115" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
     </row>
     <row r="116" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A116" t="s">
-        <v>372</v>
+        <v>371</v>
       </c>
       <c r="B116" t="s">
-        <v>375</v>
+        <v>374</v>
       </c>
       <c r="M116">
         <v>0</v>
@@ -6899,10 +6926,10 @@
     </row>
     <row r="117" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A117" t="s">
-        <v>372</v>
+        <v>371</v>
       </c>
       <c r="B117" t="s">
-        <v>324</v>
+        <v>323</v>
       </c>
       <c r="M117">
         <v>0</v>
@@ -6910,10 +6937,10 @@
     </row>
     <row r="118" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A118" t="s">
-        <v>372</v>
+        <v>371</v>
       </c>
       <c r="B118" t="s">
-        <v>376</v>
+        <v>375</v>
       </c>
       <c r="M118">
         <v>0</v>
@@ -6921,24 +6948,24 @@
     </row>
     <row r="119" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A119" t="s">
-        <v>372</v>
+        <v>371</v>
       </c>
       <c r="B119" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
       <c r="M119">
         <v>0</v>
       </c>
       <c r="N119" t="s">
-        <v>408</v>
+        <v>407</v>
       </c>
     </row>
     <row r="120" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A120" t="s">
-        <v>372</v>
+        <v>371</v>
       </c>
       <c r="B120" t="s">
-        <v>377</v>
+        <v>376</v>
       </c>
       <c r="M120">
         <v>0</v>
@@ -6946,10 +6973,10 @@
     </row>
     <row r="121" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A121" t="s">
-        <v>372</v>
+        <v>371</v>
       </c>
       <c r="B121" t="s">
-        <v>378</v>
+        <v>377</v>
       </c>
       <c r="M121">
         <v>0</v>
@@ -6957,38 +6984,38 @@
     </row>
     <row r="122" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A122" t="s">
-        <v>372</v>
+        <v>371</v>
       </c>
       <c r="B122" t="s">
-        <v>379</v>
+        <v>378</v>
       </c>
       <c r="M122">
         <v>0</v>
       </c>
       <c r="N122" t="s">
-        <v>413</v>
+        <v>412</v>
       </c>
     </row>
     <row r="123" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A123" t="s">
-        <v>372</v>
+        <v>371</v>
       </c>
       <c r="B123" t="s">
-        <v>380</v>
+        <v>379</v>
       </c>
       <c r="M123">
         <v>0</v>
       </c>
       <c r="N123" t="s">
-        <v>409</v>
+        <v>408</v>
       </c>
     </row>
     <row r="124" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A124" t="s">
-        <v>372</v>
+        <v>371</v>
       </c>
       <c r="B124" t="s">
-        <v>381</v>
+        <v>380</v>
       </c>
       <c r="D124">
         <v>-3</v>
@@ -7021,68 +7048,68 @@
         <v>-150</v>
       </c>
       <c r="N124" t="s">
-        <v>425</v>
+        <v>424</v>
       </c>
     </row>
     <row r="125" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A125" t="s">
-        <v>372</v>
+        <v>371</v>
       </c>
       <c r="B125" t="s">
-        <v>382</v>
+        <v>381</v>
       </c>
       <c r="M125">
         <v>0</v>
       </c>
       <c r="N125" t="s">
-        <v>410</v>
+        <v>409</v>
       </c>
     </row>
     <row r="126" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A126" t="s">
-        <v>372</v>
+        <v>371</v>
       </c>
       <c r="B126" t="s">
-        <v>302</v>
+        <v>301</v>
       </c>
       <c r="M126">
         <v>0</v>
       </c>
       <c r="N126" t="s">
-        <v>411</v>
+        <v>410</v>
       </c>
     </row>
     <row r="127" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A127" t="s">
-        <v>372</v>
+        <v>371</v>
       </c>
       <c r="B127" t="s">
-        <v>383</v>
+        <v>382</v>
       </c>
       <c r="M127">
         <v>0</v>
       </c>
       <c r="N127" t="s">
-        <v>412</v>
+        <v>411</v>
       </c>
     </row>
     <row r="128" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A128" t="s">
-        <v>372</v>
+        <v>371</v>
       </c>
       <c r="B128" t="s">
-        <v>384</v>
+        <v>383</v>
       </c>
       <c r="M128">
         <v>0</v>
       </c>
       <c r="N128" t="s">
-        <v>414</v>
+        <v>413</v>
       </c>
     </row>
     <row r="129" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A129" t="s">
-        <v>372</v>
+        <v>371</v>
       </c>
       <c r="B129" t="s">
         <v>24</v>
@@ -7091,15 +7118,15 @@
         <v>0</v>
       </c>
       <c r="N129" t="s">
-        <v>415</v>
+        <v>414</v>
       </c>
     </row>
     <row r="130" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A130" t="s">
-        <v>372</v>
+        <v>371</v>
       </c>
       <c r="B130" t="s">
-        <v>385</v>
+        <v>384</v>
       </c>
       <c r="D130">
         <v>-3</v>
@@ -7132,29 +7159,29 @@
         <v>30</v>
       </c>
       <c r="N130" t="s">
-        <v>424</v>
+        <v>423</v>
       </c>
     </row>
     <row r="131" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A131" t="s">
-        <v>372</v>
+        <v>371</v>
       </c>
       <c r="B131" t="s">
-        <v>386</v>
+        <v>385</v>
       </c>
       <c r="M131">
         <v>0</v>
       </c>
       <c r="N131" t="s">
-        <v>416</v>
+        <v>415</v>
       </c>
     </row>
     <row r="132" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A132" t="s">
-        <v>372</v>
+        <v>371</v>
       </c>
       <c r="B132" t="s">
-        <v>387</v>
+        <v>386</v>
       </c>
       <c r="D132">
         <v>-3</v>
@@ -7187,15 +7214,15 @@
         <v>-30</v>
       </c>
       <c r="N132" t="s">
-        <v>426</v>
+        <v>425</v>
       </c>
     </row>
     <row r="133" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A133" t="s">
-        <v>372</v>
+        <v>371</v>
       </c>
       <c r="B133" t="s">
-        <v>422</v>
+        <v>421</v>
       </c>
       <c r="D133">
         <v>-3</v>
@@ -7227,10 +7254,10 @@
     </row>
     <row r="134" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A134" t="s">
-        <v>372</v>
+        <v>371</v>
       </c>
       <c r="B134" t="s">
-        <v>388</v>
+        <v>387</v>
       </c>
       <c r="M134">
         <v>0</v>
@@ -7238,10 +7265,10 @@
     </row>
     <row r="135" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A135" t="s">
-        <v>372</v>
+        <v>371</v>
       </c>
       <c r="B135" t="s">
-        <v>389</v>
+        <v>388</v>
       </c>
       <c r="D135">
         <v>-3</v>
@@ -7274,15 +7301,15 @@
         <v>0</v>
       </c>
       <c r="N135" t="s">
-        <v>417</v>
+        <v>416</v>
       </c>
     </row>
     <row r="136" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A136" t="s">
-        <v>372</v>
+        <v>371</v>
       </c>
       <c r="B136" t="s">
-        <v>390</v>
+        <v>389</v>
       </c>
       <c r="M136">
         <v>0</v>
@@ -7290,10 +7317,10 @@
     </row>
     <row r="137" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A137" t="s">
-        <v>372</v>
+        <v>371</v>
       </c>
       <c r="B137" t="s">
-        <v>391</v>
+        <v>390</v>
       </c>
       <c r="M137">
         <v>0</v>
@@ -7301,10 +7328,10 @@
     </row>
     <row r="138" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A138" t="s">
-        <v>372</v>
+        <v>371</v>
       </c>
       <c r="B138" t="s">
-        <v>392</v>
+        <v>391</v>
       </c>
       <c r="M138">
         <v>0</v>
@@ -7312,10 +7339,10 @@
     </row>
     <row r="139" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A139" t="s">
-        <v>372</v>
+        <v>371</v>
       </c>
       <c r="B139" t="s">
-        <v>393</v>
+        <v>392</v>
       </c>
       <c r="M139">
         <v>0</v>
@@ -7323,10 +7350,10 @@
     </row>
     <row r="140" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A140" t="s">
-        <v>372</v>
+        <v>371</v>
       </c>
       <c r="B140" t="s">
-        <v>394</v>
+        <v>393</v>
       </c>
       <c r="M140">
         <v>0</v>
@@ -7334,10 +7361,10 @@
     </row>
     <row r="141" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A141" t="s">
-        <v>372</v>
+        <v>371</v>
       </c>
       <c r="B141" t="s">
-        <v>395</v>
+        <v>394</v>
       </c>
       <c r="D141">
         <v>0</v>
@@ -7372,10 +7399,10 @@
     </row>
     <row r="142" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A142" t="s">
-        <v>372</v>
+        <v>371</v>
       </c>
       <c r="B142" t="s">
-        <v>396</v>
+        <v>395</v>
       </c>
       <c r="M142">
         <v>0</v>
@@ -7383,10 +7410,10 @@
     </row>
     <row r="143" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A143" t="s">
-        <v>372</v>
+        <v>371</v>
       </c>
       <c r="B143" t="s">
-        <v>397</v>
+        <v>396</v>
       </c>
       <c r="D143">
         <v>-3</v>
@@ -7419,15 +7446,15 @@
         <v>0</v>
       </c>
       <c r="N143" t="s">
-        <v>420</v>
+        <v>419</v>
       </c>
     </row>
     <row r="144" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A144" t="s">
-        <v>372</v>
+        <v>371</v>
       </c>
       <c r="B144" t="s">
-        <v>398</v>
+        <v>397</v>
       </c>
       <c r="M144">
         <v>0</v>
@@ -7435,10 +7462,10 @@
     </row>
     <row r="145" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A145" t="s">
-        <v>372</v>
+        <v>371</v>
       </c>
       <c r="B145" t="s">
-        <v>399</v>
+        <v>398</v>
       </c>
       <c r="D145">
         <v>-3</v>
@@ -7471,15 +7498,15 @@
         <v>0</v>
       </c>
       <c r="N145" t="s">
-        <v>423</v>
+        <v>422</v>
       </c>
     </row>
     <row r="146" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A146" t="s">
-        <v>372</v>
+        <v>371</v>
       </c>
       <c r="B146" t="s">
-        <v>400</v>
+        <v>399</v>
       </c>
       <c r="M146">
         <v>0</v>
@@ -7487,24 +7514,24 @@
     </row>
     <row r="147" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A147" t="s">
-        <v>372</v>
+        <v>371</v>
       </c>
       <c r="B147" t="s">
-        <v>401</v>
+        <v>400</v>
       </c>
       <c r="M147">
         <v>0</v>
       </c>
       <c r="N147" t="s">
-        <v>421</v>
+        <v>420</v>
       </c>
     </row>
     <row r="148" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A148" t="s">
-        <v>372</v>
+        <v>371</v>
       </c>
       <c r="B148" t="s">
-        <v>402</v>
+        <v>401</v>
       </c>
       <c r="M148">
         <v>0</v>
@@ -7512,7 +7539,7 @@
     </row>
     <row r="149" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A149" t="s">
-        <v>372</v>
+        <v>371</v>
       </c>
       <c r="B149" t="s">
         <v>25</v>
@@ -7548,15 +7575,15 @@
         <v>0</v>
       </c>
       <c r="N149" t="s">
-        <v>427</v>
+        <v>426</v>
       </c>
     </row>
     <row r="150" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A150" t="s">
-        <v>372</v>
+        <v>371</v>
       </c>
       <c r="B150" t="s">
-        <v>403</v>
+        <v>402</v>
       </c>
       <c r="M150">
         <v>0</v>
@@ -7564,10 +7591,10 @@
     </row>
     <row r="151" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A151" t="s">
-        <v>372</v>
+        <v>371</v>
       </c>
       <c r="B151" t="s">
-        <v>404</v>
+        <v>403</v>
       </c>
       <c r="M151">
         <v>0</v>
@@ -7575,10 +7602,10 @@
     </row>
     <row r="152" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A152" t="s">
-        <v>372</v>
+        <v>371</v>
       </c>
       <c r="B152" t="s">
-        <v>419</v>
+        <v>418</v>
       </c>
       <c r="M152">
         <v>0</v>
@@ -7586,10 +7613,10 @@
     </row>
     <row r="153" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A153" t="s">
-        <v>372</v>
+        <v>371</v>
       </c>
       <c r="B153" t="s">
-        <v>418</v>
+        <v>417</v>
       </c>
       <c r="D153">
         <v>-3</v>
@@ -7624,10 +7651,10 @@
     </row>
     <row r="154" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A154" t="s">
-        <v>372</v>
+        <v>371</v>
       </c>
       <c r="B154" t="s">
-        <v>405</v>
+        <v>404</v>
       </c>
       <c r="D154">
         <v>-1</v>
@@ -7662,10 +7689,10 @@
     </row>
     <row r="155" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A155" t="s">
-        <v>372</v>
+        <v>371</v>
       </c>
       <c r="B155" t="s">
-        <v>406</v>
+        <v>405</v>
       </c>
       <c r="D155">
         <v>0</v>
@@ -7700,10 +7727,10 @@
     </row>
     <row r="156" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A156" t="s">
-        <v>372</v>
+        <v>371</v>
       </c>
       <c r="B156" t="s">
-        <v>407</v>
+        <v>406</v>
       </c>
       <c r="D156">
         <v>0</v>
@@ -7738,13 +7765,13 @@
     </row>
     <row r="157" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A157" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="B157" t="s">
-        <v>437</v>
+        <v>436</v>
       </c>
       <c r="C157" t="s">
-        <v>435</v>
+        <v>434</v>
       </c>
       <c r="D157">
         <v>-1</v>
@@ -7778,18 +7805,18 @@
         <v>0.44703999999999994</v>
       </c>
       <c r="N157" t="s">
-        <v>436</v>
+        <v>435</v>
       </c>
     </row>
     <row r="158" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A158" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="B158" t="s">
+        <v>437</v>
+      </c>
+      <c r="C158" t="s">
         <v>438</v>
-      </c>
-      <c r="C158" t="s">
-        <v>439</v>
       </c>
       <c r="D158">
         <v>-1</v>
@@ -7823,12 +7850,144 @@
         <v>0.27777777777777779</v>
       </c>
       <c r="N158" t="s">
-        <v>440</v>
+        <v>439</v>
+      </c>
+    </row>
+    <row r="159" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A159" t="s">
+        <v>225</v>
+      </c>
+      <c r="B159" t="s">
+        <v>441</v>
+      </c>
+      <c r="C159" t="s">
+        <v>442</v>
+      </c>
+      <c r="D159">
+        <v>-3</v>
+      </c>
+      <c r="E159">
+        <v>2</v>
+      </c>
+      <c r="F159">
+        <v>1</v>
+      </c>
+      <c r="G159">
+        <v>0</v>
+      </c>
+      <c r="H159">
+        <v>0</v>
+      </c>
+      <c r="I159">
+        <v>0</v>
+      </c>
+      <c r="J159">
+        <v>0</v>
+      </c>
+      <c r="K159">
+        <v>0</v>
+      </c>
+      <c r="L159">
+        <v>0</v>
+      </c>
+      <c r="M159">
+        <v>1</v>
+      </c>
+      <c r="N159" t="s">
+        <v>444</v>
+      </c>
+    </row>
+    <row r="160" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A160" t="s">
+        <v>225</v>
+      </c>
+      <c r="B160" t="s">
+        <v>447</v>
+      </c>
+      <c r="C160" t="s">
+        <v>448</v>
+      </c>
+      <c r="D160">
+        <v>-3</v>
+      </c>
+      <c r="E160">
+        <v>2</v>
+      </c>
+      <c r="F160">
+        <v>1</v>
+      </c>
+      <c r="G160">
+        <v>0</v>
+      </c>
+      <c r="H160">
+        <v>0</v>
+      </c>
+      <c r="I160">
+        <v>0</v>
+      </c>
+      <c r="J160">
+        <v>0</v>
+      </c>
+      <c r="K160">
+        <v>0</v>
+      </c>
+      <c r="L160">
+        <v>0</v>
+      </c>
+      <c r="M160">
+        <v>1000</v>
+      </c>
+      <c r="N160" t="s">
+        <v>449</v>
+      </c>
+    </row>
+    <row r="161" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A161" t="s">
+        <v>225</v>
+      </c>
+      <c r="B161" t="s">
+        <v>445</v>
+      </c>
+      <c r="C161" t="s">
+        <v>443</v>
+      </c>
+      <c r="D161">
+        <v>-3</v>
+      </c>
+      <c r="E161">
+        <v>2</v>
+      </c>
+      <c r="F161">
+        <v>1</v>
+      </c>
+      <c r="G161">
+        <v>0</v>
+      </c>
+      <c r="H161">
+        <v>0</v>
+      </c>
+      <c r="I161">
+        <v>0</v>
+      </c>
+      <c r="J161">
+        <v>0</v>
+      </c>
+      <c r="K161">
+        <v>0</v>
+      </c>
+      <c r="L161">
+        <v>0</v>
+      </c>
+      <c r="M161">
+        <v>1</v>
+      </c>
+      <c r="N161" t="s">
+        <v>446</v>
       </c>
     </row>
   </sheetData>
   <conditionalFormatting sqref="D1:L1048576">
-    <cfRule type="colorScale" priority="2">
+    <cfRule type="colorScale" priority="3">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="percentile" val="50"/>
@@ -7856,7 +8015,7 @@
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="B1" t="s">
         <v>0</v>
@@ -7865,18 +8024,18 @@
         <v>1</v>
       </c>
       <c r="D1" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="B2" t="s">
+        <v>292</v>
+      </c>
+      <c r="C2" t="s">
         <v>293</v>
-      </c>
-      <c r="C2" t="s">
-        <v>294</v>
       </c>
       <c r="D2">
         <v>24</v>
@@ -7884,13 +8043,13 @@
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="B3" t="s">
+        <v>294</v>
+      </c>
+      <c r="C3" t="s">
         <v>295</v>
-      </c>
-      <c r="C3" t="s">
-        <v>296</v>
       </c>
       <c r="D3">
         <v>21</v>
@@ -7898,13 +8057,13 @@
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="B4" t="s">
+        <v>296</v>
+      </c>
+      <c r="C4" t="s">
         <v>297</v>
-      </c>
-      <c r="C4" t="s">
-        <v>298</v>
       </c>
       <c r="D4">
         <v>18</v>
@@ -7912,13 +8071,13 @@
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="B5" t="s">
+        <v>298</v>
+      </c>
+      <c r="C5" t="s">
         <v>299</v>
-      </c>
-      <c r="C5" t="s">
-        <v>300</v>
       </c>
       <c r="D5">
         <v>15</v>
@@ -7926,13 +8085,13 @@
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="B6" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C6" t="s">
-        <v>301</v>
+        <v>300</v>
       </c>
       <c r="D6">
         <v>12</v>
@@ -7940,13 +8099,13 @@
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="B7" t="s">
+        <v>301</v>
+      </c>
+      <c r="C7" t="s">
         <v>302</v>
-      </c>
-      <c r="C7" t="s">
-        <v>303</v>
       </c>
       <c r="D7">
         <v>9</v>
@@ -7954,13 +8113,13 @@
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="B8" t="s">
+        <v>303</v>
+      </c>
+      <c r="C8" t="s">
         <v>304</v>
-      </c>
-      <c r="C8" t="s">
-        <v>305</v>
       </c>
       <c r="D8">
         <v>6</v>
@@ -7968,13 +8127,13 @@
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="B9" t="s">
+        <v>305</v>
+      </c>
+      <c r="C9" t="s">
         <v>306</v>
-      </c>
-      <c r="C9" t="s">
-        <v>307</v>
       </c>
       <c r="D9">
         <v>3</v>
@@ -7982,13 +8141,13 @@
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="B10" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="C10" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
       <c r="D10">
         <v>2</v>
@@ -7996,13 +8155,13 @@
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="B11" t="s">
+        <v>308</v>
+      </c>
+      <c r="C11" t="s">
         <v>309</v>
-      </c>
-      <c r="C11" t="s">
-        <v>310</v>
       </c>
       <c r="D11">
         <v>1</v>
@@ -8015,13 +8174,13 @@
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="B13" t="s">
+        <v>310</v>
+      </c>
+      <c r="C13" t="s">
         <v>311</v>
-      </c>
-      <c r="C13" t="s">
-        <v>312</v>
       </c>
       <c r="D13">
         <v>-1</v>
@@ -8029,13 +8188,13 @@
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="B14" t="s">
+        <v>312</v>
+      </c>
+      <c r="C14" t="s">
         <v>313</v>
-      </c>
-      <c r="C14" t="s">
-        <v>314</v>
       </c>
       <c r="D14">
         <v>-2</v>
@@ -8043,13 +8202,13 @@
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="B15" t="s">
         <v>3</v>
       </c>
       <c r="C15" t="s">
-        <v>315</v>
+        <v>314</v>
       </c>
       <c r="D15">
         <v>-3</v>
@@ -8057,13 +8216,13 @@
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="B16" t="s">
+        <v>315</v>
+      </c>
+      <c r="C16" t="s">
         <v>316</v>
-      </c>
-      <c r="C16" t="s">
-        <v>317</v>
       </c>
       <c r="D16">
         <v>-6</v>
@@ -8071,13 +8230,13 @@
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="B17" t="s">
+        <v>317</v>
+      </c>
+      <c r="C17" t="s">
         <v>318</v>
-      </c>
-      <c r="C17" t="s">
-        <v>319</v>
       </c>
       <c r="D17">
         <v>-9</v>
@@ -8085,13 +8244,13 @@
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="B18" t="s">
+        <v>319</v>
+      </c>
+      <c r="C18" t="s">
         <v>320</v>
-      </c>
-      <c r="C18" t="s">
-        <v>321</v>
       </c>
       <c r="D18">
         <v>-12</v>
@@ -8099,13 +8258,13 @@
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="B19" t="s">
+        <v>321</v>
+      </c>
+      <c r="C19" t="s">
         <v>322</v>
-      </c>
-      <c r="C19" t="s">
-        <v>323</v>
       </c>
       <c r="D19">
         <v>-15</v>
@@ -8113,13 +8272,13 @@
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="B20" t="s">
+        <v>323</v>
+      </c>
+      <c r="C20" t="s">
         <v>324</v>
-      </c>
-      <c r="C20" t="s">
-        <v>325</v>
       </c>
       <c r="D20">
         <v>-18</v>
@@ -8127,13 +8286,13 @@
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="B21" t="s">
+        <v>325</v>
+      </c>
+      <c r="C21" t="s">
         <v>326</v>
-      </c>
-      <c r="C21" t="s">
-        <v>327</v>
       </c>
       <c r="D21">
         <v>-21</v>
@@ -8141,13 +8300,13 @@
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="B22" t="s">
+        <v>327</v>
+      </c>
+      <c r="C22" t="s">
         <v>328</v>
-      </c>
-      <c r="C22" t="s">
-        <v>329</v>
       </c>
       <c r="D22">
         <v>-24</v>
@@ -8155,13 +8314,13 @@
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
+        <v>371</v>
+      </c>
+      <c r="B23" t="s">
         <v>372</v>
       </c>
-      <c r="B23" t="s">
+      <c r="C23" t="s">
         <v>373</v>
-      </c>
-      <c r="C23" t="s">
-        <v>374</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
passing, amended authorship declaration
</commit_message>
<xml_diff>
--- a/src/carpy/utility/data/quantities.xlsx
+++ b/src/carpy/utility/data/quantities.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\yr3g17\PycharmProjects\carpy\src\carpy\utility\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E1D4C2FC-21FF-43A6-ADC4-A936D334C31C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{57C2AA10-9853-4FDB-B618-21CE27A0CB3A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="dimensions" sheetId="1" r:id="rId1"/>
@@ -1755,27 +1755,27 @@
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="G19" sqref="G19"/>
+      <selection pane="bottomLeft"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="12.44140625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="18.44140625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="12.42578125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="18.42578125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="38" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="2.6640625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="2.44140625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="2.6640625" bestFit="1" customWidth="1"/>
-    <col min="7" max="8" width="2.44140625" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="4.109375" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="2.77734375" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="3.6640625" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="2.44140625" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="11.88671875" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="65.44140625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="2.7109375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="2.42578125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="2.7109375" bestFit="1" customWidth="1"/>
+    <col min="7" max="8" width="2.42578125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="4.140625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="2.7109375" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="3.7109375" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="2.42578125" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="11.85546875" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="65.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>75</v>
       </c>
@@ -1819,7 +1819,7 @@
         <v>129</v>
       </c>
     </row>
-    <row r="2" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>94</v>
       </c>
@@ -1863,7 +1863,7 @@
         <v>136</v>
       </c>
     </row>
-    <row r="3" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>94</v>
       </c>
@@ -1907,7 +1907,7 @@
         <v>137</v>
       </c>
     </row>
-    <row r="4" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>94</v>
       </c>
@@ -1951,7 +1951,7 @@
         <v>431</v>
       </c>
     </row>
-    <row r="5" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>94</v>
       </c>
@@ -1995,7 +1995,7 @@
         <v>138</v>
       </c>
     </row>
-    <row r="6" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>94</v>
       </c>
@@ -2039,7 +2039,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="7" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>94</v>
       </c>
@@ -2083,7 +2083,7 @@
         <v>140</v>
       </c>
     </row>
-    <row r="8" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>94</v>
       </c>
@@ -2127,7 +2127,7 @@
         <v>141</v>
       </c>
     </row>
-    <row r="9" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>94</v>
       </c>
@@ -2171,7 +2171,7 @@
         <v>142</v>
       </c>
     </row>
-    <row r="10" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>94</v>
       </c>
@@ -2215,7 +2215,7 @@
         <v>143</v>
       </c>
     </row>
-    <row r="11" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>94</v>
       </c>
@@ -2259,7 +2259,7 @@
         <v>144</v>
       </c>
     </row>
-    <row r="12" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>94</v>
       </c>
@@ -2303,7 +2303,7 @@
         <v>145</v>
       </c>
     </row>
-    <row r="13" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>94</v>
       </c>
@@ -2347,7 +2347,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="14" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>94</v>
       </c>
@@ -2391,7 +2391,7 @@
         <v>147</v>
       </c>
     </row>
-    <row r="15" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>94</v>
       </c>
@@ -2435,7 +2435,7 @@
         <v>148</v>
       </c>
     </row>
-    <row r="16" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>94</v>
       </c>
@@ -2479,7 +2479,7 @@
         <v>157</v>
       </c>
     </row>
-    <row r="17" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>94</v>
       </c>
@@ -2523,7 +2523,7 @@
         <v>149</v>
       </c>
     </row>
-    <row r="18" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>94</v>
       </c>
@@ -2567,7 +2567,7 @@
         <v>150</v>
       </c>
     </row>
-    <row r="19" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>94</v>
       </c>
@@ -2611,7 +2611,7 @@
         <v>151</v>
       </c>
     </row>
-    <row r="20" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>94</v>
       </c>
@@ -2655,7 +2655,7 @@
         <v>152</v>
       </c>
     </row>
-    <row r="21" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>94</v>
       </c>
@@ -2699,7 +2699,7 @@
         <v>153</v>
       </c>
     </row>
-    <row r="22" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>94</v>
       </c>
@@ -2743,7 +2743,7 @@
         <v>154</v>
       </c>
     </row>
-    <row r="23" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>94</v>
       </c>
@@ -2787,7 +2787,7 @@
         <v>155</v>
       </c>
     </row>
-    <row r="24" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>94</v>
       </c>
@@ -2831,7 +2831,7 @@
         <v>156</v>
       </c>
     </row>
-    <row r="25" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>94</v>
       </c>
@@ -2875,7 +2875,7 @@
         <v>158</v>
       </c>
     </row>
-    <row r="26" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>94</v>
       </c>
@@ -2919,7 +2919,7 @@
         <v>159</v>
       </c>
     </row>
-    <row r="27" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>94</v>
       </c>
@@ -2963,7 +2963,7 @@
         <v>160</v>
       </c>
     </row>
-    <row r="28" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>94</v>
       </c>
@@ -3007,7 +3007,7 @@
         <v>161</v>
       </c>
     </row>
-    <row r="29" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>94</v>
       </c>
@@ -3051,7 +3051,7 @@
         <v>162</v>
       </c>
     </row>
-    <row r="30" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>94</v>
       </c>
@@ -3095,7 +3095,7 @@
         <v>163</v>
       </c>
     </row>
-    <row r="31" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>216</v>
       </c>
@@ -3140,7 +3140,7 @@
         <v>164</v>
       </c>
     </row>
-    <row r="32" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
         <v>216</v>
       </c>
@@ -3185,7 +3185,7 @@
         <v>165</v>
       </c>
     </row>
-    <row r="33" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
         <v>216</v>
       </c>
@@ -3230,7 +3230,7 @@
         <v>166</v>
       </c>
     </row>
-    <row r="34" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
         <v>216</v>
       </c>
@@ -3274,7 +3274,7 @@
         <v>132</v>
       </c>
     </row>
-    <row r="35" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
         <v>216</v>
       </c>
@@ -3319,7 +3319,7 @@
         <v>288</v>
       </c>
     </row>
-    <row r="36" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
         <v>216</v>
       </c>
@@ -3364,7 +3364,7 @@
         <v>243</v>
       </c>
     </row>
-    <row r="37" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
         <v>216</v>
       </c>
@@ -3409,7 +3409,7 @@
         <v>172</v>
       </c>
     </row>
-    <row r="38" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
         <v>216</v>
       </c>
@@ -3454,7 +3454,7 @@
         <v>173</v>
       </c>
     </row>
-    <row r="39" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
         <v>216</v>
       </c>
@@ -3499,7 +3499,7 @@
         <v>174</v>
       </c>
     </row>
-    <row r="40" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
         <v>216</v>
       </c>
@@ -3544,7 +3544,7 @@
         <v>167</v>
       </c>
     </row>
-    <row r="41" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
         <v>216</v>
       </c>
@@ -3588,7 +3588,7 @@
         <v>168</v>
       </c>
     </row>
-    <row r="42" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
         <v>216</v>
       </c>
@@ -3633,7 +3633,7 @@
         <v>429</v>
       </c>
     </row>
-    <row r="43" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
         <v>216</v>
       </c>
@@ -3677,7 +3677,7 @@
         <v>169</v>
       </c>
     </row>
-    <row r="44" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
         <v>216</v>
       </c>
@@ -3722,7 +3722,7 @@
         <v>170</v>
       </c>
     </row>
-    <row r="45" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
         <v>216</v>
       </c>
@@ -3766,7 +3766,7 @@
         <v>361</v>
       </c>
     </row>
-    <row r="46" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
         <v>216</v>
       </c>
@@ -3811,7 +3811,7 @@
         <v>171</v>
       </c>
     </row>
-    <row r="47" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
         <v>216</v>
       </c>
@@ -3856,7 +3856,7 @@
         <v>224</v>
       </c>
     </row>
-    <row r="48" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
         <v>216</v>
       </c>
@@ -3901,7 +3901,7 @@
         <v>222</v>
       </c>
     </row>
-    <row r="49" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
         <v>216</v>
       </c>
@@ -3946,7 +3946,7 @@
         <v>223</v>
       </c>
     </row>
-    <row r="50" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
         <v>216</v>
       </c>
@@ -3991,7 +3991,7 @@
         <v>231</v>
       </c>
     </row>
-    <row r="51" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
         <v>225</v>
       </c>
@@ -4035,7 +4035,7 @@
         <v>230</v>
       </c>
     </row>
-    <row r="52" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
         <v>225</v>
       </c>
@@ -4079,7 +4079,7 @@
         <v>230</v>
       </c>
     </row>
-    <row r="53" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
         <v>225</v>
       </c>
@@ -4124,7 +4124,7 @@
         <v>239</v>
       </c>
     </row>
-    <row r="54" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
         <v>225</v>
       </c>
@@ -4169,7 +4169,7 @@
         <v>236</v>
       </c>
     </row>
-    <row r="55" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="55" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
         <v>225</v>
       </c>
@@ -4214,7 +4214,7 @@
         <v>230</v>
       </c>
     </row>
-    <row r="56" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
         <v>225</v>
       </c>
@@ -4259,7 +4259,7 @@
         <v>369</v>
       </c>
     </row>
-    <row r="57" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="57" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
         <v>225</v>
       </c>
@@ -4304,7 +4304,7 @@
         <v>370</v>
       </c>
     </row>
-    <row r="58" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="58" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
         <v>76</v>
       </c>
@@ -4349,7 +4349,7 @@
         <v>175</v>
       </c>
     </row>
-    <row r="59" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="59" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
         <v>76</v>
       </c>
@@ -4394,7 +4394,7 @@
         <v>131</v>
       </c>
     </row>
-    <row r="60" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="60" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
         <v>76</v>
       </c>
@@ -4439,7 +4439,7 @@
         <v>176</v>
       </c>
     </row>
-    <row r="61" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="61" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A61" t="s">
         <v>76</v>
       </c>
@@ -4484,7 +4484,7 @@
         <v>177</v>
       </c>
     </row>
-    <row r="62" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="62" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A62" t="s">
         <v>76</v>
       </c>
@@ -4529,7 +4529,7 @@
         <v>178</v>
       </c>
     </row>
-    <row r="63" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="63" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A63" t="s">
         <v>76</v>
       </c>
@@ -4574,7 +4574,7 @@
         <v>179</v>
       </c>
     </row>
-    <row r="64" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="64" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A64" t="s">
         <v>76</v>
       </c>
@@ -4619,7 +4619,7 @@
         <v>180</v>
       </c>
     </row>
-    <row r="65" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="65" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A65" t="s">
         <v>76</v>
       </c>
@@ -4664,7 +4664,7 @@
         <v>181</v>
       </c>
     </row>
-    <row r="66" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="66" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A66" t="s">
         <v>76</v>
       </c>
@@ -4709,7 +4709,7 @@
         <v>182</v>
       </c>
     </row>
-    <row r="67" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="67" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A67" t="s">
         <v>76</v>
       </c>
@@ -4754,7 +4754,7 @@
         <v>183</v>
       </c>
     </row>
-    <row r="68" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="68" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A68" t="s">
         <v>76</v>
       </c>
@@ -4799,7 +4799,7 @@
         <v>131</v>
       </c>
     </row>
-    <row r="69" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="69" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A69" t="s">
         <v>76</v>
       </c>
@@ -4844,7 +4844,7 @@
         <v>184</v>
       </c>
     </row>
-    <row r="70" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="70" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A70" t="s">
         <v>76</v>
       </c>
@@ -4889,7 +4889,7 @@
         <v>188</v>
       </c>
     </row>
-    <row r="71" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="71" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A71" t="s">
         <v>76</v>
       </c>
@@ -4934,7 +4934,7 @@
         <v>187</v>
       </c>
     </row>
-    <row r="72" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="72" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A72" t="s">
         <v>76</v>
       </c>
@@ -4979,7 +4979,7 @@
         <v>273</v>
       </c>
     </row>
-    <row r="73" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="73" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A73" t="s">
         <v>76</v>
       </c>
@@ -5024,7 +5024,7 @@
         <v>185</v>
       </c>
     </row>
-    <row r="74" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="74" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A74" t="s">
         <v>76</v>
       </c>
@@ -5069,7 +5069,7 @@
         <v>186</v>
       </c>
     </row>
-    <row r="75" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="75" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A75" t="s">
         <v>76</v>
       </c>
@@ -5114,7 +5114,7 @@
         <v>245</v>
       </c>
     </row>
-    <row r="76" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="76" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A76" t="s">
         <v>76</v>
       </c>
@@ -5159,7 +5159,7 @@
         <v>356</v>
       </c>
     </row>
-    <row r="77" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="77" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A77" t="s">
         <v>76</v>
       </c>
@@ -5204,7 +5204,7 @@
         <v>357</v>
       </c>
     </row>
-    <row r="78" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="78" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A78" t="s">
         <v>430</v>
       </c>
@@ -5249,7 +5249,7 @@
         <v>274</v>
       </c>
     </row>
-    <row r="79" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="79" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A79" t="s">
         <v>430</v>
       </c>
@@ -5294,7 +5294,7 @@
         <v>275</v>
       </c>
     </row>
-    <row r="80" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="80" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A80" t="s">
         <v>430</v>
       </c>
@@ -5339,7 +5339,7 @@
         <v>354</v>
       </c>
     </row>
-    <row r="81" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="81" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A81" t="s">
         <v>430</v>
       </c>
@@ -5384,7 +5384,7 @@
         <v>264</v>
       </c>
     </row>
-    <row r="82" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="82" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A82" t="s">
         <v>430</v>
       </c>
@@ -5429,7 +5429,7 @@
         <v>265</v>
       </c>
     </row>
-    <row r="83" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="83" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A83" t="s">
         <v>430</v>
       </c>
@@ -5474,7 +5474,7 @@
         <v>266</v>
       </c>
     </row>
-    <row r="84" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="84" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A84" t="s">
         <v>430</v>
       </c>
@@ -5519,7 +5519,7 @@
         <v>267</v>
       </c>
     </row>
-    <row r="85" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="85" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A85" t="s">
         <v>430</v>
       </c>
@@ -5564,7 +5564,7 @@
         <v>263</v>
       </c>
     </row>
-    <row r="86" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="86" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A86" t="s">
         <v>430</v>
       </c>
@@ -5609,7 +5609,7 @@
         <v>246</v>
       </c>
     </row>
-    <row r="87" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="87" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A87" t="s">
         <v>430</v>
       </c>
@@ -5654,7 +5654,7 @@
         <v>283</v>
       </c>
     </row>
-    <row r="88" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="88" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A88" t="s">
         <v>430</v>
       </c>
@@ -5699,7 +5699,7 @@
         <v>282</v>
       </c>
     </row>
-    <row r="89" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="89" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A89" t="s">
         <v>430</v>
       </c>
@@ -5744,7 +5744,7 @@
         <v>284</v>
       </c>
     </row>
-    <row r="90" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="90" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A90" t="s">
         <v>430</v>
       </c>
@@ -5789,7 +5789,7 @@
         <v>286</v>
       </c>
     </row>
-    <row r="91" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="91" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A91" t="s">
         <v>430</v>
       </c>
@@ -5834,7 +5834,7 @@
         <v>285</v>
       </c>
     </row>
-    <row r="92" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="92" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A92" t="s">
         <v>76</v>
       </c>
@@ -5879,7 +5879,7 @@
         <v>189</v>
       </c>
     </row>
-    <row r="93" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="93" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A93" t="s">
         <v>76</v>
       </c>
@@ -5924,7 +5924,7 @@
         <v>190</v>
       </c>
     </row>
-    <row r="94" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="94" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A94" t="s">
         <v>76</v>
       </c>
@@ -5969,7 +5969,7 @@
         <v>191</v>
       </c>
     </row>
-    <row r="95" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="95" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A95" t="s">
         <v>76</v>
       </c>
@@ -6014,7 +6014,7 @@
         <v>253</v>
       </c>
     </row>
-    <row r="96" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="96" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A96" t="s">
         <v>76</v>
       </c>
@@ -6059,7 +6059,7 @@
         <v>192</v>
       </c>
     </row>
-    <row r="97" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="97" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A97" t="s">
         <v>76</v>
       </c>
@@ -6104,7 +6104,7 @@
         <v>193</v>
       </c>
     </row>
-    <row r="98" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="98" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A98" t="s">
         <v>76</v>
       </c>
@@ -6149,7 +6149,7 @@
         <v>249</v>
       </c>
     </row>
-    <row r="99" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="99" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A99" t="s">
         <v>76</v>
       </c>
@@ -6194,7 +6194,7 @@
         <v>250</v>
       </c>
     </row>
-    <row r="100" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="100" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A100" t="s">
         <v>430</v>
       </c>
@@ -6239,7 +6239,7 @@
         <v>255</v>
       </c>
     </row>
-    <row r="101" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="101" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A101" t="s">
         <v>430</v>
       </c>
@@ -6284,7 +6284,7 @@
         <v>256</v>
       </c>
     </row>
-    <row r="102" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="102" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A102" t="s">
         <v>76</v>
       </c>
@@ -6329,7 +6329,7 @@
         <v>194</v>
       </c>
     </row>
-    <row r="103" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="103" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A103" t="s">
         <v>76</v>
       </c>
@@ -6374,7 +6374,7 @@
         <v>195</v>
       </c>
     </row>
-    <row r="104" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="104" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A104" t="s">
         <v>76</v>
       </c>
@@ -6419,7 +6419,7 @@
         <v>215</v>
       </c>
     </row>
-    <row r="105" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="105" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A105" t="s">
         <v>76</v>
       </c>
@@ -6464,7 +6464,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="106" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="106" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A106" t="s">
         <v>76</v>
       </c>
@@ -6509,7 +6509,7 @@
         <v>196</v>
       </c>
     </row>
-    <row r="107" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="107" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A107" t="s">
         <v>76</v>
       </c>
@@ -6554,7 +6554,7 @@
         <v>432</v>
       </c>
     </row>
-    <row r="108" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="108" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A108" t="s">
         <v>76</v>
       </c>
@@ -6598,7 +6598,7 @@
         <v>244</v>
       </c>
     </row>
-    <row r="109" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="109" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A109" t="s">
         <v>76</v>
       </c>
@@ -6643,7 +6643,7 @@
         <v>200</v>
       </c>
     </row>
-    <row r="110" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="110" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A110" t="s">
         <v>76</v>
       </c>
@@ -6688,7 +6688,7 @@
         <v>247</v>
       </c>
     </row>
-    <row r="111" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="111" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A111" t="s">
         <v>76</v>
       </c>
@@ -6733,7 +6733,7 @@
         <v>205</v>
       </c>
     </row>
-    <row r="112" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="112" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A112" t="s">
         <v>76</v>
       </c>
@@ -6778,7 +6778,7 @@
         <v>202</v>
       </c>
     </row>
-    <row r="113" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="113" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A113" t="s">
         <v>76</v>
       </c>
@@ -6823,7 +6823,7 @@
         <v>207</v>
       </c>
     </row>
-    <row r="114" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="114" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A114" t="s">
         <v>76</v>
       </c>
@@ -6868,7 +6868,7 @@
         <v>212</v>
       </c>
     </row>
-    <row r="115" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="115" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A115" t="s">
         <v>76</v>
       </c>
@@ -6913,7 +6913,7 @@
         <v>212</v>
       </c>
     </row>
-    <row r="116" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="116" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A116" t="s">
         <v>371</v>
       </c>
@@ -6924,7 +6924,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="117" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="117" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A117" t="s">
         <v>371</v>
       </c>
@@ -6935,7 +6935,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="118" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="118" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A118" t="s">
         <v>371</v>
       </c>
@@ -6946,7 +6946,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="119" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="119" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A119" t="s">
         <v>371</v>
       </c>
@@ -6960,7 +6960,7 @@
         <v>407</v>
       </c>
     </row>
-    <row r="120" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="120" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A120" t="s">
         <v>371</v>
       </c>
@@ -6971,7 +6971,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="121" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="121" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A121" t="s">
         <v>371</v>
       </c>
@@ -6982,7 +6982,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="122" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="122" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A122" t="s">
         <v>371</v>
       </c>
@@ -6996,7 +6996,7 @@
         <v>412</v>
       </c>
     </row>
-    <row r="123" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="123" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A123" t="s">
         <v>371</v>
       </c>
@@ -7010,7 +7010,7 @@
         <v>408</v>
       </c>
     </row>
-    <row r="124" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="124" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A124" t="s">
         <v>371</v>
       </c>
@@ -7051,7 +7051,7 @@
         <v>424</v>
       </c>
     </row>
-    <row r="125" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="125" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A125" t="s">
         <v>371</v>
       </c>
@@ -7065,7 +7065,7 @@
         <v>409</v>
       </c>
     </row>
-    <row r="126" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="126" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A126" t="s">
         <v>371</v>
       </c>
@@ -7079,7 +7079,7 @@
         <v>410</v>
       </c>
     </row>
-    <row r="127" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="127" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A127" t="s">
         <v>371</v>
       </c>
@@ -7093,7 +7093,7 @@
         <v>411</v>
       </c>
     </row>
-    <row r="128" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="128" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A128" t="s">
         <v>371</v>
       </c>
@@ -7107,7 +7107,7 @@
         <v>413</v>
       </c>
     </row>
-    <row r="129" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="129" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A129" t="s">
         <v>371</v>
       </c>
@@ -7121,7 +7121,7 @@
         <v>414</v>
       </c>
     </row>
-    <row r="130" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="130" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A130" t="s">
         <v>371</v>
       </c>
@@ -7162,7 +7162,7 @@
         <v>423</v>
       </c>
     </row>
-    <row r="131" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="131" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A131" t="s">
         <v>371</v>
       </c>
@@ -7176,7 +7176,7 @@
         <v>415</v>
       </c>
     </row>
-    <row r="132" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="132" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A132" t="s">
         <v>371</v>
       </c>
@@ -7217,7 +7217,7 @@
         <v>425</v>
       </c>
     </row>
-    <row r="133" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="133" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A133" t="s">
         <v>371</v>
       </c>
@@ -7252,7 +7252,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="134" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="134" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A134" t="s">
         <v>371</v>
       </c>
@@ -7263,7 +7263,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="135" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="135" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A135" t="s">
         <v>371</v>
       </c>
@@ -7304,7 +7304,7 @@
         <v>416</v>
       </c>
     </row>
-    <row r="136" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="136" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A136" t="s">
         <v>371</v>
       </c>
@@ -7315,7 +7315,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="137" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="137" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A137" t="s">
         <v>371</v>
       </c>
@@ -7326,7 +7326,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="138" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="138" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A138" t="s">
         <v>371</v>
       </c>
@@ -7337,7 +7337,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="139" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="139" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A139" t="s">
         <v>371</v>
       </c>
@@ -7348,7 +7348,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="140" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="140" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A140" t="s">
         <v>371</v>
       </c>
@@ -7359,7 +7359,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="141" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="141" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A141" t="s">
         <v>371</v>
       </c>
@@ -7397,7 +7397,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="142" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="142" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A142" t="s">
         <v>371</v>
       </c>
@@ -7408,7 +7408,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="143" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="143" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A143" t="s">
         <v>371</v>
       </c>
@@ -7449,7 +7449,7 @@
         <v>419</v>
       </c>
     </row>
-    <row r="144" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="144" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A144" t="s">
         <v>371</v>
       </c>
@@ -7460,7 +7460,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="145" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="145" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A145" t="s">
         <v>371</v>
       </c>
@@ -7501,7 +7501,7 @@
         <v>422</v>
       </c>
     </row>
-    <row r="146" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="146" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A146" t="s">
         <v>371</v>
       </c>
@@ -7512,7 +7512,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="147" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="147" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A147" t="s">
         <v>371</v>
       </c>
@@ -7526,7 +7526,7 @@
         <v>420</v>
       </c>
     </row>
-    <row r="148" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="148" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A148" t="s">
         <v>371</v>
       </c>
@@ -7537,7 +7537,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="149" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="149" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A149" t="s">
         <v>371</v>
       </c>
@@ -7578,7 +7578,7 @@
         <v>426</v>
       </c>
     </row>
-    <row r="150" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="150" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A150" t="s">
         <v>371</v>
       </c>
@@ -7589,7 +7589,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="151" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="151" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A151" t="s">
         <v>371</v>
       </c>
@@ -7600,7 +7600,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="152" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="152" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A152" t="s">
         <v>371</v>
       </c>
@@ -7611,7 +7611,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="153" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="153" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A153" t="s">
         <v>371</v>
       </c>
@@ -7649,7 +7649,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="154" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="154" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A154" t="s">
         <v>371</v>
       </c>
@@ -7687,7 +7687,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="155" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="155" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A155" t="s">
         <v>371</v>
       </c>
@@ -7725,7 +7725,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="156" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="156" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A156" t="s">
         <v>371</v>
       </c>
@@ -7763,7 +7763,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="157" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="157" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A157" t="s">
         <v>76</v>
       </c>
@@ -7808,7 +7808,7 @@
         <v>435</v>
       </c>
     </row>
-    <row r="158" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="158" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A158" t="s">
         <v>225</v>
       </c>
@@ -7853,7 +7853,7 @@
         <v>439</v>
       </c>
     </row>
-    <row r="159" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="159" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A159" t="s">
         <v>225</v>
       </c>
@@ -7897,7 +7897,7 @@
         <v>444</v>
       </c>
     </row>
-    <row r="160" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="160" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A160" t="s">
         <v>225</v>
       </c>
@@ -7941,7 +7941,7 @@
         <v>449</v>
       </c>
     </row>
-    <row r="161" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="161" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A161" t="s">
         <v>225</v>
       </c>
@@ -8011,9 +8011,9 @@
       <selection activeCell="A12" sqref="A12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>75</v>
       </c>
@@ -8027,7 +8027,7 @@
         <v>291</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>94</v>
       </c>
@@ -8041,7 +8041,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>94</v>
       </c>
@@ -8055,7 +8055,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>94</v>
       </c>
@@ -8069,7 +8069,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>94</v>
       </c>
@@ -8083,7 +8083,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>94</v>
       </c>
@@ -8097,7 +8097,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>94</v>
       </c>
@@ -8111,7 +8111,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>94</v>
       </c>
@@ -8125,7 +8125,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>94</v>
       </c>
@@ -8139,7 +8139,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>94</v>
       </c>
@@ -8153,7 +8153,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>94</v>
       </c>
@@ -8167,12 +8167,12 @@
         <v>1</v>
       </c>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="D12">
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>94</v>
       </c>
@@ -8186,7 +8186,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>94</v>
       </c>
@@ -8200,7 +8200,7 @@
         <v>-2</v>
       </c>
     </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>94</v>
       </c>
@@ -8214,7 +8214,7 @@
         <v>-3</v>
       </c>
     </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>94</v>
       </c>
@@ -8228,7 +8228,7 @@
         <v>-6</v>
       </c>
     </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>94</v>
       </c>
@@ -8242,7 +8242,7 @@
         <v>-9</v>
       </c>
     </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>94</v>
       </c>
@@ -8256,7 +8256,7 @@
         <v>-12</v>
       </c>
     </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>94</v>
       </c>
@@ -8270,7 +8270,7 @@
         <v>-15</v>
       </c>
     </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>94</v>
       </c>
@@ -8284,7 +8284,7 @@
         <v>-18</v>
       </c>
     </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>94</v>
       </c>
@@ -8298,7 +8298,7 @@
         <v>-21</v>
       </c>
     </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>94</v>
       </c>
@@ -8312,7 +8312,7 @@
         <v>-24</v>
       </c>
     </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>371</v>
       </c>

</xml_diff>